<commit_message>
GH ACTION Autorun Tue Feb  4 05:26:35 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FED2A6-A634-4B26-878F-5325DC296ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87774673-D1D3-4178-9F8E-AA474C39E785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4022,7 +4022,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4436,7 +4436,7 @@
         <v>6112</v>
       </c>
       <c r="F5" s="15">
-        <v>6109</v>
+        <v>6088</v>
       </c>
       <c r="G5" s="15">
         <v>6073</v>
@@ -4597,7 +4597,7 @@
         <v>13019</v>
       </c>
       <c r="F6" s="15">
-        <v>13258</v>
+        <v>13209</v>
       </c>
       <c r="G6" s="15">
         <v>13602</v>
@@ -4758,7 +4758,7 @@
         <v>18033</v>
       </c>
       <c r="F7" s="15">
-        <v>17485</v>
+        <v>17869</v>
       </c>
       <c r="G7" s="15">
         <v>17369</v>
@@ -4919,7 +4919,7 @@
         <v>3894</v>
       </c>
       <c r="F8" s="15">
-        <v>4019</v>
+        <v>4014</v>
       </c>
       <c r="G8" s="15">
         <v>4080</v>
@@ -5080,7 +5080,7 @@
         <v>7932</v>
       </c>
       <c r="F9" s="15">
-        <v>8966</v>
+        <v>8964</v>
       </c>
       <c r="G9" s="15">
         <v>9373</v>
@@ -5241,7 +5241,7 @@
         <v>12348</v>
       </c>
       <c r="F10" s="15">
-        <v>13940</v>
+        <v>13956</v>
       </c>
       <c r="G10" s="15">
         <v>15356</v>
@@ -5402,7 +5402,7 @@
         <v>40049</v>
       </c>
       <c r="F11" s="15">
-        <v>42165</v>
+        <v>42059</v>
       </c>
       <c r="G11" s="15">
         <v>41836</v>
@@ -5563,7 +5563,7 @@
         <v>101387</v>
       </c>
       <c r="F12" s="7">
-        <v>105942</v>
+        <v>106159</v>
       </c>
       <c r="G12" s="7">
         <v>107689</v>
@@ -5784,7 +5784,7 @@
         <v>441.34100899999999</v>
       </c>
       <c r="F15" s="15">
-        <v>437.040007</v>
+        <v>435.04525000000001</v>
       </c>
       <c r="G15" s="15">
         <v>437.92900900000001</v>
@@ -5945,7 +5945,7 @@
         <v>952.18820300000004</v>
       </c>
       <c r="F16" s="15">
-        <v>964.13352899999995</v>
+        <v>963.60673299999996</v>
       </c>
       <c r="G16" s="15">
         <v>975.93166799999995</v>
@@ -6106,7 +6106,7 @@
         <v>548.17622900000003</v>
       </c>
       <c r="F17" s="15">
-        <v>577.42893400000003</v>
+        <v>575.67076899999995</v>
       </c>
       <c r="G17" s="15">
         <v>584.43813499999999</v>
@@ -6267,7 +6267,7 @@
         <v>56.533883000000003</v>
       </c>
       <c r="F18" s="15">
-        <v>56.952452999999998</v>
+        <v>56.812646000000001</v>
       </c>
       <c r="G18" s="15">
         <v>57.280774999999998</v>
@@ -6428,7 +6428,7 @@
         <v>317.2758</v>
       </c>
       <c r="F19" s="15">
-        <v>379.321258</v>
+        <v>379.27885300000003</v>
       </c>
       <c r="G19" s="15">
         <v>359.04938199999998</v>
@@ -6589,7 +6589,7 @@
         <v>1271.499867</v>
       </c>
       <c r="F20" s="15">
-        <v>1404.405921</v>
+        <v>1404.9841039999999</v>
       </c>
       <c r="G20" s="15">
         <v>1561.9898499999999</v>
@@ -6750,7 +6750,7 @@
         <v>927.77234299999998</v>
       </c>
       <c r="F21" s="15">
-        <v>1020.4252310000001</v>
+        <v>1019.084356</v>
       </c>
       <c r="G21" s="15">
         <v>983.49547500000006</v>
@@ -6911,7 +6911,7 @@
         <v>4514.7873339999996</v>
       </c>
       <c r="F22" s="7">
-        <v>4839.7073330000003</v>
+        <v>4834.4827110000006</v>
       </c>
       <c r="G22" s="7">
         <v>4960.114294</v>
@@ -7114,7 +7114,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="L32" sqref="L32"/>
+      <selection pane="bottomRight" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7529,7 +7529,7 @@
         <v>5731</v>
       </c>
       <c r="F5" s="15">
-        <v>0</v>
+        <v>5348</v>
       </c>
       <c r="G5" s="15">
         <v>0</v>
@@ -7691,7 +7691,7 @@
         <v>12660</v>
       </c>
       <c r="F6" s="6">
-        <v>0</v>
+        <v>13068</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -7853,7 +7853,7 @@
         <v>16727</v>
       </c>
       <c r="F7" s="6">
-        <v>0</v>
+        <v>17127</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -8015,7 +8015,7 @@
         <v>3696</v>
       </c>
       <c r="F8" s="6">
-        <v>0</v>
+        <v>3791</v>
       </c>
       <c r="G8" s="6">
         <v>0</v>
@@ -8177,7 +8177,7 @@
         <v>9218</v>
       </c>
       <c r="F9" s="6">
-        <v>0</v>
+        <v>9938</v>
       </c>
       <c r="G9" s="6">
         <v>0</v>
@@ -8339,7 +8339,7 @@
         <v>13941</v>
       </c>
       <c r="F10" s="15">
-        <v>0</v>
+        <v>13404</v>
       </c>
       <c r="G10" s="15">
         <v>0</v>
@@ -8501,7 +8501,7 @@
         <v>38642</v>
       </c>
       <c r="F11" s="6">
-        <v>0</v>
+        <v>40951</v>
       </c>
       <c r="G11" s="6">
         <v>0</v>
@@ -8663,7 +8663,7 @@
         <v>100615</v>
       </c>
       <c r="F12" s="7">
-        <v>0</v>
+        <v>103627</v>
       </c>
       <c r="G12" s="7">
         <v>0</v>
@@ -8887,7 +8887,7 @@
         <v>422.88258300000001</v>
       </c>
       <c r="F15" s="15">
-        <v>0</v>
+        <v>382.30444399999999</v>
       </c>
       <c r="G15" s="15">
         <v>0</v>
@@ -9049,7 +9049,7 @@
         <v>947.74714100000006</v>
       </c>
       <c r="F16" s="6">
-        <v>0</v>
+        <v>930.12727900000004</v>
       </c>
       <c r="G16" s="6">
         <v>0</v>
@@ -9211,7 +9211,7 @@
         <v>484.21945799999997</v>
       </c>
       <c r="F17" s="6">
-        <v>0</v>
+        <v>631.29476399999999</v>
       </c>
       <c r="G17" s="6">
         <v>0</v>
@@ -9373,7 +9373,7 @@
         <v>56.739410999999997</v>
       </c>
       <c r="F18" s="6">
-        <v>0</v>
+        <v>54.255637999999998</v>
       </c>
       <c r="G18" s="6">
         <v>0</v>
@@ -9535,7 +9535,7 @@
         <v>418.39605499999999</v>
       </c>
       <c r="F19" s="6">
-        <v>0</v>
+        <v>472.17430100000001</v>
       </c>
       <c r="G19" s="6">
         <v>0</v>
@@ -9697,7 +9697,7 @@
         <v>1450.5708320000001</v>
       </c>
       <c r="F20" s="15">
-        <v>0</v>
+        <v>1316.27008</v>
       </c>
       <c r="G20" s="15">
         <v>0</v>
@@ -9859,7 +9859,7 @@
         <v>920.97551599999997</v>
       </c>
       <c r="F21" s="6">
-        <v>0</v>
+        <v>982.13208499999996</v>
       </c>
       <c r="G21" s="6">
         <v>0</v>
@@ -10021,7 +10021,7 @@
         <v>4701.5309959999995</v>
       </c>
       <c r="F22" s="7">
-        <v>0</v>
+        <v>4768.5585910000009</v>
       </c>
       <c r="G22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Feb 11 05:27:01 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87774673-D1D3-4178-9F8E-AA474C39E785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F811F3E8-CED7-4B59-93D6-F13206F5787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4022,7 +4022,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4439,7 +4439,7 @@
         <v>6088</v>
       </c>
       <c r="G5" s="15">
-        <v>6073</v>
+        <v>6065</v>
       </c>
       <c r="H5" s="15">
         <v>6319</v>
@@ -4600,7 +4600,7 @@
         <v>13209</v>
       </c>
       <c r="G6" s="15">
-        <v>13602</v>
+        <v>13552</v>
       </c>
       <c r="H6" s="15">
         <v>13078</v>
@@ -4761,7 +4761,7 @@
         <v>17869</v>
       </c>
       <c r="G7" s="15">
-        <v>17369</v>
+        <v>17812</v>
       </c>
       <c r="H7" s="15">
         <v>18338</v>
@@ -4922,7 +4922,7 @@
         <v>4014</v>
       </c>
       <c r="G8" s="15">
-        <v>4080</v>
+        <v>4077</v>
       </c>
       <c r="H8" s="15">
         <v>4021</v>
@@ -5083,7 +5083,7 @@
         <v>8964</v>
       </c>
       <c r="G9" s="15">
-        <v>9373</v>
+        <v>9384</v>
       </c>
       <c r="H9" s="15">
         <v>9453</v>
@@ -5244,7 +5244,7 @@
         <v>13956</v>
       </c>
       <c r="G10" s="15">
-        <v>15356</v>
+        <v>15365</v>
       </c>
       <c r="H10" s="15">
         <v>13774</v>
@@ -5405,7 +5405,7 @@
         <v>42059</v>
       </c>
       <c r="G11" s="15">
-        <v>41836</v>
+        <v>41774</v>
       </c>
       <c r="H11" s="15">
         <v>42243</v>
@@ -5566,7 +5566,7 @@
         <v>106159</v>
       </c>
       <c r="G12" s="7">
-        <v>107689</v>
+        <v>108029</v>
       </c>
       <c r="H12" s="7">
         <v>107226</v>
@@ -5787,7 +5787,7 @@
         <v>435.04525000000001</v>
       </c>
       <c r="G15" s="15">
-        <v>437.92900900000001</v>
+        <v>437.15860700000002</v>
       </c>
       <c r="H15" s="15">
         <v>475.75850000000003</v>
@@ -5948,7 +5948,7 @@
         <v>963.60673299999996</v>
       </c>
       <c r="G16" s="15">
-        <v>975.93166799999995</v>
+        <v>973.32883300000003</v>
       </c>
       <c r="H16" s="15">
         <v>939.5607</v>
@@ -6109,7 +6109,7 @@
         <v>575.67076899999995</v>
       </c>
       <c r="G17" s="15">
-        <v>584.43813499999999</v>
+        <v>580.43109600000003</v>
       </c>
       <c r="H17" s="15">
         <v>634.08169299999997</v>
@@ -6270,7 +6270,7 @@
         <v>56.812646000000001</v>
       </c>
       <c r="G18" s="15">
-        <v>57.280774999999998</v>
+        <v>57.217233</v>
       </c>
       <c r="H18" s="15">
         <v>57.660563000000003</v>
@@ -6431,7 +6431,7 @@
         <v>379.27885300000003</v>
       </c>
       <c r="G19" s="15">
-        <v>359.04938199999998</v>
+        <v>359.95370200000002</v>
       </c>
       <c r="H19" s="15">
         <v>376.42179900000002</v>
@@ -6592,7 +6592,7 @@
         <v>1404.9841039999999</v>
       </c>
       <c r="G20" s="15">
-        <v>1561.9898499999999</v>
+        <v>1562.604748</v>
       </c>
       <c r="H20" s="15">
         <v>1397.3225620000001</v>
@@ -6753,7 +6753,7 @@
         <v>1019.084356</v>
       </c>
       <c r="G21" s="15">
-        <v>983.49547500000006</v>
+        <v>982.83891600000004</v>
       </c>
       <c r="H21" s="15">
         <v>991.33487300000002</v>
@@ -6914,7 +6914,7 @@
         <v>4834.4827110000006</v>
       </c>
       <c r="G22" s="7">
-        <v>4960.114294</v>
+        <v>4953.5331349999997</v>
       </c>
       <c r="H22" s="7">
         <v>4872.1406900000002</v>
@@ -7114,7 +7114,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="I34" sqref="I34"/>
+      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7532,7 +7532,7 @@
         <v>5348</v>
       </c>
       <c r="G5" s="15">
-        <v>0</v>
+        <v>5417</v>
       </c>
       <c r="H5" s="15">
         <v>0</v>
@@ -7694,7 +7694,7 @@
         <v>13068</v>
       </c>
       <c r="G6" s="6">
-        <v>0</v>
+        <v>12127</v>
       </c>
       <c r="H6" s="6">
         <v>0</v>
@@ -7856,7 +7856,7 @@
         <v>17127</v>
       </c>
       <c r="G7" s="6">
-        <v>0</v>
+        <v>14064</v>
       </c>
       <c r="H7" s="6">
         <v>0</v>
@@ -8018,7 +8018,7 @@
         <v>3791</v>
       </c>
       <c r="G8" s="6">
-        <v>0</v>
+        <v>3939</v>
       </c>
       <c r="H8" s="6">
         <v>0</v>
@@ -8180,7 +8180,7 @@
         <v>9938</v>
       </c>
       <c r="G9" s="6">
-        <v>0</v>
+        <v>9258</v>
       </c>
       <c r="H9" s="6">
         <v>0</v>
@@ -8342,7 +8342,7 @@
         <v>13404</v>
       </c>
       <c r="G10" s="15">
-        <v>0</v>
+        <v>13238</v>
       </c>
       <c r="H10" s="15">
         <v>0</v>
@@ -8504,7 +8504,7 @@
         <v>40951</v>
       </c>
       <c r="G11" s="6">
-        <v>0</v>
+        <v>39278</v>
       </c>
       <c r="H11" s="6">
         <v>0</v>
@@ -8666,7 +8666,7 @@
         <v>103627</v>
       </c>
       <c r="G12" s="7">
-        <v>0</v>
+        <v>97321</v>
       </c>
       <c r="H12" s="7">
         <v>0</v>
@@ -8890,7 +8890,7 @@
         <v>382.30444399999999</v>
       </c>
       <c r="G15" s="15">
-        <v>0</v>
+        <v>390.40495800000002</v>
       </c>
       <c r="H15" s="15">
         <v>0</v>
@@ -9052,7 +9052,7 @@
         <v>930.12727900000004</v>
       </c>
       <c r="G16" s="6">
-        <v>0</v>
+        <v>833.34708599999999</v>
       </c>
       <c r="H16" s="6">
         <v>0</v>
@@ -9214,7 +9214,7 @@
         <v>631.29476399999999</v>
       </c>
       <c r="G17" s="6">
-        <v>0</v>
+        <v>374.94750099999999</v>
       </c>
       <c r="H17" s="6">
         <v>0</v>
@@ -9376,7 +9376,7 @@
         <v>54.255637999999998</v>
       </c>
       <c r="G18" s="6">
-        <v>0</v>
+        <v>58.281337999999998</v>
       </c>
       <c r="H18" s="6">
         <v>0</v>
@@ -9538,7 +9538,7 @@
         <v>472.17430100000001</v>
       </c>
       <c r="G19" s="6">
-        <v>0</v>
+        <v>448.47666900000002</v>
       </c>
       <c r="H19" s="6">
         <v>0</v>
@@ -9700,7 +9700,7 @@
         <v>1316.27008</v>
       </c>
       <c r="G20" s="15">
-        <v>0</v>
+        <v>1261.592337</v>
       </c>
       <c r="H20" s="15">
         <v>0</v>
@@ -9862,7 +9862,7 @@
         <v>982.13208499999996</v>
       </c>
       <c r="G21" s="6">
-        <v>0</v>
+        <v>955.18045300000006</v>
       </c>
       <c r="H21" s="6">
         <v>0</v>
@@ -10024,7 +10024,7 @@
         <v>4768.5585910000009</v>
       </c>
       <c r="G22" s="7">
-        <v>0</v>
+        <v>4322.2303419999998</v>
       </c>
       <c r="H22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Feb 18 05:27:38 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F811F3E8-CED7-4B59-93D6-F13206F5787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF410DBF-771A-498C-9F06-08DAA3BD642A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4022,7 +4022,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4442,7 +4442,7 @@
         <v>6065</v>
       </c>
       <c r="H5" s="15">
-        <v>6319</v>
+        <v>6290</v>
       </c>
       <c r="I5" s="15">
         <v>6372</v>
@@ -4603,7 +4603,7 @@
         <v>13552</v>
       </c>
       <c r="H6" s="15">
-        <v>13078</v>
+        <v>13026</v>
       </c>
       <c r="I6" s="15">
         <v>13446</v>
@@ -4764,7 +4764,7 @@
         <v>17812</v>
       </c>
       <c r="H7" s="15">
-        <v>18338</v>
+        <v>18992</v>
       </c>
       <c r="I7" s="15">
         <v>19954</v>
@@ -4925,7 +4925,7 @@
         <v>4077</v>
       </c>
       <c r="H8" s="15">
-        <v>4021</v>
+        <v>4017</v>
       </c>
       <c r="I8" s="15">
         <v>4009</v>
@@ -5086,7 +5086,7 @@
         <v>9384</v>
       </c>
       <c r="H9" s="15">
-        <v>9453</v>
+        <v>9308</v>
       </c>
       <c r="I9" s="15">
         <v>8653</v>
@@ -5247,7 +5247,7 @@
         <v>15365</v>
       </c>
       <c r="H10" s="15">
-        <v>13774</v>
+        <v>13754</v>
       </c>
       <c r="I10" s="15">
         <v>15846</v>
@@ -5408,7 +5408,7 @@
         <v>41774</v>
       </c>
       <c r="H11" s="15">
-        <v>42243</v>
+        <v>42122</v>
       </c>
       <c r="I11" s="15">
         <v>40915</v>
@@ -5569,7 +5569,7 @@
         <v>108029</v>
       </c>
       <c r="H12" s="7">
-        <v>107226</v>
+        <v>107509</v>
       </c>
       <c r="I12" s="7">
         <v>109195</v>
@@ -5790,7 +5790,7 @@
         <v>437.15860700000002</v>
       </c>
       <c r="H15" s="15">
-        <v>475.75850000000003</v>
+        <v>474.13445000000002</v>
       </c>
       <c r="I15" s="15">
         <v>473.62317100000001</v>
@@ -5951,7 +5951,7 @@
         <v>973.32883300000003</v>
       </c>
       <c r="H16" s="15">
-        <v>939.5607</v>
+        <v>937.48103100000003</v>
       </c>
       <c r="I16" s="15">
         <v>949.24278500000003</v>
@@ -6112,7 +6112,7 @@
         <v>580.43109600000003</v>
       </c>
       <c r="H17" s="15">
-        <v>634.08169299999997</v>
+        <v>632.09177</v>
       </c>
       <c r="I17" s="15">
         <v>616.20216600000003</v>
@@ -6273,7 +6273,7 @@
         <v>57.217233</v>
       </c>
       <c r="H18" s="15">
-        <v>57.660563000000003</v>
+        <v>57.584921999999999</v>
       </c>
       <c r="I18" s="15">
         <v>59.422866999999997</v>
@@ -6434,7 +6434,7 @@
         <v>359.95370200000002</v>
       </c>
       <c r="H19" s="15">
-        <v>376.42179900000002</v>
+        <v>371.83031</v>
       </c>
       <c r="I19" s="15">
         <v>327.11115799999999</v>
@@ -6595,7 +6595,7 @@
         <v>1562.604748</v>
       </c>
       <c r="H20" s="15">
-        <v>1397.3225620000001</v>
+        <v>1396.0078759999999</v>
       </c>
       <c r="I20" s="15">
         <v>1609.5020440000001</v>
@@ -6756,7 +6756,7 @@
         <v>982.83891600000004</v>
       </c>
       <c r="H21" s="15">
-        <v>991.33487300000002</v>
+        <v>989.68533300000001</v>
       </c>
       <c r="I21" s="15">
         <v>1021.273686</v>
@@ -6917,7 +6917,7 @@
         <v>4953.5331349999997</v>
       </c>
       <c r="H22" s="7">
-        <v>4872.1406900000002</v>
+        <v>4858.8156920000001</v>
       </c>
       <c r="I22" s="7">
         <v>5056.3778770000008</v>
@@ -7114,7 +7114,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7535,7 +7535,7 @@
         <v>5417</v>
       </c>
       <c r="H5" s="15">
-        <v>0</v>
+        <v>5699</v>
       </c>
       <c r="I5" s="15">
         <v>0</v>
@@ -7697,7 +7697,7 @@
         <v>12127</v>
       </c>
       <c r="H6" s="6">
-        <v>0</v>
+        <v>13294</v>
       </c>
       <c r="I6" s="6">
         <v>0</v>
@@ -7859,7 +7859,7 @@
         <v>14064</v>
       </c>
       <c r="H7" s="6">
-        <v>0</v>
+        <v>15824</v>
       </c>
       <c r="I7" s="6">
         <v>0</v>
@@ -8021,7 +8021,7 @@
         <v>3939</v>
       </c>
       <c r="H8" s="6">
-        <v>0</v>
+        <v>3614</v>
       </c>
       <c r="I8" s="6">
         <v>0</v>
@@ -8183,7 +8183,7 @@
         <v>9258</v>
       </c>
       <c r="H9" s="6">
-        <v>0</v>
+        <v>8687</v>
       </c>
       <c r="I9" s="6">
         <v>0</v>
@@ -8345,7 +8345,7 @@
         <v>13238</v>
       </c>
       <c r="H10" s="15">
-        <v>0</v>
+        <v>13222</v>
       </c>
       <c r="I10" s="15">
         <v>0</v>
@@ -8507,7 +8507,7 @@
         <v>39278</v>
       </c>
       <c r="H11" s="6">
-        <v>0</v>
+        <v>38019</v>
       </c>
       <c r="I11" s="6">
         <v>0</v>
@@ -8669,7 +8669,7 @@
         <v>97321</v>
       </c>
       <c r="H12" s="7">
-        <v>0</v>
+        <v>98359</v>
       </c>
       <c r="I12" s="7">
         <v>0</v>
@@ -8893,7 +8893,7 @@
         <v>390.40495800000002</v>
       </c>
       <c r="H15" s="15">
-        <v>0</v>
+        <v>423.70802800000001</v>
       </c>
       <c r="I15" s="15">
         <v>0</v>
@@ -9055,7 +9055,7 @@
         <v>833.34708599999999</v>
       </c>
       <c r="H16" s="6">
-        <v>0</v>
+        <v>981.10243700000001</v>
       </c>
       <c r="I16" s="6">
         <v>0</v>
@@ -9217,7 +9217,7 @@
         <v>374.94750099999999</v>
       </c>
       <c r="H17" s="6">
-        <v>0</v>
+        <v>588.44481099999996</v>
       </c>
       <c r="I17" s="6">
         <v>0</v>
@@ -9379,7 +9379,7 @@
         <v>58.281337999999998</v>
       </c>
       <c r="H18" s="6">
-        <v>0</v>
+        <v>50.971986999999999</v>
       </c>
       <c r="I18" s="6">
         <v>0</v>
@@ -9541,7 +9541,7 @@
         <v>448.47666900000002</v>
       </c>
       <c r="H19" s="6">
-        <v>0</v>
+        <v>375.38917600000002</v>
       </c>
       <c r="I19" s="6">
         <v>0</v>
@@ -9703,7 +9703,7 @@
         <v>1261.592337</v>
       </c>
       <c r="H20" s="15">
-        <v>0</v>
+        <v>1252.9104159999999</v>
       </c>
       <c r="I20" s="15">
         <v>0</v>
@@ -9865,7 +9865,7 @@
         <v>955.18045300000006</v>
       </c>
       <c r="H21" s="6">
-        <v>0</v>
+        <v>930.29922199999999</v>
       </c>
       <c r="I21" s="6">
         <v>0</v>
@@ -10027,7 +10027,7 @@
         <v>4322.2303419999998</v>
       </c>
       <c r="H22" s="7">
-        <v>0</v>
+        <v>4602.8260769999997</v>
       </c>
       <c r="I22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Feb 25 05:26:51 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF410DBF-771A-498C-9F06-08DAA3BD642A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE90835C-CA77-4AF4-8BA4-F1B6C56ADCF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -4017,12 +4017,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4445,7 +4445,7 @@
         <v>6290</v>
       </c>
       <c r="I5" s="15">
-        <v>6372</v>
+        <v>6352</v>
       </c>
       <c r="J5" s="15">
         <v>6147</v>
@@ -4606,7 +4606,7 @@
         <v>13026</v>
       </c>
       <c r="I6" s="15">
-        <v>13446</v>
+        <v>13388</v>
       </c>
       <c r="J6" s="15">
         <v>12653</v>
@@ -4767,7 +4767,7 @@
         <v>18992</v>
       </c>
       <c r="I7" s="15">
-        <v>19954</v>
+        <v>20900</v>
       </c>
       <c r="J7" s="15">
         <v>15891</v>
@@ -5089,7 +5089,7 @@
         <v>9308</v>
       </c>
       <c r="I9" s="15">
-        <v>8653</v>
+        <v>8547</v>
       </c>
       <c r="J9" s="15">
         <v>9241</v>
@@ -5250,7 +5250,7 @@
         <v>13754</v>
       </c>
       <c r="I10" s="15">
-        <v>15846</v>
+        <v>15847</v>
       </c>
       <c r="J10" s="15">
         <v>13618</v>
@@ -5411,7 +5411,7 @@
         <v>42122</v>
       </c>
       <c r="I11" s="15">
-        <v>40915</v>
+        <v>40779</v>
       </c>
       <c r="J11" s="15">
         <v>41131</v>
@@ -5572,7 +5572,7 @@
         <v>107509</v>
       </c>
       <c r="I12" s="7">
-        <v>109195</v>
+        <v>109822</v>
       </c>
       <c r="J12" s="7">
         <v>102496</v>
@@ -5793,7 +5793,7 @@
         <v>474.13445000000002</v>
       </c>
       <c r="I15" s="15">
-        <v>473.62317100000001</v>
+        <v>472.66380900000001</v>
       </c>
       <c r="J15" s="15">
         <v>447.49052899999998</v>
@@ -5954,7 +5954,7 @@
         <v>937.48103100000003</v>
       </c>
       <c r="I16" s="15">
-        <v>949.24278500000003</v>
+        <v>947.71999000000005</v>
       </c>
       <c r="J16" s="15">
         <v>902.92713000000003</v>
@@ -6115,7 +6115,7 @@
         <v>632.09177</v>
       </c>
       <c r="I17" s="15">
-        <v>616.20216600000003</v>
+        <v>621.95108400000004</v>
       </c>
       <c r="J17" s="15">
         <v>599.68771700000002</v>
@@ -6276,7 +6276,7 @@
         <v>57.584921999999999</v>
       </c>
       <c r="I18" s="15">
-        <v>59.422866999999997</v>
+        <v>59.419797000000003</v>
       </c>
       <c r="J18" s="15">
         <v>51.939256999999998</v>
@@ -6437,7 +6437,7 @@
         <v>371.83031</v>
       </c>
       <c r="I19" s="15">
-        <v>327.11115799999999</v>
+        <v>327.234938</v>
       </c>
       <c r="J19" s="15">
         <v>381.10612500000002</v>
@@ -6598,7 +6598,7 @@
         <v>1396.0078759999999</v>
       </c>
       <c r="I20" s="15">
-        <v>1609.5020440000001</v>
+        <v>1609.6643590000001</v>
       </c>
       <c r="J20" s="15">
         <v>1270.1042829999999</v>
@@ -6759,7 +6759,7 @@
         <v>989.68533300000001</v>
       </c>
       <c r="I21" s="15">
-        <v>1021.273686</v>
+        <v>1019.962046</v>
       </c>
       <c r="J21" s="15">
         <v>999.58056199999999</v>
@@ -6920,7 +6920,7 @@
         <v>4858.8156920000001</v>
       </c>
       <c r="I22" s="7">
-        <v>5056.3778770000008</v>
+        <v>5058.6160229999996</v>
       </c>
       <c r="J22" s="7">
         <v>4652.8356029999995</v>
@@ -7109,7 +7109,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
@@ -7538,7 +7538,7 @@
         <v>5699</v>
       </c>
       <c r="I5" s="15">
-        <v>0</v>
+        <v>5290</v>
       </c>
       <c r="J5" s="15">
         <v>0</v>
@@ -7700,7 +7700,7 @@
         <v>13294</v>
       </c>
       <c r="I6" s="6">
-        <v>0</v>
+        <v>12105</v>
       </c>
       <c r="J6" s="6">
         <v>0</v>
@@ -7862,7 +7862,7 @@
         <v>15824</v>
       </c>
       <c r="I7" s="6">
-        <v>0</v>
+        <v>14941</v>
       </c>
       <c r="J7" s="6">
         <v>0</v>
@@ -8024,7 +8024,7 @@
         <v>3614</v>
       </c>
       <c r="I8" s="6">
-        <v>0</v>
+        <v>4082</v>
       </c>
       <c r="J8" s="6">
         <v>0</v>
@@ -8186,7 +8186,7 @@
         <v>8687</v>
       </c>
       <c r="I9" s="6">
-        <v>0</v>
+        <v>7952</v>
       </c>
       <c r="J9" s="6">
         <v>0</v>
@@ -8348,7 +8348,7 @@
         <v>13222</v>
       </c>
       <c r="I10" s="15">
-        <v>0</v>
+        <v>9499</v>
       </c>
       <c r="J10" s="15">
         <v>0</v>
@@ -8510,7 +8510,7 @@
         <v>38019</v>
       </c>
       <c r="I11" s="6">
-        <v>0</v>
+        <v>30511</v>
       </c>
       <c r="J11" s="6">
         <v>0</v>
@@ -8672,7 +8672,7 @@
         <v>98359</v>
       </c>
       <c r="I12" s="7">
-        <v>0</v>
+        <v>84380</v>
       </c>
       <c r="J12" s="7">
         <v>0</v>
@@ -8896,7 +8896,7 @@
         <v>423.70802800000001</v>
       </c>
       <c r="I15" s="15">
-        <v>0</v>
+        <v>394.04827899999998</v>
       </c>
       <c r="J15" s="15">
         <v>0</v>
@@ -9058,7 +9058,7 @@
         <v>981.10243700000001</v>
       </c>
       <c r="I16" s="6">
-        <v>0</v>
+        <v>872.53568199999995</v>
       </c>
       <c r="J16" s="6">
         <v>0</v>
@@ -9220,7 +9220,7 @@
         <v>588.44481099999996</v>
       </c>
       <c r="I17" s="6">
-        <v>0</v>
+        <v>491.346341</v>
       </c>
       <c r="J17" s="6">
         <v>0</v>
@@ -9382,7 +9382,7 @@
         <v>50.971986999999999</v>
       </c>
       <c r="I18" s="6">
-        <v>0</v>
+        <v>70.632895000000005</v>
       </c>
       <c r="J18" s="6">
         <v>0</v>
@@ -9544,7 +9544,7 @@
         <v>375.38917600000002</v>
       </c>
       <c r="I19" s="6">
-        <v>0</v>
+        <v>342.425207</v>
       </c>
       <c r="J19" s="6">
         <v>0</v>
@@ -9706,7 +9706,7 @@
         <v>1252.9104159999999</v>
       </c>
       <c r="I20" s="15">
-        <v>0</v>
+        <v>803.46545400000002</v>
       </c>
       <c r="J20" s="15">
         <v>0</v>
@@ -9868,7 +9868,7 @@
         <v>930.29922199999999</v>
       </c>
       <c r="I21" s="6">
-        <v>0</v>
+        <v>766.710016</v>
       </c>
       <c r="J21" s="6">
         <v>0</v>
@@ -10030,7 +10030,7 @@
         <v>4602.8260769999997</v>
       </c>
       <c r="I22" s="7">
-        <v>0</v>
+        <v>3741.1638739999999</v>
       </c>
       <c r="J22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Mar  4 05:26:51 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE90835C-CA77-4AF4-8BA4-F1B6C56ADCF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A2F12B-8BDF-4B63-BFE6-FD46E30CF262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -4017,12 +4017,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4448,7 +4448,7 @@
         <v>6352</v>
       </c>
       <c r="J5" s="15">
-        <v>6147</v>
+        <v>6119</v>
       </c>
       <c r="K5" s="15">
         <v>6149</v>
@@ -4609,7 +4609,7 @@
         <v>13388</v>
       </c>
       <c r="J6" s="15">
-        <v>12653</v>
+        <v>12590</v>
       </c>
       <c r="K6" s="15">
         <v>12800</v>
@@ -4770,7 +4770,7 @@
         <v>20900</v>
       </c>
       <c r="J7" s="15">
-        <v>15891</v>
+        <v>16401</v>
       </c>
       <c r="K7" s="15">
         <v>18376</v>
@@ -4931,7 +4931,7 @@
         <v>4009</v>
       </c>
       <c r="J8" s="15">
-        <v>3815</v>
+        <v>3803</v>
       </c>
       <c r="K8" s="15">
         <v>4120</v>
@@ -5092,7 +5092,7 @@
         <v>8547</v>
       </c>
       <c r="J9" s="15">
-        <v>9241</v>
+        <v>9257</v>
       </c>
       <c r="K9" s="15">
         <v>7748</v>
@@ -5253,7 +5253,7 @@
         <v>15847</v>
       </c>
       <c r="J10" s="15">
-        <v>13618</v>
+        <v>13512</v>
       </c>
       <c r="K10" s="15">
         <v>12788</v>
@@ -5414,7 +5414,7 @@
         <v>40779</v>
       </c>
       <c r="J11" s="15">
-        <v>41131</v>
+        <v>41024</v>
       </c>
       <c r="K11" s="15">
         <v>41647</v>
@@ -5575,7 +5575,7 @@
         <v>109822</v>
       </c>
       <c r="J12" s="7">
-        <v>102496</v>
+        <v>102706</v>
       </c>
       <c r="K12" s="7">
         <v>103628</v>
@@ -5796,7 +5796,7 @@
         <v>472.66380900000001</v>
       </c>
       <c r="J15" s="15">
-        <v>447.49052899999998</v>
+        <v>445.84954399999998</v>
       </c>
       <c r="K15" s="15">
         <v>466.31968799999999</v>
@@ -5957,7 +5957,7 @@
         <v>947.71999000000005</v>
       </c>
       <c r="J16" s="15">
-        <v>902.92713000000003</v>
+        <v>902.32816800000001</v>
       </c>
       <c r="K16" s="15">
         <v>876.91640600000005</v>
@@ -6118,7 +6118,7 @@
         <v>621.95108400000004</v>
       </c>
       <c r="J17" s="15">
-        <v>599.68771700000002</v>
+        <v>598.77639299999998</v>
       </c>
       <c r="K17" s="15">
         <v>567.14239299999997</v>
@@ -6279,7 +6279,7 @@
         <v>59.419797000000003</v>
       </c>
       <c r="J18" s="15">
-        <v>51.939256999999998</v>
+        <v>51.623075</v>
       </c>
       <c r="K18" s="15">
         <v>61.927047999999999</v>
@@ -6440,7 +6440,7 @@
         <v>327.234938</v>
       </c>
       <c r="J19" s="15">
-        <v>381.10612500000002</v>
+        <v>381.87694299999998</v>
       </c>
       <c r="K19" s="15">
         <v>347.01898799999998</v>
@@ -6601,7 +6601,7 @@
         <v>1609.6643590000001</v>
       </c>
       <c r="J20" s="15">
-        <v>1270.1042829999999</v>
+        <v>1257.9603010000001</v>
       </c>
       <c r="K20" s="15">
         <v>1186.295012</v>
@@ -6762,7 +6762,7 @@
         <v>1019.962046</v>
       </c>
       <c r="J21" s="15">
-        <v>999.58056199999999</v>
+        <v>998.43278899999996</v>
       </c>
       <c r="K21" s="15">
         <v>1017.054289</v>
@@ -6923,7 +6923,7 @@
         <v>5058.6160229999996</v>
       </c>
       <c r="J22" s="7">
-        <v>4652.8356029999995</v>
+        <v>4636.8472129999991</v>
       </c>
       <c r="K22" s="7">
         <v>4522.6738239999995</v>
@@ -7109,12 +7109,12 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7541,7 +7541,7 @@
         <v>5290</v>
       </c>
       <c r="J5" s="15">
-        <v>0</v>
+        <v>5781</v>
       </c>
       <c r="K5" s="15">
         <v>0</v>
@@ -7703,7 +7703,7 @@
         <v>12105</v>
       </c>
       <c r="J6" s="6">
-        <v>0</v>
+        <v>13786</v>
       </c>
       <c r="K6" s="6">
         <v>0</v>
@@ -7865,7 +7865,7 @@
         <v>14941</v>
       </c>
       <c r="J7" s="6">
-        <v>0</v>
+        <v>16681</v>
       </c>
       <c r="K7" s="6">
         <v>0</v>
@@ -8027,7 +8027,7 @@
         <v>4082</v>
       </c>
       <c r="J8" s="6">
-        <v>0</v>
+        <v>4176</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
@@ -8189,7 +8189,7 @@
         <v>7952</v>
       </c>
       <c r="J9" s="6">
-        <v>0</v>
+        <v>9257</v>
       </c>
       <c r="K9" s="6">
         <v>0</v>
@@ -8351,7 +8351,7 @@
         <v>9499</v>
       </c>
       <c r="J10" s="15">
-        <v>0</v>
+        <v>14353</v>
       </c>
       <c r="K10" s="15">
         <v>0</v>
@@ -8513,7 +8513,7 @@
         <v>30511</v>
       </c>
       <c r="J11" s="6">
-        <v>0</v>
+        <v>38673</v>
       </c>
       <c r="K11" s="6">
         <v>0</v>
@@ -8675,7 +8675,7 @@
         <v>84380</v>
       </c>
       <c r="J12" s="7">
-        <v>0</v>
+        <v>102707</v>
       </c>
       <c r="K12" s="7">
         <v>0</v>
@@ -8899,7 +8899,7 @@
         <v>394.04827899999998</v>
       </c>
       <c r="J15" s="15">
-        <v>0</v>
+        <v>420.79112700000002</v>
       </c>
       <c r="K15" s="15">
         <v>0</v>
@@ -9061,7 +9061,7 @@
         <v>872.53568199999995</v>
       </c>
       <c r="J16" s="6">
-        <v>0</v>
+        <v>1062.701914</v>
       </c>
       <c r="K16" s="6">
         <v>0</v>
@@ -9223,7 +9223,7 @@
         <v>491.346341</v>
       </c>
       <c r="J17" s="6">
-        <v>0</v>
+        <v>559.656656</v>
       </c>
       <c r="K17" s="6">
         <v>0</v>
@@ -9385,7 +9385,7 @@
         <v>70.632895000000005</v>
       </c>
       <c r="J18" s="6">
-        <v>0</v>
+        <v>65.936772000000005</v>
       </c>
       <c r="K18" s="6">
         <v>0</v>
@@ -9547,7 +9547,7 @@
         <v>342.425207</v>
       </c>
       <c r="J19" s="6">
-        <v>0</v>
+        <v>401.23970000000003</v>
       </c>
       <c r="K19" s="6">
         <v>0</v>
@@ -9709,7 +9709,7 @@
         <v>803.46545400000002</v>
       </c>
       <c r="J20" s="15">
-        <v>0</v>
+        <v>1420.170883</v>
       </c>
       <c r="K20" s="15">
         <v>0</v>
@@ -9871,7 +9871,7 @@
         <v>766.710016</v>
       </c>
       <c r="J21" s="6">
-        <v>0</v>
+        <v>947.92271700000003</v>
       </c>
       <c r="K21" s="6">
         <v>0</v>
@@ -10033,7 +10033,7 @@
         <v>3741.1638739999999</v>
       </c>
       <c r="J22" s="7">
-        <v>0</v>
+        <v>4878.4197690000001</v>
       </c>
       <c r="K22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Mar 11 05:27:19 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A2F12B-8BDF-4B63-BFE6-FD46E30CF262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8D7572-F577-453B-89DB-572467F19C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -968,16 +968,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="9" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="9"/>
+    <col min="1" max="1" width="50.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="9" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -1034,7 +1034,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -1356,12 +1356,12 @@
         <v>42365</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>6942</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>11626</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>12499</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>6294</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>81196</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2704,12 +2704,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>470.98508700000002</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>958.98562200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>296.27038100000027</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>48.659481</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>212.439166</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>901.73460399999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>700.69452899999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>3589.7688700000003</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -4019,22 +4019,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -4091,7 +4091,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -4252,7 +4252,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -4414,12 +4414,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>6119</v>
       </c>
       <c r="K5" s="15">
-        <v>6149</v>
+        <v>6120</v>
       </c>
       <c r="L5" s="15">
         <v>6399</v>
@@ -4580,7 +4580,7 @@
         <v>4363</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>12590</v>
       </c>
       <c r="K6" s="15">
-        <v>12800</v>
+        <v>12756</v>
       </c>
       <c r="L6" s="15">
         <v>13025</v>
@@ -4741,7 +4741,7 @@
         <v>11478</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>16401</v>
       </c>
       <c r="K7" s="15">
-        <v>18376</v>
+        <v>18839</v>
       </c>
       <c r="L7" s="15">
         <v>19817</v>
@@ -4902,7 +4902,7 @@
         <v>16410</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>3803</v>
       </c>
       <c r="K8" s="15">
-        <v>4120</v>
+        <v>4110</v>
       </c>
       <c r="L8" s="15">
         <v>4695</v>
@@ -5063,7 +5063,7 @@
         <v>2807</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>9257</v>
       </c>
       <c r="K9" s="15">
-        <v>7748</v>
+        <v>7596</v>
       </c>
       <c r="L9" s="15">
         <v>9693</v>
@@ -5224,7 +5224,7 @@
         <v>8047</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>13512</v>
       </c>
       <c r="K10" s="15">
-        <v>12788</v>
+        <v>12929</v>
       </c>
       <c r="L10" s="15">
         <v>13581</v>
@@ -5385,7 +5385,7 @@
         <v>12133</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>41024</v>
       </c>
       <c r="K11" s="15">
-        <v>41647</v>
+        <v>41511</v>
       </c>
       <c r="L11" s="15">
         <v>42551</v>
@@ -5546,7 +5546,7 @@
         <v>29432</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>102706</v>
       </c>
       <c r="K12" s="7">
-        <v>103628</v>
+        <v>103861</v>
       </c>
       <c r="L12" s="7">
         <v>109761</v>
@@ -5707,7 +5707,7 @@
         <v>84670</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5762,12 +5762,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>445.84954399999998</v>
       </c>
       <c r="K15" s="15">
-        <v>466.31968799999999</v>
+        <v>464.899541</v>
       </c>
       <c r="L15" s="15">
         <v>493.06481700000001</v>
@@ -5928,7 +5928,7 @@
         <v>303.44771800000001</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>902.32816800000001</v>
       </c>
       <c r="K16" s="15">
-        <v>876.91640600000005</v>
+        <v>877.45966099999998</v>
       </c>
       <c r="L16" s="15">
         <v>883.25571000000002</v>
@@ -6089,7 +6089,7 @@
         <v>868.11864300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -6121,7 +6121,7 @@
         <v>598.77639299999998</v>
       </c>
       <c r="K17" s="15">
-        <v>567.14239299999997</v>
+        <v>570.15315899999996</v>
       </c>
       <c r="L17" s="15">
         <v>618.36236199999996</v>
@@ -6250,7 +6250,7 @@
         <v>433.165955</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -6282,7 +6282,7 @@
         <v>51.623075</v>
       </c>
       <c r="K18" s="15">
-        <v>61.927047999999999</v>
+        <v>61.761665999999998</v>
       </c>
       <c r="L18" s="15">
         <v>63.587826</v>
@@ -6411,7 +6411,7 @@
         <v>42.773207999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -6443,7 +6443,7 @@
         <v>381.87694299999998</v>
       </c>
       <c r="K19" s="15">
-        <v>347.01898799999998</v>
+        <v>342.59989000000002</v>
       </c>
       <c r="L19" s="15">
         <v>389.36037700000003</v>
@@ -6572,7 +6572,7 @@
         <v>374.79168900000002</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -6604,7 +6604,7 @@
         <v>1257.9603010000001</v>
       </c>
       <c r="K20" s="15">
-        <v>1186.295012</v>
+        <v>1209.475496</v>
       </c>
       <c r="L20" s="15">
         <v>1430.9612609999999</v>
@@ -6733,7 +6733,7 @@
         <v>1143.806075</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -6765,7 +6765,7 @@
         <v>998.43278899999996</v>
       </c>
       <c r="K21" s="15">
-        <v>1017.054289</v>
+        <v>1015.4275699999999</v>
       </c>
       <c r="L21" s="15">
         <v>984.28798800000004</v>
@@ -6894,7 +6894,7 @@
         <v>657.70498399999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>4636.8472129999991</v>
       </c>
       <c r="K22" s="7">
-        <v>4522.6738239999995</v>
+        <v>4541.7769830000007</v>
       </c>
       <c r="L22" s="7">
         <v>4862.880341</v>
@@ -7055,40 +7055,40 @@
         <v>3823.8082720000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -7111,22 +7111,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="53" width="9.42578125" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.42578125" customWidth="1"/>
-    <col min="55" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="53" width="9.44140625" style="1" customWidth="1"/>
+    <col min="54" max="54" width="9.44140625" customWidth="1"/>
+    <col min="55" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -7183,7 +7183,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -7344,7 +7344,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -7506,13 +7506,13 @@
       </c>
       <c r="BB3" s="24"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>5781</v>
       </c>
       <c r="K5" s="15">
-        <v>0</v>
+        <v>5699</v>
       </c>
       <c r="L5" s="15">
         <v>0</v>
@@ -7674,7 +7674,7 @@
       </c>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>13786</v>
       </c>
       <c r="K6" s="6">
-        <v>0</v>
+        <v>12675</v>
       </c>
       <c r="L6" s="6">
         <v>0</v>
@@ -7836,7 +7836,7 @@
       </c>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -7868,7 +7868,7 @@
         <v>16681</v>
       </c>
       <c r="K7" s="6">
-        <v>0</v>
+        <v>16977</v>
       </c>
       <c r="L7" s="6">
         <v>0</v>
@@ -7998,7 +7998,7 @@
       </c>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>4176</v>
       </c>
       <c r="K8" s="6">
-        <v>0</v>
+        <v>4189</v>
       </c>
       <c r="L8" s="6">
         <v>0</v>
@@ -8160,7 +8160,7 @@
       </c>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -8192,7 +8192,7 @@
         <v>9257</v>
       </c>
       <c r="K9" s="6">
-        <v>0</v>
+        <v>8725</v>
       </c>
       <c r="L9" s="6">
         <v>0</v>
@@ -8322,7 +8322,7 @@
       </c>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -8354,7 +8354,7 @@
         <v>14353</v>
       </c>
       <c r="K10" s="15">
-        <v>0</v>
+        <v>14251</v>
       </c>
       <c r="L10" s="15">
         <v>0</v>
@@ -8484,7 +8484,7 @@
       </c>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -8516,7 +8516,7 @@
         <v>38673</v>
       </c>
       <c r="K11" s="6">
-        <v>0</v>
+        <v>41092</v>
       </c>
       <c r="L11" s="6">
         <v>0</v>
@@ -8646,7 +8646,7 @@
       </c>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -8678,7 +8678,7 @@
         <v>102707</v>
       </c>
       <c r="K12" s="7">
-        <v>0</v>
+        <v>103608</v>
       </c>
       <c r="L12" s="7">
         <v>0</v>
@@ -8808,7 +8808,7 @@
       </c>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -8864,13 +8864,13 @@
       <c r="BA13" s="6"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -8902,7 +8902,7 @@
         <v>420.79112700000002</v>
       </c>
       <c r="K15" s="15">
-        <v>0</v>
+        <v>423.812952</v>
       </c>
       <c r="L15" s="15">
         <v>0</v>
@@ -9032,7 +9032,7 @@
       </c>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -9064,7 +9064,7 @@
         <v>1062.701914</v>
       </c>
       <c r="K16" s="6">
-        <v>0</v>
+        <v>899.76599799999997</v>
       </c>
       <c r="L16" s="6">
         <v>0</v>
@@ -9194,7 +9194,7 @@
       </c>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -9226,7 +9226,7 @@
         <v>559.656656</v>
       </c>
       <c r="K17" s="6">
-        <v>0</v>
+        <v>552.537509</v>
       </c>
       <c r="L17" s="6">
         <v>0</v>
@@ -9356,7 +9356,7 @@
       </c>
       <c r="BB17"/>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -9388,7 +9388,7 @@
         <v>65.936772000000005</v>
       </c>
       <c r="K18" s="6">
-        <v>0</v>
+        <v>66.000795999999994</v>
       </c>
       <c r="L18" s="6">
         <v>0</v>
@@ -9518,7 +9518,7 @@
       </c>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9550,7 +9550,7 @@
         <v>401.23970000000003</v>
       </c>
       <c r="K19" s="6">
-        <v>0</v>
+        <v>410.18394699999999</v>
       </c>
       <c r="L19" s="6">
         <v>0</v>
@@ -9680,7 +9680,7 @@
       </c>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -9712,7 +9712,7 @@
         <v>1420.170883</v>
       </c>
       <c r="K20" s="15">
-        <v>0</v>
+        <v>1342.8301570000001</v>
       </c>
       <c r="L20" s="15">
         <v>0</v>
@@ -9842,7 +9842,7 @@
       </c>
       <c r="BB20"/>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -9874,7 +9874,7 @@
         <v>947.92271700000003</v>
       </c>
       <c r="K21" s="6">
-        <v>0</v>
+        <v>1000.475224</v>
       </c>
       <c r="L21" s="6">
         <v>0</v>
@@ -10004,7 +10004,7 @@
       </c>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10036,7 +10036,7 @@
         <v>4878.4197690000001</v>
       </c>
       <c r="K22" s="7">
-        <v>0</v>
+        <v>4695.6065829999998</v>
       </c>
       <c r="L22" s="7">
         <v>0</v>
@@ -10166,100 +10166,100 @@
       </c>
       <c r="BB22"/>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="BB23"/>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB24"/>
     </row>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB25"/>
     </row>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB26"/>
     </row>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB27"/>
     </row>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB28"/>
     </row>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB29"/>
     </row>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB30"/>
     </row>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB31"/>
     </row>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB32"/>
     </row>
-    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB33"/>
     </row>
-    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB34"/>
     </row>
-    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB35"/>
     </row>
-    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB36"/>
     </row>
-    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB37"/>
     </row>
-    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB38"/>
     </row>
-    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB39"/>
     </row>
-    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB40"/>
     </row>
-    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB41"/>
     </row>
-    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB42"/>
     </row>
-    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB43"/>
     </row>
-    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB44"/>
     </row>
-    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB45"/>
     </row>
-    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB46"/>
     </row>
-    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB47"/>
     </row>
-    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB48"/>
     </row>
-    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB49"/>
     </row>
-    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB50"/>
     </row>
-    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB51"/>
     </row>
-    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB52"/>
     </row>
-    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB53"/>
     </row>
-    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB54"/>
     </row>
   </sheetData>
@@ -10289,16 +10289,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="17" customWidth="1"/>
     <col min="53" max="53" width="9" style="17" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="17"/>
+    <col min="54" max="16384" width="6.6640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -10355,7 +10355,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -10516,7 +10516,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -10678,12 +10678,12 @@
       </c>
       <c r="BB3" s="23"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -10844,7 +10844,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -11005,7 +11005,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -11166,7 +11166,7 @@
         <v>15693</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -11327,7 +11327,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -11488,7 +11488,7 @@
         <v>6531</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11649,7 +11649,7 @@
         <v>10908</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -11810,7 +11810,7 @@
         <v>33194</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -11971,7 +11971,7 @@
         <v>88077</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -12026,12 +12026,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -12192,7 +12192,7 @@
         <v>448.48865799999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -12353,7 +12353,7 @@
         <v>863.31579299999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -12514,7 +12514,7 @@
         <v>424.08659699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -12675,7 +12675,7 @@
         <v>49.649962000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -12836,7 +12836,7 @@
         <v>235.51133100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -12997,7 +12997,7 @@
         <v>961.98002299999996</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -13158,7 +13158,7 @@
         <v>764.98213299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -13319,38 +13319,38 @@
         <v>3748.0144969999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -13379,16 +13379,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
@@ -13445,7 +13445,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -13606,7 +13606,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -13767,12 +13767,12 @@
         <v>43093</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -13933,7 +13933,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -14094,7 +14094,7 @@
         <v>9513</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -14255,7 +14255,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -14416,7 +14416,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -14577,7 +14577,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -14738,7 +14738,7 @@
         <v>9414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -14899,7 +14899,7 @@
         <v>36964</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -15060,7 +15060,7 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -15115,12 +15115,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -15281,7 +15281,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -15442,7 +15442,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -15603,7 +15603,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -15764,7 +15764,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -15925,7 +15925,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -16086,7 +16086,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -16247,7 +16247,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -16408,38 +16408,38 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -16464,16 +16464,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
     <col min="53" max="53" width="9" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -16530,7 +16530,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16691,7 +16691,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -16853,12 +16853,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -17019,7 +17019,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -17180,7 +17180,7 @@
         <v>12729</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -17341,7 +17341,7 @@
         <v>16661</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -17502,7 +17502,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -17663,7 +17663,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -17824,7 +17824,7 @@
         <v>12175</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -17985,7 +17985,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -18146,7 +18146,7 @@
         <v>97169</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -18201,12 +18201,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -18367,7 +18367,7 @@
         <v>345.26898999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -18528,7 +18528,7 @@
         <v>1137.3429249999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -18689,7 +18689,7 @@
         <v>337.41420499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -18850,7 +18850,7 @@
         <v>40.33334</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -19011,7 +19011,7 @@
         <v>339.10771799999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -19172,7 +19172,7 @@
         <v>1247.683331</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -19333,7 +19333,7 @@
         <v>821.21724600000005</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -19494,38 +19494,38 @@
         <v>4268.3677550000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -19542,16 +19542,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -19608,7 +19608,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -19769,7 +19769,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -19931,12 +19931,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -20097,7 +20097,7 @@
         <v>5356</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -20258,7 +20258,7 @@
         <v>12576</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -20419,7 +20419,7 @@
         <v>17944</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -20580,7 +20580,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -20741,7 +20741,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -20902,7 +20902,7 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -21063,7 +21063,7 @@
         <v>38154</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -21224,7 +21224,7 @@
         <v>92789</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -21279,12 +21279,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -21445,7 +21445,7 @@
         <v>356.60756500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -21606,7 +21606,7 @@
         <v>977.829027</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -21767,7 +21767,7 @@
         <v>495.993199</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -21928,7 +21928,7 @@
         <v>37.412531000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -22089,7 +22089,7 @@
         <v>351.68923999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -22250,7 +22250,7 @@
         <v>888.50449000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -22411,7 +22411,7 @@
         <v>804.61703199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -22572,38 +22572,38 @@
         <v>3912.6530840000005</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -22620,17 +22620,17 @@
       <selection activeCell="A5" sqref="A5:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
@@ -22687,7 +22687,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -22851,7 +22851,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -23013,7 +23013,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -23177,12 +23177,12 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -23346,7 +23346,7 @@
         <v>6187</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -23510,7 +23510,7 @@
         <v>11221</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -23674,7 +23674,7 @@
         <v>16946</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -23838,7 +23838,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
@@ -24002,7 +24002,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -24166,7 +24166,7 @@
         <v>13026</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -24330,7 +24330,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -24494,7 +24494,7 @@
         <v>99721</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -24550,12 +24550,12 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -24719,7 +24719,7 @@
         <v>469.697947</v>
       </c>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -24883,7 +24883,7 @@
         <v>800.96283800000003</v>
       </c>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -25047,7 +25047,7 @@
         <v>463.52606100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
@@ -25211,7 +25211,7 @@
         <v>39.121160000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -25375,7 +25375,7 @@
         <v>320.92344600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -25539,7 +25539,7 @@
         <v>1254.2732289999999</v>
       </c>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -25703,7 +25703,7 @@
         <v>905.27916400000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -25867,38 +25867,38 @@
         <v>4253.7838449999999</v>
       </c>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -25919,16 +25919,16 @@
       <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
@@ -25985,7 +25985,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -26146,7 +26146,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -26308,12 +26308,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -26474,7 +26474,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -26635,7 +26635,7 @@
         <v>10430</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -26796,7 +26796,7 @@
         <v>15971</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -26957,7 +26957,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -27118,7 +27118,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -27279,7 +27279,7 @@
         <v>8618</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -27440,7 +27440,7 @@
         <v>34889</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -27601,7 +27601,7 @@
         <v>83267</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -27656,12 +27656,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -27822,7 +27822,7 @@
         <v>326.63437199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -27983,7 +27983,7 @@
         <v>710.31911300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -28144,7 +28144,7 @@
         <v>390.89581099999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -28305,7 +28305,7 @@
         <v>36.150655</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -28466,7 +28466,7 @@
         <v>232.43127799999999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -28627,7 +28627,7 @@
         <v>750.77748799999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -28788,7 +28788,7 @@
         <v>735.26635299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28949,40 +28949,40 @@
         <v>3182.4750699999995</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -29010,16 +29010,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -29076,7 +29076,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -29237,7 +29237,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -29399,12 +29399,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -29565,7 +29565,7 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -29726,7 +29726,7 @@
         <v>11045</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -29887,7 +29887,7 @@
         <v>14998</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -30048,7 +30048,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -30209,7 +30209,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -30370,7 +30370,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -30531,7 +30531,7 @@
         <v>31551</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -30692,7 +30692,7 @@
         <v>81088</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -30747,12 +30747,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -30913,7 +30913,7 @@
         <v>307.73157300000003</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -31074,7 +31074,7 @@
         <v>782.92677600000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -31235,7 +31235,7 @@
         <v>401.64126599999997</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -31396,7 +31396,7 @@
         <v>32.955354</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -31557,7 +31557,7 @@
         <v>272.11873100000003</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -31718,7 +31718,7 @@
         <v>976.60348099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -31879,7 +31879,7 @@
         <v>752.63757299999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -32040,40 +32040,40 @@
         <v>3526.6147539999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -32101,16 +32101,16 @@
       <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -32167,7 +32167,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -32328,7 +32328,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -32490,12 +32490,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -32656,7 +32656,7 @@
         <v>4413</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -32817,7 +32817,7 @@
         <v>11673</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -32978,7 +32978,7 @@
         <v>15590</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -33139,7 +33139,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -33300,7 +33300,7 @@
         <v>8134</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -33461,7 +33461,7 @@
         <v>9863</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -33622,7 +33622,7 @@
         <v>34066</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -33783,7 +33783,7 @@
         <v>86245</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -33838,12 +33838,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -34004,7 +34004,7 @@
         <v>298.50642199999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -34165,7 +34165,7 @@
         <v>888.297684</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -34326,7 +34326,7 @@
         <v>533.92582100000004</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -34487,7 +34487,7 @@
         <v>38.857964000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -34648,7 +34648,7 @@
         <v>364.61675700000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -34809,7 +34809,7 @@
         <v>992.76339499999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -34970,7 +34970,7 @@
         <v>755.640308</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -35131,40 +35131,40 @@
         <v>3872.6083509999999</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Mar 18 05:28:06 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8D7572-F577-453B-89DB-572467F19C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CF1B9D-97FF-442F-80B9-6C249FDDBA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -4019,10 +4019,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4454,7 +4454,7 @@
         <v>6120</v>
       </c>
       <c r="L5" s="15">
-        <v>6399</v>
+        <v>6386</v>
       </c>
       <c r="M5" s="15">
         <v>6161</v>
@@ -4615,7 +4615,7 @@
         <v>12756</v>
       </c>
       <c r="L6" s="15">
-        <v>13025</v>
+        <v>12982</v>
       </c>
       <c r="M6" s="15">
         <v>12783</v>
@@ -4776,7 +4776,7 @@
         <v>18839</v>
       </c>
       <c r="L7" s="15">
-        <v>19817</v>
+        <v>20451</v>
       </c>
       <c r="M7" s="15">
         <v>18919</v>
@@ -4937,7 +4937,7 @@
         <v>4110</v>
       </c>
       <c r="L8" s="15">
-        <v>4695</v>
+        <v>4689</v>
       </c>
       <c r="M8" s="15">
         <v>4937</v>
@@ -5098,7 +5098,7 @@
         <v>7596</v>
       </c>
       <c r="L9" s="15">
-        <v>9693</v>
+        <v>9594</v>
       </c>
       <c r="M9" s="15">
         <v>8691</v>
@@ -5259,7 +5259,7 @@
         <v>12929</v>
       </c>
       <c r="L10" s="15">
-        <v>13581</v>
+        <v>13576</v>
       </c>
       <c r="M10" s="15">
         <v>13166</v>
@@ -5420,7 +5420,7 @@
         <v>41511</v>
       </c>
       <c r="L11" s="15">
-        <v>42551</v>
+        <v>42405</v>
       </c>
       <c r="M11" s="15">
         <v>44392</v>
@@ -5581,7 +5581,7 @@
         <v>103861</v>
       </c>
       <c r="L12" s="7">
-        <v>109761</v>
+        <v>110083</v>
       </c>
       <c r="M12" s="7">
         <v>109049</v>
@@ -5802,7 +5802,7 @@
         <v>464.899541</v>
       </c>
       <c r="L15" s="15">
-        <v>493.06481700000001</v>
+        <v>492.48873800000001</v>
       </c>
       <c r="M15" s="15">
         <v>450.87778700000001</v>
@@ -5963,7 +5963,7 @@
         <v>877.45966099999998</v>
       </c>
       <c r="L16" s="15">
-        <v>883.25571000000002</v>
+        <v>883.17675499999996</v>
       </c>
       <c r="M16" s="15">
         <v>883.60495400000002</v>
@@ -6124,7 +6124,7 @@
         <v>570.15315899999996</v>
       </c>
       <c r="L17" s="15">
-        <v>618.36236199999996</v>
+        <v>616.46194500000001</v>
       </c>
       <c r="M17" s="15">
         <v>640.99145899999996</v>
@@ -6285,7 +6285,7 @@
         <v>61.761665999999998</v>
       </c>
       <c r="L18" s="15">
-        <v>63.587826</v>
+        <v>63.479092999999999</v>
       </c>
       <c r="M18" s="15">
         <v>67.511683000000005</v>
@@ -6446,7 +6446,7 @@
         <v>342.59989000000002</v>
       </c>
       <c r="L19" s="15">
-        <v>389.36037700000003</v>
+        <v>389.92883399999999</v>
       </c>
       <c r="M19" s="15">
         <v>366.55915599999997</v>
@@ -6607,7 +6607,7 @@
         <v>1209.475496</v>
       </c>
       <c r="L20" s="15">
-        <v>1430.9612609999999</v>
+        <v>1430.9431979999999</v>
       </c>
       <c r="M20" s="15">
         <v>1315.179288</v>
@@ -6768,7 +6768,7 @@
         <v>1015.4275699999999</v>
       </c>
       <c r="L21" s="15">
-        <v>984.28798800000004</v>
+        <v>983.77560200000005</v>
       </c>
       <c r="M21" s="15">
         <v>1050.65993</v>
@@ -6929,7 +6929,7 @@
         <v>4541.7769830000007</v>
       </c>
       <c r="L22" s="7">
-        <v>4862.880341</v>
+        <v>4860.2541649999994</v>
       </c>
       <c r="M22" s="7">
         <v>4775.3842569999997</v>
@@ -7111,10 +7111,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7547,7 +7547,7 @@
         <v>5699</v>
       </c>
       <c r="L5" s="15">
-        <v>0</v>
+        <v>6180</v>
       </c>
       <c r="M5" s="15">
         <v>0</v>
@@ -7709,7 +7709,7 @@
         <v>12675</v>
       </c>
       <c r="L6" s="6">
-        <v>0</v>
+        <v>13187</v>
       </c>
       <c r="M6" s="6">
         <v>0</v>
@@ -7871,7 +7871,7 @@
         <v>16977</v>
       </c>
       <c r="L7" s="6">
-        <v>0</v>
+        <v>16428</v>
       </c>
       <c r="M7" s="6">
         <v>0</v>
@@ -8033,7 +8033,7 @@
         <v>4189</v>
       </c>
       <c r="L8" s="6">
-        <v>0</v>
+        <v>4664</v>
       </c>
       <c r="M8" s="6">
         <v>0</v>
@@ -8195,7 +8195,7 @@
         <v>8725</v>
       </c>
       <c r="L9" s="6">
-        <v>0</v>
+        <v>9481</v>
       </c>
       <c r="M9" s="6">
         <v>0</v>
@@ -8357,7 +8357,7 @@
         <v>14251</v>
       </c>
       <c r="L10" s="15">
-        <v>0</v>
+        <v>15079</v>
       </c>
       <c r="M10" s="15">
         <v>0</v>
@@ -8519,7 +8519,7 @@
         <v>41092</v>
       </c>
       <c r="L11" s="6">
-        <v>0</v>
+        <v>42692</v>
       </c>
       <c r="M11" s="6">
         <v>0</v>
@@ -8681,7 +8681,7 @@
         <v>103608</v>
       </c>
       <c r="L12" s="7">
-        <v>0</v>
+        <v>107711</v>
       </c>
       <c r="M12" s="7">
         <v>0</v>
@@ -8905,7 +8905,7 @@
         <v>423.812952</v>
       </c>
       <c r="L15" s="15">
-        <v>0</v>
+        <v>461.86728299999999</v>
       </c>
       <c r="M15" s="15">
         <v>0</v>
@@ -9067,7 +9067,7 @@
         <v>899.76599799999997</v>
       </c>
       <c r="L16" s="6">
-        <v>0</v>
+        <v>989.07336199999997</v>
       </c>
       <c r="M16" s="6">
         <v>0</v>
@@ -9229,7 +9229,7 @@
         <v>552.537509</v>
       </c>
       <c r="L17" s="6">
-        <v>0</v>
+        <v>581.18060400000002</v>
       </c>
       <c r="M17" s="6">
         <v>0</v>
@@ -9391,7 +9391,7 @@
         <v>66.000795999999994</v>
       </c>
       <c r="L18" s="6">
-        <v>0</v>
+        <v>77.609133</v>
       </c>
       <c r="M18" s="6">
         <v>0</v>
@@ -9553,7 +9553,7 @@
         <v>410.18394699999999</v>
       </c>
       <c r="L19" s="6">
-        <v>0</v>
+        <v>441.30929500000002</v>
       </c>
       <c r="M19" s="6">
         <v>0</v>
@@ -9715,7 +9715,7 @@
         <v>1342.8301570000001</v>
       </c>
       <c r="L20" s="15">
-        <v>0</v>
+        <v>1532.9125839999999</v>
       </c>
       <c r="M20" s="15">
         <v>0</v>
@@ -9877,7 +9877,7 @@
         <v>1000.475224</v>
       </c>
       <c r="L21" s="6">
-        <v>0</v>
+        <v>1025.102989</v>
       </c>
       <c r="M21" s="6">
         <v>0</v>
@@ -10039,7 +10039,7 @@
         <v>4695.6065829999998</v>
       </c>
       <c r="L22" s="7">
-        <v>0</v>
+        <v>5109.0552499999994</v>
       </c>
       <c r="M22" s="7">
         <v>0</v>
@@ -10274,6 +10274,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Mar 25 05:28:36 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CF1B9D-97FF-442F-80B9-6C249FDDBA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A2ECAB9-511F-40DB-8D40-9ABD2053E978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -965,19 +965,19 @@
       <selection activeCell="B4" sqref="B4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="9" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="9"/>
+    <col min="1" max="1" width="50.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="9" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -1034,7 +1034,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -1356,12 +1356,12 @@
         <v>42365</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>6942</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>11626</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>12499</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>6294</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>81196</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2704,12 +2704,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>470.98508700000002</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>958.98562200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>296.27038100000027</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>48.659481</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>212.439166</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>901.73460399999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>700.69452899999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>3589.7688700000003</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -4010,6 +4010,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -4019,22 +4022,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -4091,7 +4094,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -4252,7 +4255,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -4414,12 +4417,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4457,7 +4460,7 @@
         <v>6386</v>
       </c>
       <c r="M5" s="15">
-        <v>6161</v>
+        <v>6139</v>
       </c>
       <c r="N5" s="15">
         <v>6106</v>
@@ -4580,7 +4583,7 @@
         <v>4363</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4618,7 +4621,7 @@
         <v>12982</v>
       </c>
       <c r="M6" s="15">
-        <v>12783</v>
+        <v>12737</v>
       </c>
       <c r="N6" s="15">
         <v>12309</v>
@@ -4741,7 +4744,7 @@
         <v>11478</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -4779,7 +4782,7 @@
         <v>20451</v>
       </c>
       <c r="M7" s="15">
-        <v>18919</v>
+        <v>19398</v>
       </c>
       <c r="N7" s="15">
         <v>18677</v>
@@ -4902,7 +4905,7 @@
         <v>16410</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -4940,7 +4943,7 @@
         <v>4689</v>
       </c>
       <c r="M8" s="15">
-        <v>4937</v>
+        <v>4932</v>
       </c>
       <c r="N8" s="15">
         <v>4142</v>
@@ -5063,7 +5066,7 @@
         <v>2807</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -5101,7 +5104,7 @@
         <v>9594</v>
       </c>
       <c r="M9" s="15">
-        <v>8691</v>
+        <v>8690</v>
       </c>
       <c r="N9" s="15">
         <v>8468</v>
@@ -5224,7 +5227,7 @@
         <v>8047</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -5262,7 +5265,7 @@
         <v>13576</v>
       </c>
       <c r="M10" s="15">
-        <v>13166</v>
+        <v>13055</v>
       </c>
       <c r="N10" s="15">
         <v>12381</v>
@@ -5385,7 +5388,7 @@
         <v>12133</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -5423,7 +5426,7 @@
         <v>42405</v>
       </c>
       <c r="M11" s="15">
-        <v>44392</v>
+        <v>44213</v>
       </c>
       <c r="N11" s="15">
         <v>42623</v>
@@ -5546,7 +5549,7 @@
         <v>29432</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -5584,7 +5587,7 @@
         <v>110083</v>
       </c>
       <c r="M12" s="7">
-        <v>109049</v>
+        <v>109164</v>
       </c>
       <c r="N12" s="7">
         <v>104706</v>
@@ -5707,7 +5710,7 @@
         <v>84670</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5762,12 +5765,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -5805,7 +5808,7 @@
         <v>492.48873800000001</v>
       </c>
       <c r="M15" s="15">
-        <v>450.87778700000001</v>
+        <v>449.94830400000001</v>
       </c>
       <c r="N15" s="15">
         <v>462.33480800000001</v>
@@ -5928,7 +5931,7 @@
         <v>303.44771800000001</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -5966,7 +5969,7 @@
         <v>883.17675499999996</v>
       </c>
       <c r="M16" s="15">
-        <v>883.60495400000002</v>
+        <v>882.49207699999999</v>
       </c>
       <c r="N16" s="15">
         <v>858.60462299999995</v>
@@ -6089,7 +6092,7 @@
         <v>868.11864300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -6127,7 +6130,7 @@
         <v>616.46194500000001</v>
       </c>
       <c r="M17" s="15">
-        <v>640.99145899999996</v>
+        <v>640.26952900000003</v>
       </c>
       <c r="N17" s="15">
         <v>627.66042200000004</v>
@@ -6250,7 +6253,7 @@
         <v>433.165955</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -6288,7 +6291,7 @@
         <v>63.479092999999999</v>
       </c>
       <c r="M18" s="15">
-        <v>67.511683000000005</v>
+        <v>67.464927000000003</v>
       </c>
       <c r="N18" s="15">
         <v>50.493682999999997</v>
@@ -6411,7 +6414,7 @@
         <v>42.773207999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -6449,7 +6452,7 @@
         <v>389.92883399999999</v>
       </c>
       <c r="M19" s="15">
-        <v>366.55915599999997</v>
+        <v>366.45326399999999</v>
       </c>
       <c r="N19" s="15">
         <v>376.586026</v>
@@ -6572,7 +6575,7 @@
         <v>374.79168900000002</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -6610,7 +6613,7 @@
         <v>1430.9431979999999</v>
       </c>
       <c r="M20" s="15">
-        <v>1315.179288</v>
+        <v>1300.1715079999999</v>
       </c>
       <c r="N20" s="15">
         <v>1154.96515</v>
@@ -6733,7 +6736,7 @@
         <v>1143.806075</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -6771,7 +6774,7 @@
         <v>983.77560200000005</v>
       </c>
       <c r="M21" s="15">
-        <v>1050.65993</v>
+        <v>1048.762563</v>
       </c>
       <c r="N21" s="15">
         <v>1032.0578250000001</v>
@@ -6894,7 +6897,7 @@
         <v>657.70498399999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -6932,7 +6935,7 @@
         <v>4860.2541649999994</v>
       </c>
       <c r="M22" s="7">
-        <v>4775.3842569999997</v>
+        <v>4755.5621719999999</v>
       </c>
       <c r="N22" s="7">
         <v>4562.7025370000001</v>
@@ -7055,40 +7058,40 @@
         <v>3823.8082720000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -7111,22 +7114,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="53" width="9.44140625" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.44140625" customWidth="1"/>
-    <col min="55" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="53" width="9.42578125" style="1" customWidth="1"/>
+    <col min="54" max="54" width="9.42578125" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -7183,7 +7186,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -7344,7 +7347,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -7506,13 +7509,13 @@
       </c>
       <c r="BB3" s="24"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -7550,7 +7553,7 @@
         <v>6180</v>
       </c>
       <c r="M5" s="15">
-        <v>0</v>
+        <v>6280</v>
       </c>
       <c r="N5" s="15">
         <v>0</v>
@@ -7674,7 +7677,7 @@
       </c>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -7712,7 +7715,7 @@
         <v>13187</v>
       </c>
       <c r="M6" s="6">
-        <v>0</v>
+        <v>12769</v>
       </c>
       <c r="N6" s="6">
         <v>0</v>
@@ -7836,7 +7839,7 @@
       </c>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -7874,7 +7877,7 @@
         <v>16428</v>
       </c>
       <c r="M7" s="6">
-        <v>0</v>
+        <v>15289</v>
       </c>
       <c r="N7" s="6">
         <v>0</v>
@@ -7998,7 +8001,7 @@
       </c>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -8036,7 +8039,7 @@
         <v>4664</v>
       </c>
       <c r="M8" s="6">
-        <v>0</v>
+        <v>4788</v>
       </c>
       <c r="N8" s="6">
         <v>0</v>
@@ -8160,7 +8163,7 @@
       </c>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -8198,7 +8201,7 @@
         <v>9481</v>
       </c>
       <c r="M9" s="6">
-        <v>0</v>
+        <v>9647</v>
       </c>
       <c r="N9" s="6">
         <v>0</v>
@@ -8322,7 +8325,7 @@
       </c>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -8360,7 +8363,7 @@
         <v>15079</v>
       </c>
       <c r="M10" s="15">
-        <v>0</v>
+        <v>15203</v>
       </c>
       <c r="N10" s="15">
         <v>0</v>
@@ -8484,7 +8487,7 @@
       </c>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -8522,7 +8525,7 @@
         <v>42692</v>
       </c>
       <c r="M11" s="6">
-        <v>0</v>
+        <v>45693</v>
       </c>
       <c r="N11" s="6">
         <v>0</v>
@@ -8646,7 +8649,7 @@
       </c>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -8684,7 +8687,7 @@
         <v>107711</v>
       </c>
       <c r="M12" s="7">
-        <v>0</v>
+        <v>109669</v>
       </c>
       <c r="N12" s="7">
         <v>0</v>
@@ -8808,7 +8811,7 @@
       </c>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -8864,13 +8867,13 @@
       <c r="BA13" s="6"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -8908,7 +8911,7 @@
         <v>461.86728299999999</v>
       </c>
       <c r="M15" s="15">
-        <v>0</v>
+        <v>477.602463</v>
       </c>
       <c r="N15" s="15">
         <v>0</v>
@@ -9032,7 +9035,7 @@
       </c>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -9070,7 +9073,7 @@
         <v>989.07336199999997</v>
       </c>
       <c r="M16" s="6">
-        <v>0</v>
+        <v>918.839741</v>
       </c>
       <c r="N16" s="6">
         <v>0</v>
@@ -9194,7 +9197,7 @@
       </c>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -9232,7 +9235,7 @@
         <v>581.18060400000002</v>
       </c>
       <c r="M17" s="6">
-        <v>0</v>
+        <v>454.86962899999997</v>
       </c>
       <c r="N17" s="6">
         <v>0</v>
@@ -9356,7 +9359,7 @@
       </c>
       <c r="BB17"/>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -9394,7 +9397,7 @@
         <v>77.609133</v>
       </c>
       <c r="M18" s="6">
-        <v>0</v>
+        <v>67.816277999999997</v>
       </c>
       <c r="N18" s="6">
         <v>0</v>
@@ -9518,7 +9521,7 @@
       </c>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9556,7 +9559,7 @@
         <v>441.30929500000002</v>
       </c>
       <c r="M19" s="6">
-        <v>0</v>
+        <v>435.214538</v>
       </c>
       <c r="N19" s="6">
         <v>0</v>
@@ -9680,7 +9683,7 @@
       </c>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -9718,7 +9721,7 @@
         <v>1532.9125839999999</v>
       </c>
       <c r="M20" s="15">
-        <v>0</v>
+        <v>1575.291183</v>
       </c>
       <c r="N20" s="15">
         <v>0</v>
@@ -9842,7 +9845,7 @@
       </c>
       <c r="BB20"/>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -9880,7 +9883,7 @@
         <v>1025.102989</v>
       </c>
       <c r="M21" s="6">
-        <v>0</v>
+        <v>1114.512667</v>
       </c>
       <c r="N21" s="6">
         <v>0</v>
@@ -10004,7 +10007,7 @@
       </c>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10042,7 +10045,7 @@
         <v>5109.0552499999994</v>
       </c>
       <c r="M22" s="7">
-        <v>0</v>
+        <v>5044.1464990000004</v>
       </c>
       <c r="N22" s="7">
         <v>0</v>
@@ -10166,100 +10169,100 @@
       </c>
       <c r="BB22"/>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="BB23"/>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB24"/>
     </row>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB25"/>
     </row>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB26"/>
     </row>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB27"/>
     </row>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB28"/>
     </row>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB29"/>
     </row>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB30"/>
     </row>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB31"/>
     </row>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB32"/>
     </row>
-    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB33"/>
     </row>
-    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB34"/>
     </row>
-    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB35"/>
     </row>
-    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB36"/>
     </row>
-    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB37"/>
     </row>
-    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB38"/>
     </row>
-    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB39"/>
     </row>
-    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB40"/>
     </row>
-    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB41"/>
     </row>
-    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB42"/>
     </row>
-    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB43"/>
     </row>
-    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB44"/>
     </row>
-    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB45"/>
     </row>
-    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB46"/>
     </row>
-    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB47"/>
     </row>
-    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB48"/>
     </row>
-    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB49"/>
     </row>
-    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB50"/>
     </row>
-    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB51"/>
     </row>
-    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB52"/>
     </row>
-    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB53"/>
     </row>
-    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB54"/>
     </row>
   </sheetData>
@@ -10289,19 +10292,19 @@
       <selection activeCell="B4" sqref="B4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="17" customWidth="1"/>
     <col min="53" max="53" width="9" style="17" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="17"/>
+    <col min="54" max="16384" width="6.7109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -10358,7 +10361,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -10519,7 +10522,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -10681,12 +10684,12 @@
       </c>
       <c r="BB3" s="23"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -10847,7 +10850,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -11008,7 +11011,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -11169,7 +11172,7 @@
         <v>15693</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -11330,7 +11333,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -11491,7 +11494,7 @@
         <v>6531</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11652,7 +11655,7 @@
         <v>10908</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -11813,7 +11816,7 @@
         <v>33194</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -11974,7 +11977,7 @@
         <v>88077</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -12029,12 +12032,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -12195,7 +12198,7 @@
         <v>448.48865799999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -12356,7 +12359,7 @@
         <v>863.31579299999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -12517,7 +12520,7 @@
         <v>424.08659699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -12678,7 +12681,7 @@
         <v>49.649962000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -12839,7 +12842,7 @@
         <v>235.51133100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -13000,7 +13003,7 @@
         <v>961.98002299999996</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -13161,7 +13164,7 @@
         <v>764.98213299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -13322,38 +13325,38 @@
         <v>3748.0144969999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -13376,22 +13379,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
@@ -13448,7 +13451,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -13609,7 +13612,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -13770,12 +13773,12 @@
         <v>43093</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -13936,7 +13939,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -14097,7 +14100,7 @@
         <v>9513</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -14258,7 +14261,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -14419,7 +14422,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -14580,7 +14583,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -14741,7 +14744,7 @@
         <v>9414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -14902,7 +14905,7 @@
         <v>36964</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -15063,7 +15066,7 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -15118,12 +15121,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -15284,7 +15287,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -15445,7 +15448,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -15606,7 +15609,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -15767,7 +15770,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -15928,7 +15931,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -16089,7 +16092,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -16250,7 +16253,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -16411,38 +16414,38 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -16464,19 +16467,19 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A22"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
     <col min="53" max="53" width="9" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -16533,7 +16536,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16694,7 +16697,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -16856,12 +16859,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -17022,7 +17025,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -17183,7 +17186,7 @@
         <v>12729</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -17344,7 +17347,7 @@
         <v>16661</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -17505,7 +17508,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -17666,7 +17669,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -17827,7 +17830,7 @@
         <v>12175</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -17988,7 +17991,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -18149,7 +18152,7 @@
         <v>97169</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -18204,12 +18207,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -18370,7 +18373,7 @@
         <v>345.26898999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -18531,7 +18534,7 @@
         <v>1137.3429249999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -18692,7 +18695,7 @@
         <v>337.41420499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -18853,7 +18856,7 @@
         <v>40.33334</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -19014,7 +19017,7 @@
         <v>339.10771799999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -19175,7 +19178,7 @@
         <v>1247.683331</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -19336,7 +19339,7 @@
         <v>821.21724600000005</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -19497,38 +19500,38 @@
         <v>4268.3677550000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -19542,19 +19545,19 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A22"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -19611,7 +19614,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -19772,7 +19775,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -19934,12 +19937,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -20100,7 +20103,7 @@
         <v>5356</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -20261,7 +20264,7 @@
         <v>12576</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -20422,7 +20425,7 @@
         <v>17944</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -20583,7 +20586,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -20744,7 +20747,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -20905,7 +20908,7 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -21066,7 +21069,7 @@
         <v>38154</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -21227,7 +21230,7 @@
         <v>92789</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -21282,12 +21285,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -21448,7 +21451,7 @@
         <v>356.60756500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -21609,7 +21612,7 @@
         <v>977.829027</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -21770,7 +21773,7 @@
         <v>495.993199</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -21931,7 +21934,7 @@
         <v>37.412531000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -22092,7 +22095,7 @@
         <v>351.68923999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -22253,7 +22256,7 @@
         <v>888.50449000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -22414,7 +22417,7 @@
         <v>804.61703199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -22575,38 +22578,38 @@
         <v>3912.6530840000005</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -22620,20 +22623,20 @@
   <dimension ref="A1:BB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
@@ -22690,7 +22693,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="23.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -22854,7 +22857,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -23016,7 +23019,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -23180,12 +23183,12 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -23349,7 +23352,7 @@
         <v>6187</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -23513,7 +23516,7 @@
         <v>11221</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -23677,7 +23680,7 @@
         <v>16946</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -23841,7 +23844,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
@@ -24005,7 +24008,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -24169,7 +24172,7 @@
         <v>13026</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -24333,7 +24336,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -24497,7 +24500,7 @@
         <v>99721</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -24553,12 +24556,12 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -24722,7 +24725,7 @@
         <v>469.697947</v>
       </c>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -24886,7 +24889,7 @@
         <v>800.96283800000003</v>
       </c>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -25050,7 +25053,7 @@
         <v>463.52606100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
@@ -25214,7 +25217,7 @@
         <v>39.121160000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -25378,7 +25381,7 @@
         <v>320.92344600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -25542,7 +25545,7 @@
         <v>1254.2732289999999</v>
       </c>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -25706,7 +25709,7 @@
         <v>905.27916400000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -25870,38 +25873,38 @@
         <v>4253.7838449999999</v>
       </c>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -25916,22 +25919,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
@@ -25988,7 +25991,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -26149,7 +26152,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -26311,12 +26314,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -26477,7 +26480,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -26638,7 +26641,7 @@
         <v>10430</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -26799,7 +26802,7 @@
         <v>15971</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -26960,7 +26963,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -27121,7 +27124,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -27282,7 +27285,7 @@
         <v>8618</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -27443,7 +27446,7 @@
         <v>34889</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -27604,7 +27607,7 @@
         <v>83267</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -27659,12 +27662,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -27825,7 +27828,7 @@
         <v>326.63437199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -27986,7 +27989,7 @@
         <v>710.31911300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -28147,7 +28150,7 @@
         <v>390.89581099999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -28308,7 +28311,7 @@
         <v>36.150655</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -28469,7 +28472,7 @@
         <v>232.43127799999999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -28630,7 +28633,7 @@
         <v>750.77748799999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -28791,7 +28794,7 @@
         <v>735.26635299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28952,40 +28955,40 @@
         <v>3182.4750699999995</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -29007,22 +29010,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -29079,7 +29082,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -29240,7 +29243,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -29402,12 +29405,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -29568,7 +29571,7 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -29729,7 +29732,7 @@
         <v>11045</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -29890,7 +29893,7 @@
         <v>14998</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -30051,7 +30054,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -30212,7 +30215,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -30373,7 +30376,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -30534,7 +30537,7 @@
         <v>31551</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -30695,7 +30698,7 @@
         <v>81088</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -30750,12 +30753,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -30916,7 +30919,7 @@
         <v>307.73157300000003</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -31077,7 +31080,7 @@
         <v>782.92677600000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -31238,7 +31241,7 @@
         <v>401.64126599999997</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -31399,7 +31402,7 @@
         <v>32.955354</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -31560,7 +31563,7 @@
         <v>272.11873100000003</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -31721,7 +31724,7 @@
         <v>976.60348099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -31882,7 +31885,7 @@
         <v>752.63757299999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -32043,40 +32046,40 @@
         <v>3526.6147539999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -32098,22 +32101,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -32170,7 +32173,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -32331,7 +32334,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -32493,12 +32496,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -32659,7 +32662,7 @@
         <v>4413</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -32820,7 +32823,7 @@
         <v>11673</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -32981,7 +32984,7 @@
         <v>15590</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -33142,7 +33145,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -33303,7 +33306,7 @@
         <v>8134</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -33464,7 +33467,7 @@
         <v>9863</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -33625,7 +33628,7 @@
         <v>34066</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -33786,7 +33789,7 @@
         <v>86245</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -33841,12 +33844,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -34007,7 +34010,7 @@
         <v>298.50642199999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -34168,7 +34171,7 @@
         <v>888.297684</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -34329,7 +34332,7 @@
         <v>533.92582100000004</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -34490,7 +34493,7 @@
         <v>38.857964000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -34651,7 +34654,7 @@
         <v>364.61675700000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -34812,7 +34815,7 @@
         <v>992.76339499999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -34973,7 +34976,7 @@
         <v>755.640308</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -35134,40 +35137,40 @@
         <v>3872.6083509999999</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Apr  1 05:29:15 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A2ECAB9-511F-40DB-8D40-9ABD2053E978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F91B5B2-84BC-463E-81E0-BA94F60191E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -965,7 +965,7 @@
       <selection activeCell="B4" sqref="B4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4010,9 +4010,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -4022,9 +4019,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -4463,7 +4460,7 @@
         <v>6139</v>
       </c>
       <c r="N5" s="15">
-        <v>6106</v>
+        <v>6099</v>
       </c>
       <c r="O5" s="15">
         <v>6082</v>
@@ -4624,7 +4621,7 @@
         <v>12737</v>
       </c>
       <c r="N6" s="15">
-        <v>12309</v>
+        <v>12274</v>
       </c>
       <c r="O6" s="15">
         <v>12447</v>
@@ -4785,7 +4782,7 @@
         <v>19398</v>
       </c>
       <c r="N7" s="15">
-        <v>18677</v>
+        <v>18903</v>
       </c>
       <c r="O7" s="15">
         <v>18893</v>
@@ -4946,7 +4943,7 @@
         <v>4932</v>
       </c>
       <c r="N8" s="15">
-        <v>4142</v>
+        <v>4116</v>
       </c>
       <c r="O8" s="15">
         <v>4557</v>
@@ -5107,7 +5104,7 @@
         <v>8690</v>
       </c>
       <c r="N9" s="15">
-        <v>8468</v>
+        <v>8466</v>
       </c>
       <c r="O9" s="15">
         <v>9036</v>
@@ -5268,7 +5265,7 @@
         <v>13055</v>
       </c>
       <c r="N10" s="15">
-        <v>12381</v>
+        <v>12426</v>
       </c>
       <c r="O10" s="15">
         <v>15342</v>
@@ -5429,7 +5426,7 @@
         <v>44213</v>
       </c>
       <c r="N11" s="15">
-        <v>42623</v>
+        <v>42528</v>
       </c>
       <c r="O11" s="15">
         <v>44683</v>
@@ -5590,7 +5587,7 @@
         <v>109164</v>
       </c>
       <c r="N12" s="7">
-        <v>104706</v>
+        <v>104812</v>
       </c>
       <c r="O12" s="7">
         <v>111040</v>
@@ -5811,7 +5808,7 @@
         <v>449.94830400000001</v>
       </c>
       <c r="N15" s="15">
-        <v>462.33480800000001</v>
+        <v>462.57709399999999</v>
       </c>
       <c r="O15" s="15">
         <v>449.88557500000002</v>
@@ -5972,7 +5969,7 @@
         <v>882.49207699999999</v>
       </c>
       <c r="N16" s="15">
-        <v>858.60462299999995</v>
+        <v>858.11595699999998</v>
       </c>
       <c r="O16" s="15">
         <v>925.42625199999998</v>
@@ -6133,7 +6130,7 @@
         <v>640.26952900000003</v>
       </c>
       <c r="N17" s="15">
-        <v>627.66042200000004</v>
+        <v>627.79621999999995</v>
       </c>
       <c r="O17" s="15">
         <v>507.87456900000001</v>
@@ -6294,7 +6291,7 @@
         <v>67.464927000000003</v>
       </c>
       <c r="N18" s="15">
-        <v>50.493682999999997</v>
+        <v>50.033371000000002</v>
       </c>
       <c r="O18" s="15">
         <v>66.240499</v>
@@ -6455,7 +6452,7 @@
         <v>366.45326399999999</v>
       </c>
       <c r="N19" s="15">
-        <v>376.586026</v>
+        <v>376.44401800000003</v>
       </c>
       <c r="O19" s="15">
         <v>419.41336200000001</v>
@@ -6616,7 +6613,7 @@
         <v>1300.1715079999999</v>
       </c>
       <c r="N20" s="15">
-        <v>1154.96515</v>
+        <v>1161.207527</v>
       </c>
       <c r="O20" s="15">
         <v>1510.259963</v>
@@ -6777,7 +6774,7 @@
         <v>1048.762563</v>
       </c>
       <c r="N21" s="15">
-        <v>1032.0578250000001</v>
+        <v>1031.326088</v>
       </c>
       <c r="O21" s="15">
         <v>1064.179216</v>
@@ -6938,7 +6935,7 @@
         <v>4755.5621719999999</v>
       </c>
       <c r="N22" s="7">
-        <v>4562.7025370000001</v>
+        <v>4567.5002750000003</v>
       </c>
       <c r="O22" s="7">
         <v>4943.2794359999998</v>
@@ -7104,6 +7101,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -7556,7 +7556,7 @@
         <v>6280</v>
       </c>
       <c r="N5" s="15">
-        <v>0</v>
+        <v>5803</v>
       </c>
       <c r="O5" s="15">
         <v>0</v>
@@ -7718,7 +7718,7 @@
         <v>12769</v>
       </c>
       <c r="N6" s="6">
-        <v>0</v>
+        <v>12914</v>
       </c>
       <c r="O6" s="6">
         <v>0</v>
@@ -7880,7 +7880,7 @@
         <v>15289</v>
       </c>
       <c r="N7" s="6">
-        <v>0</v>
+        <v>18277</v>
       </c>
       <c r="O7" s="6">
         <v>0</v>
@@ -8042,7 +8042,7 @@
         <v>4788</v>
       </c>
       <c r="N8" s="6">
-        <v>0</v>
+        <v>5469</v>
       </c>
       <c r="O8" s="6">
         <v>0</v>
@@ -8204,7 +8204,7 @@
         <v>9647</v>
       </c>
       <c r="N9" s="6">
-        <v>0</v>
+        <v>9989</v>
       </c>
       <c r="O9" s="6">
         <v>0</v>
@@ -8366,7 +8366,7 @@
         <v>15203</v>
       </c>
       <c r="N10" s="15">
-        <v>0</v>
+        <v>14185</v>
       </c>
       <c r="O10" s="15">
         <v>0</v>
@@ -8528,7 +8528,7 @@
         <v>45693</v>
       </c>
       <c r="N11" s="6">
-        <v>0</v>
+        <v>45520</v>
       </c>
       <c r="O11" s="6">
         <v>0</v>
@@ -8690,7 +8690,7 @@
         <v>109669</v>
       </c>
       <c r="N12" s="7">
-        <v>0</v>
+        <v>112157</v>
       </c>
       <c r="O12" s="7">
         <v>0</v>
@@ -8914,7 +8914,7 @@
         <v>477.602463</v>
       </c>
       <c r="N15" s="15">
-        <v>0</v>
+        <v>428.95517699999999</v>
       </c>
       <c r="O15" s="15">
         <v>0</v>
@@ -9076,7 +9076,7 @@
         <v>918.839741</v>
       </c>
       <c r="N16" s="6">
-        <v>0</v>
+        <v>943.04638899999998</v>
       </c>
       <c r="O16" s="6">
         <v>0</v>
@@ -9238,7 +9238,7 @@
         <v>454.86962899999997</v>
       </c>
       <c r="N17" s="6">
-        <v>0</v>
+        <v>519.26245400000005</v>
       </c>
       <c r="O17" s="6">
         <v>0</v>
@@ -9400,7 +9400,7 @@
         <v>67.816277999999997</v>
       </c>
       <c r="N18" s="6">
-        <v>0</v>
+        <v>82.009820000000005</v>
       </c>
       <c r="O18" s="6">
         <v>0</v>
@@ -9562,7 +9562,7 @@
         <v>435.214538</v>
       </c>
       <c r="N19" s="6">
-        <v>0</v>
+        <v>452.00419900000003</v>
       </c>
       <c r="O19" s="6">
         <v>0</v>
@@ -9724,7 +9724,7 @@
         <v>1575.291183</v>
       </c>
       <c r="N20" s="15">
-        <v>0</v>
+        <v>1284.684526</v>
       </c>
       <c r="O20" s="15">
         <v>0</v>
@@ -9886,7 +9886,7 @@
         <v>1114.512667</v>
       </c>
       <c r="N21" s="6">
-        <v>0</v>
+        <v>1088.7126270000001</v>
       </c>
       <c r="O21" s="6">
         <v>0</v>
@@ -10048,7 +10048,7 @@
         <v>5044.1464990000004</v>
       </c>
       <c r="N22" s="7">
-        <v>0</v>
+        <v>4798.6751920000006</v>
       </c>
       <c r="O22" s="7">
         <v>0</v>
@@ -10292,7 +10292,7 @@
       <selection activeCell="B4" sqref="B4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13379,10 +13379,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16467,7 +16467,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19545,7 +19545,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22623,7 +22623,7 @@
   <dimension ref="A1:BB55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25919,10 +25919,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29010,10 +29010,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -32101,10 +32101,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Apr  8 05:29:31 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F91B5B2-84BC-463E-81E0-BA94F60191E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5DF08C-AF32-44C9-88DE-7257CAB31625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -4018,11 +4018,11 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AF4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="AP9" sqref="AP9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4463,7 +4463,7 @@
         <v>6099</v>
       </c>
       <c r="O5" s="15">
-        <v>6082</v>
+        <v>6066</v>
       </c>
       <c r="P5" s="15">
         <v>6355</v>
@@ -4624,7 +4624,7 @@
         <v>12274</v>
       </c>
       <c r="O6" s="15">
-        <v>12447</v>
+        <v>12387</v>
       </c>
       <c r="P6" s="15">
         <v>12708</v>
@@ -4785,7 +4785,7 @@
         <v>18903</v>
       </c>
       <c r="O7" s="15">
-        <v>18893</v>
+        <v>19307</v>
       </c>
       <c r="P7" s="15">
         <v>18576</v>
@@ -4946,7 +4946,7 @@
         <v>4116</v>
       </c>
       <c r="O8" s="15">
-        <v>4557</v>
+        <v>4528</v>
       </c>
       <c r="P8" s="15">
         <v>4443</v>
@@ -5107,7 +5107,7 @@
         <v>8466</v>
       </c>
       <c r="O9" s="15">
-        <v>9036</v>
+        <v>9038</v>
       </c>
       <c r="P9" s="15">
         <v>9029</v>
@@ -5268,7 +5268,7 @@
         <v>12426</v>
       </c>
       <c r="O10" s="15">
-        <v>15342</v>
+        <v>15408</v>
       </c>
       <c r="P10" s="15">
         <v>12157</v>
@@ -5429,7 +5429,7 @@
         <v>42528</v>
       </c>
       <c r="O11" s="15">
-        <v>44683</v>
+        <v>44557</v>
       </c>
       <c r="P11" s="15">
         <v>45262</v>
@@ -5590,7 +5590,7 @@
         <v>104812</v>
       </c>
       <c r="O12" s="7">
-        <v>111040</v>
+        <v>111291</v>
       </c>
       <c r="P12" s="7">
         <v>108530</v>
@@ -5811,7 +5811,7 @@
         <v>462.57709399999999</v>
       </c>
       <c r="O15" s="15">
-        <v>449.88557500000002</v>
+        <v>448.92158699999999</v>
       </c>
       <c r="P15" s="15">
         <v>481.79653500000001</v>
@@ -5972,7 +5972,7 @@
         <v>858.11595699999998</v>
       </c>
       <c r="O16" s="15">
-        <v>925.42625199999998</v>
+        <v>924.264591</v>
       </c>
       <c r="P16" s="15">
         <v>916.365587</v>
@@ -6133,7 +6133,7 @@
         <v>627.79621999999995</v>
       </c>
       <c r="O17" s="15">
-        <v>507.87456900000001</v>
+        <v>507.66684500000002</v>
       </c>
       <c r="P17" s="15">
         <v>630.45217300000002</v>
@@ -6294,7 +6294,7 @@
         <v>50.033371000000002</v>
       </c>
       <c r="O18" s="15">
-        <v>66.240499</v>
+        <v>65.542045000000002</v>
       </c>
       <c r="P18" s="15">
         <v>67.073419000000001</v>
@@ -6455,7 +6455,7 @@
         <v>376.44401800000003</v>
       </c>
       <c r="O19" s="15">
-        <v>419.41336200000001</v>
+        <v>419.35392100000001</v>
       </c>
       <c r="P19" s="15">
         <v>425.74363299999999</v>
@@ -6616,7 +6616,7 @@
         <v>1161.207527</v>
       </c>
       <c r="O20" s="15">
-        <v>1510.259963</v>
+        <v>1520.259589</v>
       </c>
       <c r="P20" s="15">
         <v>1088.0119890000001</v>
@@ -6777,7 +6777,7 @@
         <v>1031.326088</v>
       </c>
       <c r="O21" s="15">
-        <v>1064.179216</v>
+        <v>1061.772528</v>
       </c>
       <c r="P21" s="15">
         <v>1116.276061</v>
@@ -6938,7 +6938,7 @@
         <v>4567.5002750000003</v>
       </c>
       <c r="O22" s="7">
-        <v>4943.2794359999998</v>
+        <v>4947.7811060000004</v>
       </c>
       <c r="P22" s="7">
         <v>4725.7193969999998</v>
@@ -7114,10 +7114,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7559,7 +7559,7 @@
         <v>5803</v>
       </c>
       <c r="O5" s="15">
-        <v>0</v>
+        <v>5228</v>
       </c>
       <c r="P5" s="15">
         <v>0</v>
@@ -7721,7 +7721,7 @@
         <v>12914</v>
       </c>
       <c r="O6" s="6">
-        <v>0</v>
+        <v>11772</v>
       </c>
       <c r="P6" s="6">
         <v>0</v>
@@ -7883,7 +7883,7 @@
         <v>18277</v>
       </c>
       <c r="O7" s="6">
-        <v>0</v>
+        <v>17531</v>
       </c>
       <c r="P7" s="6">
         <v>0</v>
@@ -8045,7 +8045,7 @@
         <v>5469</v>
       </c>
       <c r="O8" s="6">
-        <v>0</v>
+        <v>4338</v>
       </c>
       <c r="P8" s="6">
         <v>0</v>
@@ -8207,7 +8207,7 @@
         <v>9989</v>
       </c>
       <c r="O9" s="6">
-        <v>0</v>
+        <v>9119</v>
       </c>
       <c r="P9" s="6">
         <v>0</v>
@@ -8369,7 +8369,7 @@
         <v>14185</v>
       </c>
       <c r="O10" s="15">
-        <v>0</v>
+        <v>16611</v>
       </c>
       <c r="P10" s="15">
         <v>0</v>
@@ -8531,7 +8531,7 @@
         <v>45520</v>
       </c>
       <c r="O11" s="6">
-        <v>0</v>
+        <v>40693</v>
       </c>
       <c r="P11" s="6">
         <v>0</v>
@@ -8693,7 +8693,7 @@
         <v>112157</v>
       </c>
       <c r="O12" s="7">
-        <v>0</v>
+        <v>105292</v>
       </c>
       <c r="P12" s="7">
         <v>0</v>
@@ -8917,7 +8917,7 @@
         <v>428.95517699999999</v>
       </c>
       <c r="O15" s="15">
-        <v>0</v>
+        <v>367.061443</v>
       </c>
       <c r="P15" s="15">
         <v>0</v>
@@ -9079,7 +9079,7 @@
         <v>943.04638899999998</v>
       </c>
       <c r="O16" s="6">
-        <v>0</v>
+        <v>817.88185399999998</v>
       </c>
       <c r="P16" s="6">
         <v>0</v>
@@ -9241,7 +9241,7 @@
         <v>519.26245400000005</v>
       </c>
       <c r="O17" s="6">
-        <v>0</v>
+        <v>534.92430400000001</v>
       </c>
       <c r="P17" s="6">
         <v>0</v>
@@ -9403,7 +9403,7 @@
         <v>82.009820000000005</v>
       </c>
       <c r="O18" s="6">
-        <v>0</v>
+        <v>62.312376</v>
       </c>
       <c r="P18" s="6">
         <v>0</v>
@@ -9565,7 +9565,7 @@
         <v>452.00419900000003</v>
       </c>
       <c r="O19" s="6">
-        <v>0</v>
+        <v>401.76117199999999</v>
       </c>
       <c r="P19" s="6">
         <v>0</v>
@@ -9727,7 +9727,7 @@
         <v>1284.684526</v>
       </c>
       <c r="O20" s="15">
-        <v>0</v>
+        <v>1595.719605</v>
       </c>
       <c r="P20" s="15">
         <v>0</v>
@@ -9889,7 +9889,7 @@
         <v>1088.7126270000001</v>
       </c>
       <c r="O21" s="6">
-        <v>0</v>
+        <v>1030.8898830000001</v>
       </c>
       <c r="P21" s="6">
         <v>0</v>
@@ -10051,7 +10051,7 @@
         <v>4798.6751920000006</v>
       </c>
       <c r="O22" s="7">
-        <v>0</v>
+        <v>4810.5506370000003</v>
       </c>
       <c r="P22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Apr 15 05:29:19 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5DF08C-AF32-44C9-88DE-7257CAB31625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D6F95D-7348-40C6-B2CD-D985EBC5821C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -4019,10 +4019,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="AF4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="AP9" sqref="AP9"/>
+      <selection activeCell="E16" sqref="E16"/>
+      <selection pane="topRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4466,7 +4466,7 @@
         <v>6066</v>
       </c>
       <c r="P5" s="15">
-        <v>6355</v>
+        <v>6331</v>
       </c>
       <c r="Q5" s="15">
         <v>6331</v>
@@ -4627,7 +4627,7 @@
         <v>12387</v>
       </c>
       <c r="P6" s="15">
-        <v>12708</v>
+        <v>12653</v>
       </c>
       <c r="Q6" s="15">
         <v>12636</v>
@@ -4788,7 +4788,7 @@
         <v>19307</v>
       </c>
       <c r="P7" s="15">
-        <v>18576</v>
+        <v>18974</v>
       </c>
       <c r="Q7" s="15">
         <v>20123</v>
@@ -4949,7 +4949,7 @@
         <v>4528</v>
       </c>
       <c r="P8" s="15">
-        <v>4443</v>
+        <v>4439</v>
       </c>
       <c r="Q8" s="15">
         <v>4388</v>
@@ -5110,7 +5110,7 @@
         <v>9038</v>
       </c>
       <c r="P9" s="15">
-        <v>9029</v>
+        <v>8922</v>
       </c>
       <c r="Q9" s="15">
         <v>8151</v>
@@ -5271,7 +5271,7 @@
         <v>15408</v>
       </c>
       <c r="P10" s="15">
-        <v>12157</v>
+        <v>12147</v>
       </c>
       <c r="Q10" s="15">
         <v>13591</v>
@@ -5432,7 +5432,7 @@
         <v>44557</v>
       </c>
       <c r="P11" s="15">
-        <v>45262</v>
+        <v>45175</v>
       </c>
       <c r="Q11" s="15">
         <v>46453</v>
@@ -5593,7 +5593,7 @@
         <v>111291</v>
       </c>
       <c r="P12" s="7">
-        <v>108530</v>
+        <v>108641</v>
       </c>
       <c r="Q12" s="7">
         <v>111673</v>
@@ -5814,7 +5814,7 @@
         <v>448.92158699999999</v>
       </c>
       <c r="P15" s="15">
-        <v>481.79653500000001</v>
+        <v>479.855726</v>
       </c>
       <c r="Q15" s="15">
         <v>470.19374299999998</v>
@@ -5975,7 +5975,7 @@
         <v>924.264591</v>
       </c>
       <c r="P16" s="15">
-        <v>916.365587</v>
+        <v>915.01673600000004</v>
       </c>
       <c r="Q16" s="15">
         <v>911.31394899999998</v>
@@ -6136,7 +6136,7 @@
         <v>507.66684500000002</v>
       </c>
       <c r="P17" s="15">
-        <v>630.45217300000002</v>
+        <v>622.653143</v>
       </c>
       <c r="Q17" s="15">
         <v>581.45679600000005</v>
@@ -6297,7 +6297,7 @@
         <v>65.542045000000002</v>
       </c>
       <c r="P18" s="15">
-        <v>67.073419000000001</v>
+        <v>66.999771999999993</v>
       </c>
       <c r="Q18" s="15">
         <v>62.793635000000002</v>
@@ -6458,7 +6458,7 @@
         <v>419.35392100000001</v>
       </c>
       <c r="P19" s="15">
-        <v>425.74363299999999</v>
+        <v>425.82050800000002</v>
       </c>
       <c r="Q19" s="15">
         <v>416.92520500000001</v>
@@ -6619,7 +6619,7 @@
         <v>1520.259589</v>
       </c>
       <c r="P20" s="15">
-        <v>1088.0119890000001</v>
+        <v>1087.7460940000001</v>
       </c>
       <c r="Q20" s="15">
         <v>1263.4938099999999</v>
@@ -6780,7 +6780,7 @@
         <v>1061.772528</v>
       </c>
       <c r="P21" s="15">
-        <v>1116.276061</v>
+        <v>1116.5547759999999</v>
       </c>
       <c r="Q21" s="15">
         <v>1137.813885</v>
@@ -6941,7 +6941,7 @@
         <v>4947.7811060000004</v>
       </c>
       <c r="P22" s="7">
-        <v>4725.7193969999998</v>
+        <v>4714.6467549999998</v>
       </c>
       <c r="Q22" s="7">
         <v>4843.9910230000005</v>
@@ -7114,10 +7114,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
+      <selection activeCell="AH31" sqref="A1:XFD1048576"/>
+      <selection pane="topRight" activeCell="AH31" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="AH31" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7562,7 +7562,7 @@
         <v>5228</v>
       </c>
       <c r="P5" s="15">
-        <v>0</v>
+        <v>5885</v>
       </c>
       <c r="Q5" s="15">
         <v>0</v>
@@ -7724,7 +7724,7 @@
         <v>11772</v>
       </c>
       <c r="P6" s="6">
-        <v>0</v>
+        <v>12265</v>
       </c>
       <c r="Q6" s="6">
         <v>0</v>
@@ -7886,7 +7886,7 @@
         <v>17531</v>
       </c>
       <c r="P7" s="6">
-        <v>0</v>
+        <v>17214</v>
       </c>
       <c r="Q7" s="6">
         <v>0</v>
@@ -8048,7 +8048,7 @@
         <v>4338</v>
       </c>
       <c r="P8" s="6">
-        <v>0</v>
+        <v>4116</v>
       </c>
       <c r="Q8" s="6">
         <v>0</v>
@@ -8210,7 +8210,7 @@
         <v>9119</v>
       </c>
       <c r="P9" s="6">
-        <v>0</v>
+        <v>9297</v>
       </c>
       <c r="Q9" s="6">
         <v>0</v>
@@ -8372,7 +8372,7 @@
         <v>16611</v>
       </c>
       <c r="P10" s="15">
-        <v>0</v>
+        <v>13536</v>
       </c>
       <c r="Q10" s="15">
         <v>0</v>
@@ -8534,7 +8534,7 @@
         <v>40693</v>
       </c>
       <c r="P11" s="6">
-        <v>0</v>
+        <v>45417</v>
       </c>
       <c r="Q11" s="6">
         <v>0</v>
@@ -8696,7 +8696,7 @@
         <v>105292</v>
       </c>
       <c r="P12" s="7">
-        <v>0</v>
+        <v>107730</v>
       </c>
       <c r="Q12" s="7">
         <v>0</v>
@@ -8920,7 +8920,7 @@
         <v>367.061443</v>
       </c>
       <c r="P15" s="15">
-        <v>0</v>
+        <v>420.85454399999998</v>
       </c>
       <c r="Q15" s="15">
         <v>0</v>
@@ -9082,7 +9082,7 @@
         <v>817.88185399999998</v>
       </c>
       <c r="P16" s="6">
-        <v>0</v>
+        <v>870.28412700000001</v>
       </c>
       <c r="Q16" s="6">
         <v>0</v>
@@ -9244,7 +9244,7 @@
         <v>534.92430400000001</v>
       </c>
       <c r="P17" s="6">
-        <v>0</v>
+        <v>488.95255700000001</v>
       </c>
       <c r="Q17" s="6">
         <v>0</v>
@@ -9406,7 +9406,7 @@
         <v>62.312376</v>
       </c>
       <c r="P18" s="6">
-        <v>0</v>
+        <v>57.738802999999997</v>
       </c>
       <c r="Q18" s="6">
         <v>0</v>
@@ -9568,7 +9568,7 @@
         <v>401.76117199999999</v>
       </c>
       <c r="P19" s="6">
-        <v>0</v>
+        <v>422.169353</v>
       </c>
       <c r="Q19" s="6">
         <v>0</v>
@@ -9730,7 +9730,7 @@
         <v>1595.719605</v>
       </c>
       <c r="P20" s="15">
-        <v>0</v>
+        <v>1271.8982140000001</v>
       </c>
       <c r="Q20" s="15">
         <v>0</v>
@@ -9892,7 +9892,7 @@
         <v>1030.8898830000001</v>
       </c>
       <c r="P21" s="6">
-        <v>0</v>
+        <v>1046.101287</v>
       </c>
       <c r="Q21" s="6">
         <v>0</v>
@@ -10054,7 +10054,7 @@
         <v>4810.5506370000003</v>
       </c>
       <c r="P22" s="7">
-        <v>0</v>
+        <v>4577.9988849999991</v>
       </c>
       <c r="Q22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Apr 22 05:29:43 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D6F95D-7348-40C6-B2CD-D985EBC5821C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9877F3A5-3D9B-455D-859D-44570ACA0AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -961,11 +961,11 @@
   <dimension ref="A1:BA23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B4" sqref="B4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection pane="bottomRight" activeCell="O12" sqref="O12:X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4019,10 +4019,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="AF4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="E16" sqref="E16"/>
-      <selection pane="topRight" activeCell="E16" sqref="E16"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection activeCell="E22" sqref="A1:XFD1048576"/>
+      <selection pane="topRight" activeCell="E22" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4469,7 +4469,7 @@
         <v>6331</v>
       </c>
       <c r="Q5" s="15">
-        <v>6331</v>
+        <v>6293</v>
       </c>
       <c r="R5" s="15">
         <v>5958</v>
@@ -4630,7 +4630,7 @@
         <v>12653</v>
       </c>
       <c r="Q6" s="15">
-        <v>12636</v>
+        <v>12575</v>
       </c>
       <c r="R6" s="15">
         <v>12738</v>
@@ -4791,7 +4791,7 @@
         <v>18974</v>
       </c>
       <c r="Q7" s="15">
-        <v>20123</v>
+        <v>20602</v>
       </c>
       <c r="R7" s="15">
         <v>17916</v>
@@ -4952,7 +4952,7 @@
         <v>4439</v>
       </c>
       <c r="Q8" s="15">
-        <v>4388</v>
+        <v>4386</v>
       </c>
       <c r="R8" s="15">
         <v>4398</v>
@@ -5113,7 +5113,7 @@
         <v>8922</v>
       </c>
       <c r="Q9" s="15">
-        <v>8151</v>
+        <v>8157</v>
       </c>
       <c r="R9" s="15">
         <v>8985</v>
@@ -5274,7 +5274,7 @@
         <v>12147</v>
       </c>
       <c r="Q10" s="15">
-        <v>13591</v>
+        <v>13618</v>
       </c>
       <c r="R10" s="15">
         <v>13598</v>
@@ -5435,7 +5435,7 @@
         <v>45175</v>
       </c>
       <c r="Q11" s="15">
-        <v>46453</v>
+        <v>46379</v>
       </c>
       <c r="R11" s="15">
         <v>48028</v>
@@ -5596,7 +5596,7 @@
         <v>108641</v>
       </c>
       <c r="Q12" s="7">
-        <v>111673</v>
+        <v>112010</v>
       </c>
       <c r="R12" s="7">
         <v>111621</v>
@@ -5817,7 +5817,7 @@
         <v>479.855726</v>
       </c>
       <c r="Q15" s="15">
-        <v>470.19374299999998</v>
+        <v>466.76651600000002</v>
       </c>
       <c r="R15" s="15">
         <v>434.28164199999998</v>
@@ -5978,7 +5978,7 @@
         <v>915.01673600000004</v>
       </c>
       <c r="Q16" s="15">
-        <v>911.31394899999998</v>
+        <v>909.53954399999998</v>
       </c>
       <c r="R16" s="15">
         <v>960.82308999999998</v>
@@ -6139,7 +6139,7 @@
         <v>622.653143</v>
       </c>
       <c r="Q17" s="15">
-        <v>581.45679600000005</v>
+        <v>582.22220200000004</v>
       </c>
       <c r="R17" s="15">
         <v>580.56163300000003</v>
@@ -6300,7 +6300,7 @@
         <v>66.999771999999993</v>
       </c>
       <c r="Q18" s="15">
-        <v>62.793635000000002</v>
+        <v>62.842471000000003</v>
       </c>
       <c r="R18" s="15">
         <v>60.100155999999998</v>
@@ -6461,7 +6461,7 @@
         <v>425.82050800000002</v>
       </c>
       <c r="Q19" s="15">
-        <v>416.92520500000001</v>
+        <v>416.86198000000002</v>
       </c>
       <c r="R19" s="15">
         <v>416.42678799999999</v>
@@ -6622,7 +6622,7 @@
         <v>1087.7460940000001</v>
       </c>
       <c r="Q20" s="15">
-        <v>1263.4938099999999</v>
+        <v>1266.0550499999999</v>
       </c>
       <c r="R20" s="15">
         <v>1243.4376119999999</v>
@@ -6783,7 +6783,7 @@
         <v>1116.5547759999999</v>
       </c>
       <c r="Q21" s="15">
-        <v>1137.813885</v>
+        <v>1137.121359</v>
       </c>
       <c r="R21" s="15">
         <v>1177.19389</v>
@@ -6944,7 +6944,7 @@
         <v>4714.6467549999998</v>
       </c>
       <c r="Q22" s="7">
-        <v>4843.9910230000005</v>
+        <v>4841.409122</v>
       </c>
       <c r="R22" s="7">
         <v>4872.8248110000004</v>
@@ -7114,10 +7114,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="AH31" sqref="A1:XFD1048576"/>
-      <selection pane="topRight" activeCell="AH31" sqref="A1:XFD1048576"/>
-      <selection pane="bottomLeft" activeCell="AH31" sqref="A1:XFD1048576"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection activeCell="E22" sqref="A1:XFD1048576"/>
+      <selection pane="topRight" activeCell="E22" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7565,7 +7565,7 @@
         <v>5885</v>
       </c>
       <c r="Q5" s="15">
-        <v>0</v>
+        <v>5871</v>
       </c>
       <c r="R5" s="15">
         <v>0</v>
@@ -7727,7 +7727,7 @@
         <v>12265</v>
       </c>
       <c r="Q6" s="6">
-        <v>0</v>
+        <v>11850</v>
       </c>
       <c r="R6" s="6">
         <v>0</v>
@@ -7889,7 +7889,7 @@
         <v>17214</v>
       </c>
       <c r="Q7" s="6">
-        <v>0</v>
+        <v>16394</v>
       </c>
       <c r="R7" s="6">
         <v>0</v>
@@ -8051,7 +8051,7 @@
         <v>4116</v>
       </c>
       <c r="Q8" s="6">
-        <v>0</v>
+        <v>4688</v>
       </c>
       <c r="R8" s="6">
         <v>0</v>
@@ -8213,7 +8213,7 @@
         <v>9297</v>
       </c>
       <c r="Q9" s="6">
-        <v>0</v>
+        <v>9794</v>
       </c>
       <c r="R9" s="6">
         <v>0</v>
@@ -8375,7 +8375,7 @@
         <v>13536</v>
       </c>
       <c r="Q10" s="15">
-        <v>0</v>
+        <v>14085</v>
       </c>
       <c r="R10" s="15">
         <v>0</v>
@@ -8537,7 +8537,7 @@
         <v>45417</v>
       </c>
       <c r="Q11" s="6">
-        <v>0</v>
+        <v>43999</v>
       </c>
       <c r="R11" s="6">
         <v>0</v>
@@ -8699,7 +8699,7 @@
         <v>107730</v>
       </c>
       <c r="Q12" s="7">
-        <v>0</v>
+        <v>106681</v>
       </c>
       <c r="R12" s="7">
         <v>0</v>
@@ -8923,7 +8923,7 @@
         <v>420.85454399999998</v>
       </c>
       <c r="Q15" s="15">
-        <v>0</v>
+        <v>416.032217</v>
       </c>
       <c r="R15" s="15">
         <v>0</v>
@@ -9085,7 +9085,7 @@
         <v>870.28412700000001</v>
       </c>
       <c r="Q16" s="6">
-        <v>0</v>
+        <v>847.46041200000002</v>
       </c>
       <c r="R16" s="6">
         <v>0</v>
@@ -9247,7 +9247,7 @@
         <v>488.95255700000001</v>
       </c>
       <c r="Q17" s="6">
-        <v>0</v>
+        <v>486.53375299999999</v>
       </c>
       <c r="R17" s="6">
         <v>0</v>
@@ -9409,7 +9409,7 @@
         <v>57.738802999999997</v>
       </c>
       <c r="Q18" s="6">
-        <v>0</v>
+        <v>75.546479000000005</v>
       </c>
       <c r="R18" s="6">
         <v>0</v>
@@ -9571,7 +9571,7 @@
         <v>422.169353</v>
       </c>
       <c r="Q19" s="6">
-        <v>0</v>
+        <v>453.855433</v>
       </c>
       <c r="R19" s="6">
         <v>0</v>
@@ -9733,7 +9733,7 @@
         <v>1271.8982140000001</v>
       </c>
       <c r="Q20" s="15">
-        <v>0</v>
+        <v>1338.1306589999999</v>
       </c>
       <c r="R20" s="15">
         <v>0</v>
@@ -9895,7 +9895,7 @@
         <v>1046.101287</v>
       </c>
       <c r="Q21" s="6">
-        <v>0</v>
+        <v>981.18432499999994</v>
       </c>
       <c r="R21" s="6">
         <v>0</v>
@@ -10057,7 +10057,7 @@
         <v>4577.9988849999991</v>
       </c>
       <c r="Q22" s="7">
-        <v>0</v>
+        <v>4598.7432779999999</v>
       </c>
       <c r="R22" s="7">
         <v>0</v>
@@ -10292,7 +10292,7 @@
       <selection activeCell="B4" sqref="B4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
+      <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Apr 29 05:29:42 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9877F3A5-3D9B-455D-859D-44570ACA0AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37C24C59-817E-4270-8086-19EC871F15FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4019,10 +4019,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="AF4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="E22" sqref="A1:XFD1048576"/>
-      <selection pane="topRight" activeCell="E22" sqref="A1:XFD1048576"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="A1:XFD1048576"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="A1:XFD1048576"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="AJ25" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4472,7 +4472,7 @@
         <v>6293</v>
       </c>
       <c r="R5" s="15">
-        <v>5958</v>
+        <v>5924</v>
       </c>
       <c r="S5" s="15">
         <v>5983</v>
@@ -4633,7 +4633,7 @@
         <v>12575</v>
       </c>
       <c r="R6" s="15">
-        <v>12738</v>
+        <v>12661</v>
       </c>
       <c r="S6" s="15">
         <v>12348</v>
@@ -4794,7 +4794,7 @@
         <v>20602</v>
       </c>
       <c r="R7" s="15">
-        <v>17916</v>
+        <v>18272</v>
       </c>
       <c r="S7" s="15">
         <v>18257</v>
@@ -4955,7 +4955,7 @@
         <v>4386</v>
       </c>
       <c r="R8" s="15">
-        <v>4398</v>
+        <v>4378</v>
       </c>
       <c r="S8" s="15">
         <v>4592</v>
@@ -5116,7 +5116,7 @@
         <v>8157</v>
       </c>
       <c r="R9" s="15">
-        <v>8985</v>
+        <v>8832</v>
       </c>
       <c r="S9" s="15">
         <v>9617</v>
@@ -5277,7 +5277,7 @@
         <v>13618</v>
       </c>
       <c r="R10" s="15">
-        <v>13598</v>
+        <v>13495</v>
       </c>
       <c r="S10" s="15">
         <v>13097</v>
@@ -5438,7 +5438,7 @@
         <v>46379</v>
       </c>
       <c r="R11" s="15">
-        <v>48028</v>
+        <v>47771</v>
       </c>
       <c r="S11" s="15">
         <v>47852</v>
@@ -5599,7 +5599,7 @@
         <v>112010</v>
       </c>
       <c r="R12" s="7">
-        <v>111621</v>
+        <v>111333</v>
       </c>
       <c r="S12" s="7">
         <v>111746</v>
@@ -5820,7 +5820,7 @@
         <v>466.76651600000002</v>
       </c>
       <c r="R15" s="15">
-        <v>434.28164199999998</v>
+        <v>432.52366599999999</v>
       </c>
       <c r="S15" s="15">
         <v>437.72687500000001</v>
@@ -5981,7 +5981,7 @@
         <v>909.53954399999998</v>
       </c>
       <c r="R16" s="15">
-        <v>960.82308999999998</v>
+        <v>958.96485099999995</v>
       </c>
       <c r="S16" s="15">
         <v>897.21795999999995</v>
@@ -6142,7 +6142,7 @@
         <v>582.22220200000004</v>
       </c>
       <c r="R17" s="15">
-        <v>580.56163300000003</v>
+        <v>580.18517199999997</v>
       </c>
       <c r="S17" s="15">
         <v>525.17944599999998</v>
@@ -6303,7 +6303,7 @@
         <v>62.842471000000003</v>
       </c>
       <c r="R18" s="15">
-        <v>60.100155999999998</v>
+        <v>59.659866999999998</v>
       </c>
       <c r="S18" s="15">
         <v>59.563484000000003</v>
@@ -6464,7 +6464,7 @@
         <v>416.86198000000002</v>
       </c>
       <c r="R19" s="15">
-        <v>416.42678799999999</v>
+        <v>411.595395</v>
       </c>
       <c r="S19" s="15">
         <v>436.07745199999999</v>
@@ -6625,7 +6625,7 @@
         <v>1266.0550499999999</v>
       </c>
       <c r="R20" s="15">
-        <v>1243.4376119999999</v>
+        <v>1233.8073380000001</v>
       </c>
       <c r="S20" s="15">
         <v>1224.9980250000001</v>
@@ -6786,7 +6786,7 @@
         <v>1137.121359</v>
       </c>
       <c r="R21" s="15">
-        <v>1177.19389</v>
+        <v>1170.4094789999999</v>
       </c>
       <c r="S21" s="15">
         <v>1165.948071</v>
@@ -6947,7 +6947,7 @@
         <v>4841.409122</v>
       </c>
       <c r="R22" s="7">
-        <v>4872.8248110000004</v>
+        <v>4847.1457680000003</v>
       </c>
       <c r="S22" s="7">
         <v>4746.7113129999998</v>
@@ -7114,10 +7114,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="E22" sqref="A1:XFD1048576"/>
-      <selection pane="topRight" activeCell="E22" sqref="A1:XFD1048576"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="A1:XFD1048576"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="A1:XFD1048576"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7568,7 +7568,7 @@
         <v>5871</v>
       </c>
       <c r="R5" s="15">
-        <v>0</v>
+        <v>5746</v>
       </c>
       <c r="S5" s="15">
         <v>0</v>
@@ -7730,7 +7730,7 @@
         <v>11850</v>
       </c>
       <c r="R6" s="6">
-        <v>0</v>
+        <v>11708</v>
       </c>
       <c r="S6" s="6">
         <v>0</v>
@@ -7892,7 +7892,7 @@
         <v>16394</v>
       </c>
       <c r="R7" s="6">
-        <v>0</v>
+        <v>17345</v>
       </c>
       <c r="S7" s="6">
         <v>0</v>
@@ -8054,7 +8054,7 @@
         <v>4688</v>
       </c>
       <c r="R8" s="6">
-        <v>0</v>
+        <v>3775</v>
       </c>
       <c r="S8" s="6">
         <v>0</v>
@@ -8216,7 +8216,7 @@
         <v>9794</v>
       </c>
       <c r="R9" s="6">
-        <v>0</v>
+        <v>10004</v>
       </c>
       <c r="S9" s="6">
         <v>0</v>
@@ -8378,7 +8378,7 @@
         <v>14085</v>
       </c>
       <c r="R10" s="15">
-        <v>0</v>
+        <v>15798</v>
       </c>
       <c r="S10" s="15">
         <v>0</v>
@@ -8540,7 +8540,7 @@
         <v>43999</v>
       </c>
       <c r="R11" s="6">
-        <v>0</v>
+        <v>49080</v>
       </c>
       <c r="S11" s="6">
         <v>0</v>
@@ -8702,7 +8702,7 @@
         <v>106681</v>
       </c>
       <c r="R12" s="7">
-        <v>0</v>
+        <v>113456</v>
       </c>
       <c r="S12" s="7">
         <v>0</v>
@@ -8926,7 +8926,7 @@
         <v>416.032217</v>
       </c>
       <c r="R15" s="15">
-        <v>0</v>
+        <v>402.27622200000002</v>
       </c>
       <c r="S15" s="15">
         <v>0</v>
@@ -9088,7 +9088,7 @@
         <v>847.46041200000002</v>
       </c>
       <c r="R16" s="6">
-        <v>0</v>
+        <v>848.62150999999994</v>
       </c>
       <c r="S16" s="6">
         <v>0</v>
@@ -9250,7 +9250,7 @@
         <v>486.53375299999999</v>
       </c>
       <c r="R17" s="6">
-        <v>0</v>
+        <v>413.43809199999998</v>
       </c>
       <c r="S17" s="6">
         <v>0</v>
@@ -9412,7 +9412,7 @@
         <v>75.546479000000005</v>
       </c>
       <c r="R18" s="6">
-        <v>0</v>
+        <v>61.153872</v>
       </c>
       <c r="S18" s="6">
         <v>0</v>
@@ -9574,7 +9574,7 @@
         <v>453.855433</v>
       </c>
       <c r="R19" s="6">
-        <v>0</v>
+        <v>467.47982000000002</v>
       </c>
       <c r="S19" s="6">
         <v>0</v>
@@ -9736,7 +9736,7 @@
         <v>1338.1306589999999</v>
       </c>
       <c r="R20" s="15">
-        <v>0</v>
+        <v>1511.7129030000001</v>
       </c>
       <c r="S20" s="15">
         <v>0</v>
@@ -9898,7 +9898,7 @@
         <v>981.18432499999994</v>
       </c>
       <c r="R21" s="6">
-        <v>0</v>
+        <v>1189.11205</v>
       </c>
       <c r="S21" s="6">
         <v>0</v>
@@ -10060,7 +10060,7 @@
         <v>4598.7432779999999</v>
       </c>
       <c r="R22" s="7">
-        <v>0</v>
+        <v>4893.7944690000004</v>
       </c>
       <c r="S22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue May  6 05:30:34 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37C24C59-817E-4270-8086-19EC871F15FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BFBABAE-D72D-41A2-909B-2B4AF7571F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -968,16 +968,16 @@
       <selection pane="bottomRight" activeCell="O12" sqref="O12:X12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="9" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="9"/>
+    <col min="1" max="1" width="50.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="9" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -1034,7 +1034,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -1356,12 +1356,12 @@
         <v>42365</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>6942</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>11626</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>12499</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>6294</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>81196</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2704,12 +2704,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>470.98508700000002</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>958.98562200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>296.27038100000027</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>48.659481</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>212.439166</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>901.73460399999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>700.69452899999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>3589.7688700000003</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -4018,23 +4018,23 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AF4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="AJ25" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -4091,7 +4091,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -4252,7 +4252,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -4414,12 +4414,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>5924</v>
       </c>
       <c r="S5" s="15">
-        <v>5983</v>
+        <v>5973</v>
       </c>
       <c r="T5" s="15">
         <v>5969</v>
@@ -4580,7 +4580,7 @@
         <v>4363</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>12661</v>
       </c>
       <c r="S6" s="15">
-        <v>12348</v>
+        <v>12333</v>
       </c>
       <c r="T6" s="15">
         <v>13351</v>
@@ -4741,7 +4741,7 @@
         <v>11478</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>18272</v>
       </c>
       <c r="S7" s="15">
-        <v>18257</v>
+        <v>18873</v>
       </c>
       <c r="T7" s="15">
         <v>20116</v>
@@ -4902,7 +4902,7 @@
         <v>16410</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>4378</v>
       </c>
       <c r="S8" s="15">
-        <v>4592</v>
+        <v>4560</v>
       </c>
       <c r="T8" s="15">
         <v>4625</v>
@@ -5063,7 +5063,7 @@
         <v>2807</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -5119,7 +5119,7 @@
         <v>8832</v>
       </c>
       <c r="S9" s="15">
-        <v>9617</v>
+        <v>9382</v>
       </c>
       <c r="T9" s="15">
         <v>9214</v>
@@ -5224,7 +5224,7 @@
         <v>8047</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>13495</v>
       </c>
       <c r="S10" s="15">
-        <v>13097</v>
+        <v>13162</v>
       </c>
       <c r="T10" s="15">
         <v>13234</v>
@@ -5385,7 +5385,7 @@
         <v>12133</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>47771</v>
       </c>
       <c r="S11" s="15">
-        <v>47852</v>
+        <v>47746</v>
       </c>
       <c r="T11" s="15">
         <v>47183</v>
@@ -5546,7 +5546,7 @@
         <v>29432</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>111333</v>
       </c>
       <c r="S12" s="7">
-        <v>111746</v>
+        <v>112029</v>
       </c>
       <c r="T12" s="7">
         <v>113692</v>
@@ -5707,7 +5707,7 @@
         <v>84670</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5762,12 +5762,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -5823,7 +5823,7 @@
         <v>432.52366599999999</v>
       </c>
       <c r="S15" s="15">
-        <v>437.72687500000001</v>
+        <v>437.05608100000001</v>
       </c>
       <c r="T15" s="15">
         <v>468.84776099999999</v>
@@ -5928,7 +5928,7 @@
         <v>303.44771800000001</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -5984,7 +5984,7 @@
         <v>958.96485099999995</v>
       </c>
       <c r="S16" s="15">
-        <v>897.21795999999995</v>
+        <v>895.51400100000001</v>
       </c>
       <c r="T16" s="15">
         <v>961.49862599999994</v>
@@ -6089,7 +6089,7 @@
         <v>868.11864300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>580.18517199999997</v>
       </c>
       <c r="S17" s="15">
-        <v>525.17944599999998</v>
+        <v>524.87520500000005</v>
       </c>
       <c r="T17" s="15">
         <v>600.91141400000004</v>
@@ -6250,7 +6250,7 @@
         <v>433.165955</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>59.659866999999998</v>
       </c>
       <c r="S18" s="15">
-        <v>59.563484000000003</v>
+        <v>58.891680999999998</v>
       </c>
       <c r="T18" s="15">
         <v>63.698661000000001</v>
@@ -6411,7 +6411,7 @@
         <v>42.773207999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -6467,7 +6467,7 @@
         <v>411.595395</v>
       </c>
       <c r="S19" s="15">
-        <v>436.07745199999999</v>
+        <v>431.96934599999997</v>
       </c>
       <c r="T19" s="15">
         <v>441.94848300000001</v>
@@ -6572,7 +6572,7 @@
         <v>374.79168900000002</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -6628,7 +6628,7 @@
         <v>1233.8073380000001</v>
       </c>
       <c r="S20" s="15">
-        <v>1224.9980250000001</v>
+        <v>1228.3774980000001</v>
       </c>
       <c r="T20" s="15">
         <v>1206.7248500000001</v>
@@ -6733,7 +6733,7 @@
         <v>1143.806075</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -6789,7 +6789,7 @@
         <v>1170.4094789999999</v>
       </c>
       <c r="S21" s="15">
-        <v>1165.948071</v>
+        <v>1164.0974289999999</v>
       </c>
       <c r="T21" s="15">
         <v>1130.783817</v>
@@ -6894,7 +6894,7 @@
         <v>657.70498399999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>4847.1457680000003</v>
       </c>
       <c r="S22" s="7">
-        <v>4746.7113129999998</v>
+        <v>4740.7812410000006</v>
       </c>
       <c r="T22" s="7">
         <v>4874.4136120000003</v>
@@ -7055,40 +7055,40 @@
         <v>3823.8082720000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -7114,22 +7114,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="53" width="9.42578125" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.42578125" customWidth="1"/>
-    <col min="55" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="53" width="9.44140625" style="1" customWidth="1"/>
+    <col min="54" max="54" width="9.44140625" customWidth="1"/>
+    <col min="55" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -7186,7 +7186,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -7347,7 +7347,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -7509,13 +7509,13 @@
       </c>
       <c r="BB3" s="24"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -7571,7 +7571,7 @@
         <v>5746</v>
       </c>
       <c r="S5" s="15">
-        <v>0</v>
+        <v>5583</v>
       </c>
       <c r="T5" s="15">
         <v>0</v>
@@ -7677,7 +7677,7 @@
       </c>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -7733,7 +7733,7 @@
         <v>11708</v>
       </c>
       <c r="S6" s="6">
-        <v>0</v>
+        <v>11560</v>
       </c>
       <c r="T6" s="6">
         <v>0</v>
@@ -7839,7 +7839,7 @@
       </c>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -7895,7 +7895,7 @@
         <v>17345</v>
       </c>
       <c r="S7" s="6">
-        <v>0</v>
+        <v>16720</v>
       </c>
       <c r="T7" s="6">
         <v>0</v>
@@ -8001,7 +8001,7 @@
       </c>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -8057,7 +8057,7 @@
         <v>3775</v>
       </c>
       <c r="S8" s="6">
-        <v>0</v>
+        <v>4179</v>
       </c>
       <c r="T8" s="6">
         <v>0</v>
@@ -8163,7 +8163,7 @@
       </c>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -8219,7 +8219,7 @@
         <v>10004</v>
       </c>
       <c r="S9" s="6">
-        <v>0</v>
+        <v>9340</v>
       </c>
       <c r="T9" s="6">
         <v>0</v>
@@ -8325,7 +8325,7 @@
       </c>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -8381,7 +8381,7 @@
         <v>15798</v>
       </c>
       <c r="S10" s="15">
-        <v>0</v>
+        <v>16024</v>
       </c>
       <c r="T10" s="15">
         <v>0</v>
@@ -8487,7 +8487,7 @@
       </c>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -8543,7 +8543,7 @@
         <v>49080</v>
       </c>
       <c r="S11" s="6">
-        <v>0</v>
+        <v>48450</v>
       </c>
       <c r="T11" s="6">
         <v>0</v>
@@ -8649,7 +8649,7 @@
       </c>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -8705,7 +8705,7 @@
         <v>113456</v>
       </c>
       <c r="S12" s="7">
-        <v>0</v>
+        <v>111856</v>
       </c>
       <c r="T12" s="7">
         <v>0</v>
@@ -8811,7 +8811,7 @@
       </c>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -8867,13 +8867,13 @@
       <c r="BA13" s="6"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -8929,7 +8929,7 @@
         <v>402.27622200000002</v>
       </c>
       <c r="S15" s="15">
-        <v>0</v>
+        <v>402.90270500000003</v>
       </c>
       <c r="T15" s="15">
         <v>0</v>
@@ -9035,7 +9035,7 @@
       </c>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -9091,7 +9091,7 @@
         <v>848.62150999999994</v>
       </c>
       <c r="S16" s="6">
-        <v>0</v>
+        <v>843.89408000000003</v>
       </c>
       <c r="T16" s="6">
         <v>0</v>
@@ -9197,7 +9197,7 @@
       </c>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -9253,7 +9253,7 @@
         <v>413.43809199999998</v>
       </c>
       <c r="S17" s="6">
-        <v>0</v>
+        <v>552.20851100000004</v>
       </c>
       <c r="T17" s="6">
         <v>0</v>
@@ -9359,7 +9359,7 @@
       </c>
       <c r="BB17"/>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -9415,7 +9415,7 @@
         <v>61.153872</v>
       </c>
       <c r="S18" s="6">
-        <v>0</v>
+        <v>63.105718000000003</v>
       </c>
       <c r="T18" s="6">
         <v>0</v>
@@ -9521,7 +9521,7 @@
       </c>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9577,7 +9577,7 @@
         <v>467.47982000000002</v>
       </c>
       <c r="S19" s="6">
-        <v>0</v>
+        <v>439.507722</v>
       </c>
       <c r="T19" s="6">
         <v>0</v>
@@ -9683,7 +9683,7 @@
       </c>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -9739,7 +9739,7 @@
         <v>1511.7129030000001</v>
       </c>
       <c r="S20" s="15">
-        <v>0</v>
+        <v>1606.8460190000001</v>
       </c>
       <c r="T20" s="15">
         <v>0</v>
@@ -9845,7 +9845,7 @@
       </c>
       <c r="BB20"/>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -9901,7 +9901,7 @@
         <v>1189.11205</v>
       </c>
       <c r="S21" s="6">
-        <v>0</v>
+        <v>1160.1779160000001</v>
       </c>
       <c r="T21" s="6">
         <v>0</v>
@@ -10007,7 +10007,7 @@
       </c>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10063,7 +10063,7 @@
         <v>4893.7944690000004</v>
       </c>
       <c r="S22" s="7">
-        <v>0</v>
+        <v>5068.6426709999996</v>
       </c>
       <c r="T22" s="7">
         <v>0</v>
@@ -10169,100 +10169,100 @@
       </c>
       <c r="BB22"/>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="BB23"/>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB24"/>
     </row>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB25"/>
     </row>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB26"/>
     </row>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB27"/>
     </row>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB28"/>
     </row>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB29"/>
     </row>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB30"/>
     </row>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB31"/>
     </row>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB32"/>
     </row>
-    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB33"/>
     </row>
-    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB34"/>
     </row>
-    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB35"/>
     </row>
-    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB36"/>
     </row>
-    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB37"/>
     </row>
-    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB38"/>
     </row>
-    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB39"/>
     </row>
-    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB40"/>
     </row>
-    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB41"/>
     </row>
-    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB42"/>
     </row>
-    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB43"/>
     </row>
-    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB44"/>
     </row>
-    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB45"/>
     </row>
-    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB46"/>
     </row>
-    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB47"/>
     </row>
-    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB48"/>
     </row>
-    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB49"/>
     </row>
-    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB50"/>
     </row>
-    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB51"/>
     </row>
-    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB52"/>
     </row>
-    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB53"/>
     </row>
-    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB54"/>
     </row>
   </sheetData>
@@ -10295,16 +10295,16 @@
       <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="17" customWidth="1"/>
     <col min="53" max="53" width="9" style="17" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="17"/>
+    <col min="54" max="16384" width="6.6640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -10361,7 +10361,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -10522,7 +10522,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -10684,12 +10684,12 @@
       </c>
       <c r="BB3" s="23"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -10850,7 +10850,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -11011,7 +11011,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -11172,7 +11172,7 @@
         <v>15693</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -11333,7 +11333,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -11494,7 +11494,7 @@
         <v>6531</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11655,7 +11655,7 @@
         <v>10908</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -11816,7 +11816,7 @@
         <v>33194</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -11977,7 +11977,7 @@
         <v>88077</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -12032,12 +12032,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -12198,7 +12198,7 @@
         <v>448.48865799999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -12359,7 +12359,7 @@
         <v>863.31579299999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -12520,7 +12520,7 @@
         <v>424.08659699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -12681,7 +12681,7 @@
         <v>49.649962000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -12842,7 +12842,7 @@
         <v>235.51133100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -13003,7 +13003,7 @@
         <v>961.98002299999996</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -13164,7 +13164,7 @@
         <v>764.98213299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -13325,38 +13325,38 @@
         <v>3748.0144969999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -13385,16 +13385,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
@@ -13451,7 +13451,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -13612,7 +13612,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -13773,12 +13773,12 @@
         <v>43093</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -13939,7 +13939,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -14100,7 +14100,7 @@
         <v>9513</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -14261,7 +14261,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -14422,7 +14422,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -14583,7 +14583,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -14744,7 +14744,7 @@
         <v>9414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -14905,7 +14905,7 @@
         <v>36964</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -15066,7 +15066,7 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -15121,12 +15121,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -15287,7 +15287,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -15448,7 +15448,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -15609,7 +15609,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -15770,7 +15770,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -15931,7 +15931,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -16092,7 +16092,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -16253,7 +16253,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -16414,38 +16414,38 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -16470,16 +16470,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
     <col min="53" max="53" width="9" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -16536,7 +16536,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16697,7 +16697,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -16859,12 +16859,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -17025,7 +17025,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -17186,7 +17186,7 @@
         <v>12729</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -17347,7 +17347,7 @@
         <v>16661</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -17508,7 +17508,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -17669,7 +17669,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -17830,7 +17830,7 @@
         <v>12175</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -17991,7 +17991,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -18152,7 +18152,7 @@
         <v>97169</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -18207,12 +18207,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -18373,7 +18373,7 @@
         <v>345.26898999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -18534,7 +18534,7 @@
         <v>1137.3429249999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -18695,7 +18695,7 @@
         <v>337.41420499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -18856,7 +18856,7 @@
         <v>40.33334</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -19017,7 +19017,7 @@
         <v>339.10771799999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -19178,7 +19178,7 @@
         <v>1247.683331</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -19339,7 +19339,7 @@
         <v>821.21724600000005</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -19500,38 +19500,38 @@
         <v>4268.3677550000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -19548,16 +19548,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -19614,7 +19614,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -19775,7 +19775,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -19937,12 +19937,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -20103,7 +20103,7 @@
         <v>5356</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -20264,7 +20264,7 @@
         <v>12576</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -20425,7 +20425,7 @@
         <v>17944</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -20586,7 +20586,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -20747,7 +20747,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -20908,7 +20908,7 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -21069,7 +21069,7 @@
         <v>38154</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -21230,7 +21230,7 @@
         <v>92789</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -21285,12 +21285,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -21451,7 +21451,7 @@
         <v>356.60756500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -21612,7 +21612,7 @@
         <v>977.829027</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -21773,7 +21773,7 @@
         <v>495.993199</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -21934,7 +21934,7 @@
         <v>37.412531000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -22095,7 +22095,7 @@
         <v>351.68923999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -22256,7 +22256,7 @@
         <v>888.50449000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -22417,7 +22417,7 @@
         <v>804.61703199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -22578,38 +22578,38 @@
         <v>3912.6530840000005</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -22626,17 +22626,17 @@
       <selection activeCell="A5" sqref="A5:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
@@ -22693,7 +22693,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -22857,7 +22857,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -23019,7 +23019,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -23183,12 +23183,12 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -23352,7 +23352,7 @@
         <v>6187</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -23516,7 +23516,7 @@
         <v>11221</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -23680,7 +23680,7 @@
         <v>16946</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -23844,7 +23844,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
@@ -24008,7 +24008,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -24172,7 +24172,7 @@
         <v>13026</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -24336,7 +24336,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -24500,7 +24500,7 @@
         <v>99721</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -24556,12 +24556,12 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -24725,7 +24725,7 @@
         <v>469.697947</v>
       </c>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -24889,7 +24889,7 @@
         <v>800.96283800000003</v>
       </c>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -25053,7 +25053,7 @@
         <v>463.52606100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
@@ -25217,7 +25217,7 @@
         <v>39.121160000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -25381,7 +25381,7 @@
         <v>320.92344600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -25545,7 +25545,7 @@
         <v>1254.2732289999999</v>
       </c>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -25709,7 +25709,7 @@
         <v>905.27916400000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -25873,38 +25873,38 @@
         <v>4253.7838449999999</v>
       </c>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -25925,16 +25925,16 @@
       <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
@@ -25991,7 +25991,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -26152,7 +26152,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -26314,12 +26314,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -26480,7 +26480,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -26641,7 +26641,7 @@
         <v>10430</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -26802,7 +26802,7 @@
         <v>15971</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -26963,7 +26963,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -27124,7 +27124,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -27285,7 +27285,7 @@
         <v>8618</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -27446,7 +27446,7 @@
         <v>34889</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -27607,7 +27607,7 @@
         <v>83267</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -27662,12 +27662,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -27828,7 +27828,7 @@
         <v>326.63437199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -27989,7 +27989,7 @@
         <v>710.31911300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -28150,7 +28150,7 @@
         <v>390.89581099999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -28311,7 +28311,7 @@
         <v>36.150655</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -28472,7 +28472,7 @@
         <v>232.43127799999999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -28633,7 +28633,7 @@
         <v>750.77748799999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -28794,7 +28794,7 @@
         <v>735.26635299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28955,40 +28955,40 @@
         <v>3182.4750699999995</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -29001,6 +29001,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -29016,16 +29019,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -29082,7 +29085,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -29243,7 +29246,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -29405,12 +29408,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -29571,7 +29574,7 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -29732,7 +29735,7 @@
         <v>11045</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -29893,7 +29896,7 @@
         <v>14998</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -30054,7 +30057,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -30215,7 +30218,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -30376,7 +30379,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -30537,7 +30540,7 @@
         <v>31551</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -30698,7 +30701,7 @@
         <v>81088</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -30753,12 +30756,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -30919,7 +30922,7 @@
         <v>307.73157300000003</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -31080,7 +31083,7 @@
         <v>782.92677600000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -31241,7 +31244,7 @@
         <v>401.64126599999997</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -31402,7 +31405,7 @@
         <v>32.955354</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -31563,7 +31566,7 @@
         <v>272.11873100000003</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -31724,7 +31727,7 @@
         <v>976.60348099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -31885,7 +31888,7 @@
         <v>752.63757299999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -32046,40 +32049,40 @@
         <v>3526.6147539999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -32107,16 +32110,16 @@
       <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -32173,7 +32176,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -32334,7 +32337,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -32496,12 +32499,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -32662,7 +32665,7 @@
         <v>4413</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -32823,7 +32826,7 @@
         <v>11673</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -32984,7 +32987,7 @@
         <v>15590</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -33145,7 +33148,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -33306,7 +33309,7 @@
         <v>8134</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -33467,7 +33470,7 @@
         <v>9863</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -33628,7 +33631,7 @@
         <v>34066</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -33789,7 +33792,7 @@
         <v>86245</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -33844,12 +33847,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -34010,7 +34013,7 @@
         <v>298.50642199999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -34171,7 +34174,7 @@
         <v>888.297684</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -34332,7 +34335,7 @@
         <v>533.92582100000004</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -34493,7 +34496,7 @@
         <v>38.857964000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -34654,7 +34657,7 @@
         <v>364.61675700000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -34815,7 +34818,7 @@
         <v>992.76339499999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -34976,7 +34979,7 @@
         <v>755.640308</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -35137,40 +35140,40 @@
         <v>3872.6083509999999</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue May 13 05:29:59 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BFBABAE-D72D-41A2-909B-2B4AF7571F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B47D5A10-03A5-4EFE-B299-17391970486D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -317,7 +317,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="26">
   <si>
     <t>METALS&amp;MINERALS \ MÉTAUX ET MINÉRAUX</t>
   </si>
@@ -395,6 +395,9 @@
   </si>
   <si>
     <t>GRAIN &amp; FERTS \ PRODUITS CÉRÉALIERS ET ENGRAIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CN 2025 – Business Units Carloads and RTMs by AAR weeks \ Sommaire hebdomadaires des wagons complets et TMC par groupe commercial </t>
   </si>
 </sst>
 </file>
@@ -4036,7 +4039,7 @@
   <sheetData>
     <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -4478,7 +4481,7 @@
         <v>5973</v>
       </c>
       <c r="T5" s="15">
-        <v>5969</v>
+        <v>5951</v>
       </c>
       <c r="U5" s="15">
         <v>6196</v>
@@ -4639,7 +4642,7 @@
         <v>12333</v>
       </c>
       <c r="T6" s="15">
-        <v>13351</v>
+        <v>13315</v>
       </c>
       <c r="U6" s="15">
         <v>13018</v>
@@ -4800,7 +4803,7 @@
         <v>18873</v>
       </c>
       <c r="T7" s="15">
-        <v>20116</v>
+        <v>20598</v>
       </c>
       <c r="U7" s="15">
         <v>19484</v>
@@ -4961,7 +4964,7 @@
         <v>4560</v>
       </c>
       <c r="T8" s="15">
-        <v>4625</v>
+        <v>4618</v>
       </c>
       <c r="U8" s="15">
         <v>4874</v>
@@ -5122,7 +5125,7 @@
         <v>9382</v>
       </c>
       <c r="T9" s="15">
-        <v>9214</v>
+        <v>9066</v>
       </c>
       <c r="U9" s="15">
         <v>8202</v>
@@ -5283,7 +5286,7 @@
         <v>13162</v>
       </c>
       <c r="T10" s="15">
-        <v>13234</v>
+        <v>13217</v>
       </c>
       <c r="U10" s="15">
         <v>12545</v>
@@ -5444,7 +5447,7 @@
         <v>47746</v>
       </c>
       <c r="T11" s="15">
-        <v>47183</v>
+        <v>47131</v>
       </c>
       <c r="U11" s="15">
         <v>48405</v>
@@ -5605,7 +5608,7 @@
         <v>112029</v>
       </c>
       <c r="T12" s="7">
-        <v>113692</v>
+        <v>113896</v>
       </c>
       <c r="U12" s="7">
         <v>112724</v>
@@ -5826,7 +5829,7 @@
         <v>437.05608100000001</v>
       </c>
       <c r="T15" s="15">
-        <v>468.84776099999999</v>
+        <v>468.43502999999998</v>
       </c>
       <c r="U15" s="15">
         <v>475.30123500000002</v>
@@ -5987,7 +5990,7 @@
         <v>895.51400100000001</v>
       </c>
       <c r="T16" s="15">
-        <v>961.49862599999994</v>
+        <v>961.06531600000005</v>
       </c>
       <c r="U16" s="15">
         <v>939.90050799999995</v>
@@ -6148,7 +6151,7 @@
         <v>524.87520500000005</v>
       </c>
       <c r="T17" s="15">
-        <v>600.91141400000004</v>
+        <v>599.87053300000002</v>
       </c>
       <c r="U17" s="15">
         <v>641.60517800000002</v>
@@ -6309,7 +6312,7 @@
         <v>58.891680999999998</v>
       </c>
       <c r="T18" s="15">
-        <v>63.698661000000001</v>
+        <v>63.670783999999998</v>
       </c>
       <c r="U18" s="15">
         <v>74.179484000000002</v>
@@ -6470,7 +6473,7 @@
         <v>431.96934599999997</v>
       </c>
       <c r="T19" s="15">
-        <v>441.94848300000001</v>
+        <v>437.38442700000002</v>
       </c>
       <c r="U19" s="15">
         <v>419.12581699999998</v>
@@ -6631,7 +6634,7 @@
         <v>1228.3774980000001</v>
       </c>
       <c r="T20" s="15">
-        <v>1206.7248500000001</v>
+        <v>1204.2712320000001</v>
       </c>
       <c r="U20" s="15">
         <v>1118.5150249999999</v>
@@ -6792,7 +6795,7 @@
         <v>1164.0974289999999</v>
       </c>
       <c r="T21" s="15">
-        <v>1130.783817</v>
+        <v>1129.892636</v>
       </c>
       <c r="U21" s="15">
         <v>1084.9743530000001</v>
@@ -6953,7 +6956,7 @@
         <v>4740.7812410000006</v>
       </c>
       <c r="T22" s="7">
-        <v>4874.4136120000003</v>
+        <v>4864.5899580000005</v>
       </c>
       <c r="U22" s="7">
         <v>4753.6016</v>
@@ -7114,9 +7117,9 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -7131,7 +7134,7 @@
   <sheetData>
     <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -7574,7 +7577,7 @@
         <v>5583</v>
       </c>
       <c r="T5" s="15">
-        <v>0</v>
+        <v>5667</v>
       </c>
       <c r="U5" s="15">
         <v>0</v>
@@ -7736,7 +7739,7 @@
         <v>11560</v>
       </c>
       <c r="T6" s="6">
-        <v>0</v>
+        <v>11831</v>
       </c>
       <c r="U6" s="6">
         <v>0</v>
@@ -7898,7 +7901,7 @@
         <v>16720</v>
       </c>
       <c r="T7" s="6">
-        <v>0</v>
+        <v>19801</v>
       </c>
       <c r="U7" s="6">
         <v>0</v>
@@ -8060,7 +8063,7 @@
         <v>4179</v>
       </c>
       <c r="T8" s="6">
-        <v>0</v>
+        <v>4156</v>
       </c>
       <c r="U8" s="6">
         <v>0</v>
@@ -8222,7 +8225,7 @@
         <v>9340</v>
       </c>
       <c r="T9" s="6">
-        <v>0</v>
+        <v>8632</v>
       </c>
       <c r="U9" s="6">
         <v>0</v>
@@ -8384,7 +8387,7 @@
         <v>16024</v>
       </c>
       <c r="T10" s="15">
-        <v>0</v>
+        <v>14346</v>
       </c>
       <c r="U10" s="15">
         <v>0</v>
@@ -8546,7 +8549,7 @@
         <v>48450</v>
       </c>
       <c r="T11" s="6">
-        <v>0</v>
+        <v>48795</v>
       </c>
       <c r="U11" s="6">
         <v>0</v>
@@ -8708,7 +8711,7 @@
         <v>111856</v>
       </c>
       <c r="T12" s="7">
-        <v>0</v>
+        <v>113228</v>
       </c>
       <c r="U12" s="7">
         <v>0</v>
@@ -8932,7 +8935,7 @@
         <v>402.90270500000003</v>
       </c>
       <c r="T15" s="15">
-        <v>0</v>
+        <v>393.793789</v>
       </c>
       <c r="U15" s="15">
         <v>0</v>
@@ -9094,7 +9097,7 @@
         <v>843.89408000000003</v>
       </c>
       <c r="T16" s="6">
-        <v>0</v>
+        <v>840.71608300000003</v>
       </c>
       <c r="U16" s="6">
         <v>0</v>
@@ -9256,7 +9259,7 @@
         <v>552.20851100000004</v>
       </c>
       <c r="T17" s="6">
-        <v>0</v>
+        <v>637.60634900000002</v>
       </c>
       <c r="U17" s="6">
         <v>0</v>
@@ -9418,7 +9421,7 @@
         <v>63.105718000000003</v>
       </c>
       <c r="T18" s="6">
-        <v>0</v>
+        <v>65.083873999999994</v>
       </c>
       <c r="U18" s="6">
         <v>0</v>
@@ -9580,7 +9583,7 @@
         <v>439.507722</v>
       </c>
       <c r="T19" s="6">
-        <v>0</v>
+        <v>414.64652000000001</v>
       </c>
       <c r="U19" s="6">
         <v>0</v>
@@ -9742,7 +9745,7 @@
         <v>1606.8460190000001</v>
       </c>
       <c r="T20" s="15">
-        <v>0</v>
+        <v>1406.443096</v>
       </c>
       <c r="U20" s="15">
         <v>0</v>
@@ -9904,7 +9907,7 @@
         <v>1160.1779160000001</v>
       </c>
       <c r="T21" s="6">
-        <v>0</v>
+        <v>1120.8255489999999</v>
       </c>
       <c r="U21" s="6">
         <v>0</v>
@@ -10066,7 +10069,7 @@
         <v>5068.6426709999996</v>
       </c>
       <c r="T22" s="7">
-        <v>0</v>
+        <v>4879.1152600000005</v>
       </c>
       <c r="U22" s="7">
         <v>0</v>
@@ -29001,9 +29004,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
GH ACTION Autorun Wed May 21 05:30:47 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B47D5A10-03A5-4EFE-B299-17391970486D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFF61911-A6B2-4666-97BE-2C2F17A57892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -971,16 +971,16 @@
       <selection pane="bottomRight" activeCell="O12" sqref="O12:X12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="9" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="9"/>
+    <col min="1" max="1" width="50.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="9" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -1359,12 +1359,12 @@
         <v>42365</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>6942</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>11626</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>12499</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>6294</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>81196</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2707,12 +2707,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>470.98508700000002</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>958.98562200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>296.27038100000027</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>48.659481</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>212.439166</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>901.73460399999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>700.69452899999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>3589.7688700000003</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -4022,22 +4022,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
       <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -4094,7 +4094,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -4417,12 +4417,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4484,7 +4484,7 @@
         <v>5951</v>
       </c>
       <c r="U5" s="15">
-        <v>6196</v>
+        <v>6146</v>
       </c>
       <c r="V5" s="15">
         <v>5707</v>
@@ -4583,7 +4583,7 @@
         <v>4363</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>13315</v>
       </c>
       <c r="U6" s="15">
-        <v>13018</v>
+        <v>12995</v>
       </c>
       <c r="V6" s="15">
         <v>12167</v>
@@ -4744,7 +4744,7 @@
         <v>11478</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>20598</v>
       </c>
       <c r="U7" s="15">
-        <v>19484</v>
+        <v>19773</v>
       </c>
       <c r="V7" s="15">
         <v>17331</v>
@@ -4905,7 +4905,7 @@
         <v>16410</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>4618</v>
       </c>
       <c r="U8" s="15">
-        <v>4874</v>
+        <v>4854</v>
       </c>
       <c r="V8" s="15">
         <v>4511</v>
@@ -5066,7 +5066,7 @@
         <v>2807</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>9066</v>
       </c>
       <c r="U9" s="15">
-        <v>8202</v>
+        <v>8090</v>
       </c>
       <c r="V9" s="15">
         <v>7624</v>
@@ -5227,7 +5227,7 @@
         <v>8047</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>13217</v>
       </c>
       <c r="U10" s="15">
-        <v>12545</v>
+        <v>12576</v>
       </c>
       <c r="V10" s="15">
         <v>10439</v>
@@ -5388,7 +5388,7 @@
         <v>12133</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -5450,7 +5450,7 @@
         <v>47131</v>
       </c>
       <c r="U11" s="15">
-        <v>48405</v>
+        <v>48323</v>
       </c>
       <c r="V11" s="15">
         <v>45570</v>
@@ -5549,7 +5549,7 @@
         <v>29432</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>113896</v>
       </c>
       <c r="U12" s="7">
-        <v>112724</v>
+        <v>112757</v>
       </c>
       <c r="V12" s="7">
         <v>103349</v>
@@ -5710,7 +5710,7 @@
         <v>84670</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5765,12 +5765,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>468.43502999999998</v>
       </c>
       <c r="U15" s="15">
-        <v>475.30123500000002</v>
+        <v>473.15153099999998</v>
       </c>
       <c r="V15" s="15">
         <v>427.03443399999998</v>
@@ -5931,7 +5931,7 @@
         <v>303.44771800000001</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>961.06531600000005</v>
       </c>
       <c r="U16" s="15">
-        <v>939.90050799999995</v>
+        <v>939.98229800000001</v>
       </c>
       <c r="V16" s="15">
         <v>869.87526500000001</v>
@@ -6092,7 +6092,7 @@
         <v>868.11864300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>599.87053300000002</v>
       </c>
       <c r="U17" s="15">
-        <v>641.60517800000002</v>
+        <v>641.10987799999998</v>
       </c>
       <c r="V17" s="15">
         <v>472.37036000000001</v>
@@ -6253,7 +6253,7 @@
         <v>433.165955</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -6315,7 +6315,7 @@
         <v>63.670783999999998</v>
       </c>
       <c r="U18" s="15">
-        <v>74.179484000000002</v>
+        <v>73.363805999999997</v>
       </c>
       <c r="V18" s="15">
         <v>64.859252999999995</v>
@@ -6414,7 +6414,7 @@
         <v>42.773207999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -6476,7 +6476,7 @@
         <v>437.38442700000002</v>
       </c>
       <c r="U19" s="15">
-        <v>419.12581699999998</v>
+        <v>419.00699700000001</v>
       </c>
       <c r="V19" s="15">
         <v>366.07052399999998</v>
@@ -6575,7 +6575,7 @@
         <v>374.79168900000002</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -6637,7 +6637,7 @@
         <v>1204.2712320000001</v>
       </c>
       <c r="U20" s="15">
-        <v>1118.5150249999999</v>
+        <v>1124.2792099999999</v>
       </c>
       <c r="V20" s="15">
         <v>857.57130099999995</v>
@@ -6736,7 +6736,7 @@
         <v>1143.806075</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -6798,7 +6798,7 @@
         <v>1129.892636</v>
       </c>
       <c r="U21" s="15">
-        <v>1084.9743530000001</v>
+        <v>1083.8981650000001</v>
       </c>
       <c r="V21" s="15">
         <v>1072.583959</v>
@@ -6897,7 +6897,7 @@
         <v>657.70498399999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -6959,7 +6959,7 @@
         <v>4864.5899580000005</v>
       </c>
       <c r="U22" s="7">
-        <v>4753.6016</v>
+        <v>4754.7918849999987</v>
       </c>
       <c r="V22" s="7">
         <v>4130.3650959999995</v>
@@ -7058,40 +7058,40 @@
         <v>3823.8082720000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -7117,22 +7117,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
       <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="53" width="9.44140625" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.44140625" customWidth="1"/>
-    <col min="55" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="53" width="9.42578125" style="1" customWidth="1"/>
+    <col min="54" max="54" width="9.42578125" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>25</v>
       </c>
@@ -7189,7 +7189,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -7350,7 +7350,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -7512,13 +7512,13 @@
       </c>
       <c r="BB3" s="24"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -7580,7 +7580,7 @@
         <v>5667</v>
       </c>
       <c r="U5" s="15">
-        <v>0</v>
+        <v>5740</v>
       </c>
       <c r="V5" s="15">
         <v>0</v>
@@ -7680,7 +7680,7 @@
       </c>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -7742,7 +7742,7 @@
         <v>11831</v>
       </c>
       <c r="U6" s="6">
-        <v>0</v>
+        <v>11463</v>
       </c>
       <c r="V6" s="6">
         <v>0</v>
@@ -7842,7 +7842,7 @@
       </c>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -7904,7 +7904,7 @@
         <v>19801</v>
       </c>
       <c r="U7" s="6">
-        <v>0</v>
+        <v>18004</v>
       </c>
       <c r="V7" s="6">
         <v>0</v>
@@ -8004,7 +8004,7 @@
       </c>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -8066,7 +8066,7 @@
         <v>4156</v>
       </c>
       <c r="U8" s="6">
-        <v>0</v>
+        <v>4614</v>
       </c>
       <c r="V8" s="6">
         <v>0</v>
@@ -8166,7 +8166,7 @@
       </c>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -8228,7 +8228,7 @@
         <v>8632</v>
       </c>
       <c r="U9" s="6">
-        <v>0</v>
+        <v>8656</v>
       </c>
       <c r="V9" s="6">
         <v>0</v>
@@ -8328,7 +8328,7 @@
       </c>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -8390,7 +8390,7 @@
         <v>14346</v>
       </c>
       <c r="U10" s="15">
-        <v>0</v>
+        <v>13298</v>
       </c>
       <c r="V10" s="15">
         <v>0</v>
@@ -8490,7 +8490,7 @@
       </c>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -8552,7 +8552,7 @@
         <v>48795</v>
       </c>
       <c r="U11" s="6">
-        <v>0</v>
+        <v>46920</v>
       </c>
       <c r="V11" s="6">
         <v>0</v>
@@ -8652,7 +8652,7 @@
       </c>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -8714,7 +8714,7 @@
         <v>113228</v>
       </c>
       <c r="U12" s="7">
-        <v>0</v>
+        <v>108695</v>
       </c>
       <c r="V12" s="7">
         <v>0</v>
@@ -8814,7 +8814,7 @@
       </c>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -8870,13 +8870,13 @@
       <c r="BA13" s="6"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -8938,7 +8938,7 @@
         <v>393.793789</v>
       </c>
       <c r="U15" s="15">
-        <v>0</v>
+        <v>414.97911699999997</v>
       </c>
       <c r="V15" s="15">
         <v>0</v>
@@ -9038,7 +9038,7 @@
       </c>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -9100,7 +9100,7 @@
         <v>840.71608300000003</v>
       </c>
       <c r="U16" s="6">
-        <v>0</v>
+        <v>776.15857300000005</v>
       </c>
       <c r="V16" s="6">
         <v>0</v>
@@ -9200,7 +9200,7 @@
       </c>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -9262,7 +9262,7 @@
         <v>637.60634900000002</v>
       </c>
       <c r="U17" s="6">
-        <v>0</v>
+        <v>590.33088999999995</v>
       </c>
       <c r="V17" s="6">
         <v>0</v>
@@ -9362,7 +9362,7 @@
       </c>
       <c r="BB17"/>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -9424,7 +9424,7 @@
         <v>65.083873999999994</v>
       </c>
       <c r="U18" s="6">
-        <v>0</v>
+        <v>65.705006999999995</v>
       </c>
       <c r="V18" s="6">
         <v>0</v>
@@ -9524,7 +9524,7 @@
       </c>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9586,7 +9586,7 @@
         <v>414.64652000000001</v>
       </c>
       <c r="U19" s="6">
-        <v>0</v>
+        <v>393.46231299999999</v>
       </c>
       <c r="V19" s="6">
         <v>0</v>
@@ -9686,7 +9686,7 @@
       </c>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -9748,7 +9748,7 @@
         <v>1406.443096</v>
       </c>
       <c r="U20" s="15">
-        <v>0</v>
+        <v>1245.4669490000001</v>
       </c>
       <c r="V20" s="15">
         <v>0</v>
@@ -9848,7 +9848,7 @@
       </c>
       <c r="BB20"/>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -9910,7 +9910,7 @@
         <v>1120.8255489999999</v>
       </c>
       <c r="U21" s="6">
-        <v>0</v>
+        <v>1085.4425639999999</v>
       </c>
       <c r="V21" s="6">
         <v>0</v>
@@ -10010,7 +10010,7 @@
       </c>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10072,7 +10072,7 @@
         <v>4879.1152600000005</v>
       </c>
       <c r="U22" s="7">
-        <v>0</v>
+        <v>4571.5454129999998</v>
       </c>
       <c r="V22" s="7">
         <v>0</v>
@@ -10172,100 +10172,100 @@
       </c>
       <c r="BB22"/>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="BB23"/>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB24"/>
     </row>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB25"/>
     </row>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB26"/>
     </row>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB27"/>
     </row>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB28"/>
     </row>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB29"/>
     </row>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB30"/>
     </row>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB31"/>
     </row>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB32"/>
     </row>
-    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB33"/>
     </row>
-    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB34"/>
     </row>
-    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB35"/>
     </row>
-    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB36"/>
     </row>
-    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB37"/>
     </row>
-    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB38"/>
     </row>
-    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB39"/>
     </row>
-    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB40"/>
     </row>
-    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB41"/>
     </row>
-    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB42"/>
     </row>
-    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB43"/>
     </row>
-    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB44"/>
     </row>
-    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB45"/>
     </row>
-    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB46"/>
     </row>
-    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB47"/>
     </row>
-    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB48"/>
     </row>
-    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB49"/>
     </row>
-    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB50"/>
     </row>
-    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB51"/>
     </row>
-    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB52"/>
     </row>
-    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB53"/>
     </row>
-    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB54"/>
     </row>
   </sheetData>
@@ -10298,16 +10298,16 @@
       <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="17" customWidth="1"/>
     <col min="53" max="53" width="9" style="17" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="17"/>
+    <col min="54" max="16384" width="6.7109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -10364,7 +10364,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -10525,7 +10525,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -10687,12 +10687,12 @@
       </c>
       <c r="BB3" s="23"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -10853,7 +10853,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -11014,7 +11014,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -11175,7 +11175,7 @@
         <v>15693</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -11336,7 +11336,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -11497,7 +11497,7 @@
         <v>6531</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11658,7 +11658,7 @@
         <v>10908</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -11819,7 +11819,7 @@
         <v>33194</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -11980,7 +11980,7 @@
         <v>88077</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -12035,12 +12035,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -12201,7 +12201,7 @@
         <v>448.48865799999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -12362,7 +12362,7 @@
         <v>863.31579299999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -12523,7 +12523,7 @@
         <v>424.08659699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -12684,7 +12684,7 @@
         <v>49.649962000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -12845,7 +12845,7 @@
         <v>235.51133100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -13006,7 +13006,7 @@
         <v>961.98002299999996</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -13167,7 +13167,7 @@
         <v>764.98213299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -13328,38 +13328,38 @@
         <v>3748.0144969999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -13388,16 +13388,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
@@ -13454,7 +13454,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -13615,7 +13615,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -13776,12 +13776,12 @@
         <v>43093</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -13942,7 +13942,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -14103,7 +14103,7 @@
         <v>9513</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -14264,7 +14264,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -14425,7 +14425,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -14586,7 +14586,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -14747,7 +14747,7 @@
         <v>9414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -14908,7 +14908,7 @@
         <v>36964</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -15069,7 +15069,7 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -15124,12 +15124,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -15290,7 +15290,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -15451,7 +15451,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -15612,7 +15612,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -15773,7 +15773,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -15934,7 +15934,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -16095,7 +16095,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -16256,7 +16256,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -16417,38 +16417,38 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -16473,16 +16473,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
     <col min="53" max="53" width="9" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -16539,7 +16539,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16700,7 +16700,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -16862,12 +16862,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -17028,7 +17028,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -17189,7 +17189,7 @@
         <v>12729</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -17350,7 +17350,7 @@
         <v>16661</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -17511,7 +17511,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -17672,7 +17672,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -17833,7 +17833,7 @@
         <v>12175</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -17994,7 +17994,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -18155,7 +18155,7 @@
         <v>97169</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -18210,12 +18210,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -18376,7 +18376,7 @@
         <v>345.26898999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -18537,7 +18537,7 @@
         <v>1137.3429249999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -18698,7 +18698,7 @@
         <v>337.41420499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -18859,7 +18859,7 @@
         <v>40.33334</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -19020,7 +19020,7 @@
         <v>339.10771799999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -19181,7 +19181,7 @@
         <v>1247.683331</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -19342,7 +19342,7 @@
         <v>821.21724600000005</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -19503,38 +19503,38 @@
         <v>4268.3677550000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -19551,16 +19551,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -19617,7 +19617,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -19778,7 +19778,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -19940,12 +19940,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -20106,7 +20106,7 @@
         <v>5356</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -20267,7 +20267,7 @@
         <v>12576</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -20428,7 +20428,7 @@
         <v>17944</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -20589,7 +20589,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -20750,7 +20750,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -20911,7 +20911,7 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -21072,7 +21072,7 @@
         <v>38154</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -21233,7 +21233,7 @@
         <v>92789</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -21288,12 +21288,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -21454,7 +21454,7 @@
         <v>356.60756500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -21615,7 +21615,7 @@
         <v>977.829027</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -21776,7 +21776,7 @@
         <v>495.993199</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -21937,7 +21937,7 @@
         <v>37.412531000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -22098,7 +22098,7 @@
         <v>351.68923999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -22259,7 +22259,7 @@
         <v>888.50449000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -22420,7 +22420,7 @@
         <v>804.61703199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -22581,38 +22581,38 @@
         <v>3912.6530840000005</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -22629,17 +22629,17 @@
       <selection activeCell="A5" sqref="A5:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
@@ -22696,7 +22696,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="23.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -22860,7 +22860,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -23022,7 +23022,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -23186,12 +23186,12 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -23355,7 +23355,7 @@
         <v>6187</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -23519,7 +23519,7 @@
         <v>11221</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -23683,7 +23683,7 @@
         <v>16946</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -23847,7 +23847,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
@@ -24011,7 +24011,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -24175,7 +24175,7 @@
         <v>13026</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -24339,7 +24339,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -24503,7 +24503,7 @@
         <v>99721</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -24559,12 +24559,12 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -24728,7 +24728,7 @@
         <v>469.697947</v>
       </c>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -24892,7 +24892,7 @@
         <v>800.96283800000003</v>
       </c>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -25056,7 +25056,7 @@
         <v>463.52606100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
@@ -25220,7 +25220,7 @@
         <v>39.121160000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -25384,7 +25384,7 @@
         <v>320.92344600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -25548,7 +25548,7 @@
         <v>1254.2732289999999</v>
       </c>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -25712,7 +25712,7 @@
         <v>905.27916400000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -25876,38 +25876,38 @@
         <v>4253.7838449999999</v>
       </c>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -25928,16 +25928,16 @@
       <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
@@ -25994,7 +25994,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -26155,7 +26155,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -26317,12 +26317,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -26483,7 +26483,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -26644,7 +26644,7 @@
         <v>10430</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -26805,7 +26805,7 @@
         <v>15971</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -26966,7 +26966,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -27127,7 +27127,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -27288,7 +27288,7 @@
         <v>8618</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -27449,7 +27449,7 @@
         <v>34889</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -27610,7 +27610,7 @@
         <v>83267</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -27665,12 +27665,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -27831,7 +27831,7 @@
         <v>326.63437199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -27992,7 +27992,7 @@
         <v>710.31911300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -28153,7 +28153,7 @@
         <v>390.89581099999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -28314,7 +28314,7 @@
         <v>36.150655</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -28475,7 +28475,7 @@
         <v>232.43127799999999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -28636,7 +28636,7 @@
         <v>750.77748799999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -28797,7 +28797,7 @@
         <v>735.26635299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28958,40 +28958,40 @@
         <v>3182.4750699999995</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -29019,16 +29019,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -29085,7 +29085,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -29246,7 +29246,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -29408,12 +29408,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -29574,7 +29574,7 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -29735,7 +29735,7 @@
         <v>11045</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -29896,7 +29896,7 @@
         <v>14998</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -30057,7 +30057,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -30218,7 +30218,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -30379,7 +30379,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -30540,7 +30540,7 @@
         <v>31551</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -30701,7 +30701,7 @@
         <v>81088</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -30756,12 +30756,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -30922,7 +30922,7 @@
         <v>307.73157300000003</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -31083,7 +31083,7 @@
         <v>782.92677600000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -31244,7 +31244,7 @@
         <v>401.64126599999997</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -31405,7 +31405,7 @@
         <v>32.955354</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -31566,7 +31566,7 @@
         <v>272.11873100000003</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -31727,7 +31727,7 @@
         <v>976.60348099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -31888,7 +31888,7 @@
         <v>752.63757299999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -32049,40 +32049,40 @@
         <v>3526.6147539999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -32110,16 +32110,16 @@
       <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -32176,7 +32176,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -32337,7 +32337,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -32499,12 +32499,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -32665,7 +32665,7 @@
         <v>4413</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -32826,7 +32826,7 @@
         <v>11673</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -32987,7 +32987,7 @@
         <v>15590</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -33148,7 +33148,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -33309,7 +33309,7 @@
         <v>8134</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -33470,7 +33470,7 @@
         <v>9863</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -33631,7 +33631,7 @@
         <v>34066</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -33792,7 +33792,7 @@
         <v>86245</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -33847,12 +33847,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -34013,7 +34013,7 @@
         <v>298.50642199999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -34174,7 +34174,7 @@
         <v>888.297684</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -34335,7 +34335,7 @@
         <v>533.92582100000004</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -34496,7 +34496,7 @@
         <v>38.857964000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -34657,7 +34657,7 @@
         <v>364.61675700000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -34818,7 +34818,7 @@
         <v>992.76339499999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -34979,7 +34979,7 @@
         <v>755.640308</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -35140,40 +35140,40 @@
         <v>3872.6083509999999</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -35186,5 +35186,8 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GH ACTION Autorun Tue May 27 05:30:24 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFF61911-A6B2-4666-97BE-2C2F17A57892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A3F3B0F-71BD-4DE8-848F-7C480C598083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -971,16 +971,16 @@
       <selection pane="bottomRight" activeCell="O12" sqref="O12:X12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="9" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="9"/>
+    <col min="1" max="1" width="50.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="9" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -1359,12 +1359,12 @@
         <v>42365</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>6942</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>11626</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>12499</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>6294</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>81196</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2707,12 +2707,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>470.98508700000002</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>958.98562200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>296.27038100000027</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>48.659481</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>212.439166</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>901.73460399999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>700.69452899999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>3589.7688700000003</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -4022,22 +4022,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -4094,7 +4094,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -4417,12 +4417,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>6146</v>
       </c>
       <c r="V5" s="15">
-        <v>5707</v>
+        <v>5673</v>
       </c>
       <c r="W5" s="15">
         <v>5878</v>
@@ -4583,7 +4583,7 @@
         <v>4363</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>12995</v>
       </c>
       <c r="V6" s="15">
-        <v>12167</v>
+        <v>12114</v>
       </c>
       <c r="W6" s="15">
         <v>11536</v>
@@ -4744,7 +4744,7 @@
         <v>11478</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>19773</v>
       </c>
       <c r="V7" s="15">
-        <v>17331</v>
+        <v>17783</v>
       </c>
       <c r="W7" s="15">
         <v>19726</v>
@@ -4905,7 +4905,7 @@
         <v>16410</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>4854</v>
       </c>
       <c r="V8" s="15">
-        <v>4511</v>
+        <v>4497</v>
       </c>
       <c r="W8" s="15">
         <v>4424</v>
@@ -5066,7 +5066,7 @@
         <v>2807</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>8090</v>
       </c>
       <c r="V9" s="15">
-        <v>7624</v>
+        <v>7627</v>
       </c>
       <c r="W9" s="15">
         <v>9176</v>
@@ -5227,7 +5227,7 @@
         <v>8047</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>12576</v>
       </c>
       <c r="V10" s="15">
-        <v>10439</v>
+        <v>10329</v>
       </c>
       <c r="W10" s="15">
         <v>10866</v>
@@ -5388,7 +5388,7 @@
         <v>12133</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>48323</v>
       </c>
       <c r="V11" s="15">
-        <v>45570</v>
+        <v>45531</v>
       </c>
       <c r="W11" s="15">
         <v>45937</v>
@@ -5549,7 +5549,7 @@
         <v>29432</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>112757</v>
       </c>
       <c r="V12" s="7">
-        <v>103349</v>
+        <v>103554</v>
       </c>
       <c r="W12" s="7">
         <v>107543</v>
@@ -5710,7 +5710,7 @@
         <v>84670</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5765,12 +5765,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>473.15153099999998</v>
       </c>
       <c r="V15" s="15">
-        <v>427.03443399999998</v>
+        <v>425.25603100000001</v>
       </c>
       <c r="W15" s="15">
         <v>430.20757600000002</v>
@@ -5931,7 +5931,7 @@
         <v>303.44771800000001</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -5996,7 +5996,7 @@
         <v>939.98229800000001</v>
       </c>
       <c r="V16" s="15">
-        <v>869.87526500000001</v>
+        <v>867.05403999999999</v>
       </c>
       <c r="W16" s="15">
         <v>784.34190000000001</v>
@@ -6092,7 +6092,7 @@
         <v>868.11864300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -6157,7 +6157,7 @@
         <v>641.10987799999998</v>
       </c>
       <c r="V17" s="15">
-        <v>472.37036000000001</v>
+        <v>472.15919200000002</v>
       </c>
       <c r="W17" s="15">
         <v>556.07526700000005</v>
@@ -6253,7 +6253,7 @@
         <v>433.165955</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>73.363805999999997</v>
       </c>
       <c r="V18" s="15">
-        <v>64.859252999999995</v>
+        <v>64.714905999999999</v>
       </c>
       <c r="W18" s="15">
         <v>66.278502000000003</v>
@@ -6414,7 +6414,7 @@
         <v>42.773207999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -6479,7 +6479,7 @@
         <v>419.00699700000001</v>
       </c>
       <c r="V19" s="15">
-        <v>366.07052399999998</v>
+        <v>366.36616500000002</v>
       </c>
       <c r="W19" s="15">
         <v>393.01427000000001</v>
@@ -6575,7 +6575,7 @@
         <v>374.79168900000002</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>1124.2792099999999</v>
       </c>
       <c r="V20" s="15">
-        <v>857.57130099999995</v>
+        <v>846.41466100000002</v>
       </c>
       <c r="W20" s="15">
         <v>922.801649</v>
@@ -6736,7 +6736,7 @@
         <v>1143.806075</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -6801,7 +6801,7 @@
         <v>1083.8981650000001</v>
       </c>
       <c r="V21" s="15">
-        <v>1072.583959</v>
+        <v>1071.9282740000001</v>
       </c>
       <c r="W21" s="15">
         <v>1063.811273</v>
@@ -6897,7 +6897,7 @@
         <v>657.70498399999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>4754.7918849999987</v>
       </c>
       <c r="V22" s="7">
-        <v>4130.3650959999995</v>
+        <v>4113.8932690000001</v>
       </c>
       <c r="W22" s="7">
         <v>4216.5304370000003</v>
@@ -7058,40 +7058,40 @@
         <v>3823.8082720000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -7117,22 +7117,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B4" sqref="B4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="53" width="9.42578125" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.42578125" customWidth="1"/>
-    <col min="55" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="53" width="9.44140625" style="1" customWidth="1"/>
+    <col min="54" max="54" width="9.44140625" customWidth="1"/>
+    <col min="55" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>25</v>
       </c>
@@ -7189,7 +7189,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -7350,7 +7350,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -7512,13 +7512,13 @@
       </c>
       <c r="BB3" s="24"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -7583,7 +7583,7 @@
         <v>5740</v>
       </c>
       <c r="V5" s="15">
-        <v>0</v>
+        <v>5646</v>
       </c>
       <c r="W5" s="15">
         <v>0</v>
@@ -7680,7 +7680,7 @@
       </c>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -7745,7 +7745,7 @@
         <v>11463</v>
       </c>
       <c r="V6" s="6">
-        <v>0</v>
+        <v>11471</v>
       </c>
       <c r="W6" s="6">
         <v>0</v>
@@ -7842,7 +7842,7 @@
       </c>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -7907,7 +7907,7 @@
         <v>18004</v>
       </c>
       <c r="V7" s="6">
-        <v>0</v>
+        <v>18630</v>
       </c>
       <c r="W7" s="6">
         <v>0</v>
@@ -8004,7 +8004,7 @@
       </c>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -8069,7 +8069,7 @@
         <v>4614</v>
       </c>
       <c r="V8" s="6">
-        <v>0</v>
+        <v>4133</v>
       </c>
       <c r="W8" s="6">
         <v>0</v>
@@ -8166,7 +8166,7 @@
       </c>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -8231,7 +8231,7 @@
         <v>8656</v>
       </c>
       <c r="V9" s="6">
-        <v>0</v>
+        <v>7557</v>
       </c>
       <c r="W9" s="6">
         <v>0</v>
@@ -8328,7 +8328,7 @@
       </c>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -8393,7 +8393,7 @@
         <v>13298</v>
       </c>
       <c r="V10" s="15">
-        <v>0</v>
+        <v>12746</v>
       </c>
       <c r="W10" s="15">
         <v>0</v>
@@ -8490,7 +8490,7 @@
       </c>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -8555,7 +8555,7 @@
         <v>46920</v>
       </c>
       <c r="V11" s="6">
-        <v>0</v>
+        <v>44186</v>
       </c>
       <c r="W11" s="6">
         <v>0</v>
@@ -8652,7 +8652,7 @@
       </c>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -8717,7 +8717,7 @@
         <v>108695</v>
       </c>
       <c r="V12" s="7">
-        <v>0</v>
+        <v>104369</v>
       </c>
       <c r="W12" s="7">
         <v>0</v>
@@ -8814,7 +8814,7 @@
       </c>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -8870,13 +8870,13 @@
       <c r="BA13" s="6"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -8941,7 +8941,7 @@
         <v>414.97911699999997</v>
       </c>
       <c r="V15" s="15">
-        <v>0</v>
+        <v>404.07235600000001</v>
       </c>
       <c r="W15" s="15">
         <v>0</v>
@@ -9038,7 +9038,7 @@
       </c>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -9103,7 +9103,7 @@
         <v>776.15857300000005</v>
       </c>
       <c r="V16" s="6">
-        <v>0</v>
+        <v>790.26504399999999</v>
       </c>
       <c r="W16" s="6">
         <v>0</v>
@@ -9200,7 +9200,7 @@
       </c>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -9265,7 +9265,7 @@
         <v>590.33088999999995</v>
       </c>
       <c r="V17" s="6">
-        <v>0</v>
+        <v>587.69023500000003</v>
       </c>
       <c r="W17" s="6">
         <v>0</v>
@@ -9362,7 +9362,7 @@
       </c>
       <c r="BB17"/>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -9427,7 +9427,7 @@
         <v>65.705006999999995</v>
       </c>
       <c r="V18" s="6">
-        <v>0</v>
+        <v>56.712780000000002</v>
       </c>
       <c r="W18" s="6">
         <v>0</v>
@@ -9524,7 +9524,7 @@
       </c>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9589,7 +9589,7 @@
         <v>393.46231299999999</v>
       </c>
       <c r="V19" s="6">
-        <v>0</v>
+        <v>311.51239399999997</v>
       </c>
       <c r="W19" s="6">
         <v>0</v>
@@ -9686,7 +9686,7 @@
       </c>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -9751,7 +9751,7 @@
         <v>1245.4669490000001</v>
       </c>
       <c r="V20" s="15">
-        <v>0</v>
+        <v>1151.7692930000001</v>
       </c>
       <c r="W20" s="15">
         <v>0</v>
@@ -9848,7 +9848,7 @@
       </c>
       <c r="BB20"/>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -9913,7 +9913,7 @@
         <v>1085.4425639999999</v>
       </c>
       <c r="V21" s="6">
-        <v>0</v>
+        <v>946.39353800000004</v>
       </c>
       <c r="W21" s="6">
         <v>0</v>
@@ -10010,7 +10010,7 @@
       </c>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10075,7 +10075,7 @@
         <v>4571.5454129999998</v>
       </c>
       <c r="V22" s="7">
-        <v>0</v>
+        <v>4248.4156400000002</v>
       </c>
       <c r="W22" s="7">
         <v>0</v>
@@ -10172,100 +10172,100 @@
       </c>
       <c r="BB22"/>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="BB23"/>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB24"/>
     </row>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB25"/>
     </row>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB26"/>
     </row>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB27"/>
     </row>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB28"/>
     </row>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB29"/>
     </row>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB30"/>
     </row>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB31"/>
     </row>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB32"/>
     </row>
-    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB33"/>
     </row>
-    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB34"/>
     </row>
-    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB35"/>
     </row>
-    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB36"/>
     </row>
-    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB37"/>
     </row>
-    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB38"/>
     </row>
-    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB39"/>
     </row>
-    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB40"/>
     </row>
-    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB41"/>
     </row>
-    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB42"/>
     </row>
-    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB43"/>
     </row>
-    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB44"/>
     </row>
-    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB45"/>
     </row>
-    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB46"/>
     </row>
-    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB47"/>
     </row>
-    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB48"/>
     </row>
-    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB49"/>
     </row>
-    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB50"/>
     </row>
-    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB51"/>
     </row>
-    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB52"/>
     </row>
-    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB53"/>
     </row>
-    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB54"/>
     </row>
   </sheetData>
@@ -10298,16 +10298,16 @@
       <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="17" customWidth="1"/>
     <col min="53" max="53" width="9" style="17" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="17"/>
+    <col min="54" max="16384" width="6.6640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -10364,7 +10364,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -10525,7 +10525,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -10687,12 +10687,12 @@
       </c>
       <c r="BB3" s="23"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -10853,7 +10853,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -11014,7 +11014,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -11175,7 +11175,7 @@
         <v>15693</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -11336,7 +11336,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -11497,7 +11497,7 @@
         <v>6531</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11658,7 +11658,7 @@
         <v>10908</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -11819,7 +11819,7 @@
         <v>33194</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -11980,7 +11980,7 @@
         <v>88077</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -12035,12 +12035,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -12201,7 +12201,7 @@
         <v>448.48865799999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -12362,7 +12362,7 @@
         <v>863.31579299999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -12523,7 +12523,7 @@
         <v>424.08659699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -12684,7 +12684,7 @@
         <v>49.649962000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -12845,7 +12845,7 @@
         <v>235.51133100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -13006,7 +13006,7 @@
         <v>961.98002299999996</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -13167,7 +13167,7 @@
         <v>764.98213299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -13328,38 +13328,38 @@
         <v>3748.0144969999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -13388,16 +13388,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
@@ -13454,7 +13454,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -13615,7 +13615,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -13776,12 +13776,12 @@
         <v>43093</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -13942,7 +13942,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -14103,7 +14103,7 @@
         <v>9513</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -14264,7 +14264,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -14425,7 +14425,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -14586,7 +14586,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -14747,7 +14747,7 @@
         <v>9414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -14908,7 +14908,7 @@
         <v>36964</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -15069,7 +15069,7 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -15124,12 +15124,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -15290,7 +15290,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -15451,7 +15451,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -15612,7 +15612,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -15773,7 +15773,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -15934,7 +15934,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -16095,7 +16095,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -16256,7 +16256,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -16417,38 +16417,38 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -16473,16 +16473,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
     <col min="53" max="53" width="9" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -16539,7 +16539,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16700,7 +16700,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -16862,12 +16862,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -17028,7 +17028,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -17189,7 +17189,7 @@
         <v>12729</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -17350,7 +17350,7 @@
         <v>16661</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -17511,7 +17511,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -17672,7 +17672,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -17833,7 +17833,7 @@
         <v>12175</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -17994,7 +17994,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -18155,7 +18155,7 @@
         <v>97169</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -18210,12 +18210,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -18376,7 +18376,7 @@
         <v>345.26898999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -18537,7 +18537,7 @@
         <v>1137.3429249999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -18698,7 +18698,7 @@
         <v>337.41420499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -18859,7 +18859,7 @@
         <v>40.33334</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -19020,7 +19020,7 @@
         <v>339.10771799999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -19181,7 +19181,7 @@
         <v>1247.683331</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -19342,7 +19342,7 @@
         <v>821.21724600000005</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -19503,38 +19503,38 @@
         <v>4268.3677550000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -19551,16 +19551,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -19617,7 +19617,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -19778,7 +19778,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -19940,12 +19940,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -20106,7 +20106,7 @@
         <v>5356</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -20267,7 +20267,7 @@
         <v>12576</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -20428,7 +20428,7 @@
         <v>17944</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -20589,7 +20589,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -20750,7 +20750,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -20911,7 +20911,7 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -21072,7 +21072,7 @@
         <v>38154</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -21233,7 +21233,7 @@
         <v>92789</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -21288,12 +21288,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -21454,7 +21454,7 @@
         <v>356.60756500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -21615,7 +21615,7 @@
         <v>977.829027</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -21776,7 +21776,7 @@
         <v>495.993199</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -21937,7 +21937,7 @@
         <v>37.412531000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -22098,7 +22098,7 @@
         <v>351.68923999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -22259,7 +22259,7 @@
         <v>888.50449000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -22420,7 +22420,7 @@
         <v>804.61703199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -22581,38 +22581,38 @@
         <v>3912.6530840000005</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -22629,17 +22629,17 @@
       <selection activeCell="A5" sqref="A5:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
@@ -22696,7 +22696,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -22860,7 +22860,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -23022,7 +23022,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -23186,12 +23186,12 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -23355,7 +23355,7 @@
         <v>6187</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -23519,7 +23519,7 @@
         <v>11221</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -23683,7 +23683,7 @@
         <v>16946</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -23847,7 +23847,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
@@ -24011,7 +24011,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -24175,7 +24175,7 @@
         <v>13026</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -24339,7 +24339,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -24503,7 +24503,7 @@
         <v>99721</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -24559,12 +24559,12 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -24728,7 +24728,7 @@
         <v>469.697947</v>
       </c>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -24892,7 +24892,7 @@
         <v>800.96283800000003</v>
       </c>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -25056,7 +25056,7 @@
         <v>463.52606100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
@@ -25220,7 +25220,7 @@
         <v>39.121160000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -25384,7 +25384,7 @@
         <v>320.92344600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -25548,7 +25548,7 @@
         <v>1254.2732289999999</v>
       </c>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -25712,7 +25712,7 @@
         <v>905.27916400000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -25876,38 +25876,38 @@
         <v>4253.7838449999999</v>
       </c>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -25928,16 +25928,16 @@
       <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
@@ -25994,7 +25994,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -26155,7 +26155,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -26317,12 +26317,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -26483,7 +26483,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -26644,7 +26644,7 @@
         <v>10430</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -26805,7 +26805,7 @@
         <v>15971</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -26966,7 +26966,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -27127,7 +27127,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -27288,7 +27288,7 @@
         <v>8618</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -27449,7 +27449,7 @@
         <v>34889</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -27610,7 +27610,7 @@
         <v>83267</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -27665,12 +27665,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -27831,7 +27831,7 @@
         <v>326.63437199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -27992,7 +27992,7 @@
         <v>710.31911300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -28153,7 +28153,7 @@
         <v>390.89581099999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -28314,7 +28314,7 @@
         <v>36.150655</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -28475,7 +28475,7 @@
         <v>232.43127799999999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -28636,7 +28636,7 @@
         <v>750.77748799999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -28797,7 +28797,7 @@
         <v>735.26635299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28958,40 +28958,40 @@
         <v>3182.4750699999995</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -29019,16 +29019,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -29085,7 +29085,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -29246,7 +29246,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -29408,12 +29408,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -29574,7 +29574,7 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -29735,7 +29735,7 @@
         <v>11045</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -29896,7 +29896,7 @@
         <v>14998</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -30057,7 +30057,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -30218,7 +30218,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -30379,7 +30379,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -30540,7 +30540,7 @@
         <v>31551</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -30701,7 +30701,7 @@
         <v>81088</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -30756,12 +30756,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -30922,7 +30922,7 @@
         <v>307.73157300000003</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -31083,7 +31083,7 @@
         <v>782.92677600000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -31244,7 +31244,7 @@
         <v>401.64126599999997</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -31405,7 +31405,7 @@
         <v>32.955354</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -31566,7 +31566,7 @@
         <v>272.11873100000003</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -31727,7 +31727,7 @@
         <v>976.60348099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -31888,7 +31888,7 @@
         <v>752.63757299999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -32049,40 +32049,40 @@
         <v>3526.6147539999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -32110,16 +32110,16 @@
       <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -32176,7 +32176,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -32337,7 +32337,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -32499,12 +32499,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -32665,7 +32665,7 @@
         <v>4413</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -32826,7 +32826,7 @@
         <v>11673</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -32987,7 +32987,7 @@
         <v>15590</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -33148,7 +33148,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -33309,7 +33309,7 @@
         <v>8134</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -33470,7 +33470,7 @@
         <v>9863</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -33631,7 +33631,7 @@
         <v>34066</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -33792,7 +33792,7 @@
         <v>86245</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -33847,12 +33847,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -34013,7 +34013,7 @@
         <v>298.50642199999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -34174,7 +34174,7 @@
         <v>888.297684</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -34335,7 +34335,7 @@
         <v>533.92582100000004</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -34496,7 +34496,7 @@
         <v>38.857964000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -34657,7 +34657,7 @@
         <v>364.61675700000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -34818,7 +34818,7 @@
         <v>992.76339499999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -34979,7 +34979,7 @@
         <v>755.640308</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -35140,40 +35140,40 @@
         <v>3872.6083509999999</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -35186,8 +35186,5 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GH ACTION Autorun Tue Jun  3 05:31:11 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A3F3B0F-71BD-4DE8-848F-7C480C598083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{614625A1-9704-44F0-8B6B-D6C5A2B10F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -971,16 +971,16 @@
       <selection pane="bottomRight" activeCell="O12" sqref="O12:X12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="9" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="9"/>
+    <col min="1" max="1" width="50.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="9" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -1359,12 +1359,12 @@
         <v>42365</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>6942</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>11626</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>12499</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>6294</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>81196</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2707,12 +2707,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>470.98508700000002</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>958.98562200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>296.27038100000027</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>48.659481</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>212.439166</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>901.73460399999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>700.69452899999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>3589.7688700000003</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -4025,19 +4025,19 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -4094,7 +4094,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -4417,12 +4417,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>5673</v>
       </c>
       <c r="W5" s="15">
-        <v>5878</v>
+        <v>5853</v>
       </c>
       <c r="X5" s="15">
         <v>5874</v>
@@ -4583,7 +4583,7 @@
         <v>4363</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>12114</v>
       </c>
       <c r="W6" s="15">
-        <v>11536</v>
+        <v>11500</v>
       </c>
       <c r="X6" s="15">
         <v>12095</v>
@@ -4744,7 +4744,7 @@
         <v>11478</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>17783</v>
       </c>
       <c r="W7" s="15">
-        <v>19726</v>
+        <v>19963</v>
       </c>
       <c r="X7" s="15">
         <v>18468</v>
@@ -4905,7 +4905,7 @@
         <v>16410</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -4973,7 +4973,7 @@
         <v>4497</v>
       </c>
       <c r="W8" s="15">
-        <v>4424</v>
+        <v>4306</v>
       </c>
       <c r="X8" s="15">
         <v>4571</v>
@@ -5066,7 +5066,7 @@
         <v>2807</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>7627</v>
       </c>
       <c r="W9" s="15">
-        <v>9176</v>
+        <v>9073</v>
       </c>
       <c r="X9" s="15">
         <v>7751</v>
@@ -5227,7 +5227,7 @@
         <v>8047</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>10329</v>
       </c>
       <c r="W10" s="15">
-        <v>10866</v>
+        <v>10896</v>
       </c>
       <c r="X10" s="15">
         <v>11250</v>
@@ -5388,7 +5388,7 @@
         <v>12133</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>45531</v>
       </c>
       <c r="W11" s="15">
-        <v>45937</v>
+        <v>45891</v>
       </c>
       <c r="X11" s="15">
         <v>43589</v>
@@ -5549,7 +5549,7 @@
         <v>29432</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>103554</v>
       </c>
       <c r="W12" s="7">
-        <v>107543</v>
+        <v>107482</v>
       </c>
       <c r="X12" s="7">
         <v>103598</v>
@@ -5710,7 +5710,7 @@
         <v>84670</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5765,12 +5765,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>425.25603100000001</v>
       </c>
       <c r="W15" s="15">
-        <v>430.20757600000002</v>
+        <v>429.16437500000001</v>
       </c>
       <c r="X15" s="15">
         <v>428.31920300000002</v>
@@ -5931,7 +5931,7 @@
         <v>303.44771800000001</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -5999,7 +5999,7 @@
         <v>867.05403999999999</v>
       </c>
       <c r="W16" s="15">
-        <v>784.34190000000001</v>
+        <v>783.65950199999997</v>
       </c>
       <c r="X16" s="15">
         <v>876.91632200000004</v>
@@ -6092,7 +6092,7 @@
         <v>868.11864300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -6160,7 +6160,7 @@
         <v>472.15919200000002</v>
       </c>
       <c r="W17" s="15">
-        <v>556.07526700000005</v>
+        <v>534.56419600000004</v>
       </c>
       <c r="X17" s="15">
         <v>646.64573700000005</v>
@@ -6253,7 +6253,7 @@
         <v>433.165955</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -6321,7 +6321,7 @@
         <v>64.714905999999999</v>
       </c>
       <c r="W18" s="15">
-        <v>66.278502000000003</v>
+        <v>62.198132000000001</v>
       </c>
       <c r="X18" s="15">
         <v>73.203108999999998</v>
@@ -6414,7 +6414,7 @@
         <v>42.773207999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -6482,7 +6482,7 @@
         <v>366.36616500000002</v>
       </c>
       <c r="W19" s="15">
-        <v>393.01427000000001</v>
+        <v>393.15206699999999</v>
       </c>
       <c r="X19" s="15">
         <v>332.23893800000002</v>
@@ -6575,7 +6575,7 @@
         <v>374.79168900000002</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -6643,7 +6643,7 @@
         <v>846.41466100000002</v>
       </c>
       <c r="W20" s="15">
-        <v>922.801649</v>
+        <v>925.26028399999996</v>
       </c>
       <c r="X20" s="15">
         <v>979.10364200000004</v>
@@ -6736,7 +6736,7 @@
         <v>1143.806075</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -6804,7 +6804,7 @@
         <v>1071.9282740000001</v>
       </c>
       <c r="W21" s="15">
-        <v>1063.811273</v>
+        <v>1063.907545</v>
       </c>
       <c r="X21" s="15">
         <v>1045.6775700000001</v>
@@ -6897,7 +6897,7 @@
         <v>657.70498399999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -6965,7 +6965,7 @@
         <v>4113.8932690000001</v>
       </c>
       <c r="W22" s="7">
-        <v>4216.5304370000003</v>
+        <v>4191.9061010000005</v>
       </c>
       <c r="X22" s="7">
         <v>4382.1045210000002</v>
@@ -7058,40 +7058,40 @@
         <v>3823.8082720000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -7104,9 +7104,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -7120,19 +7117,19 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="53" width="9.44140625" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.44140625" customWidth="1"/>
-    <col min="55" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="53" width="9.42578125" style="1" customWidth="1"/>
+    <col min="54" max="54" width="9.42578125" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>25</v>
       </c>
@@ -7189,7 +7186,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -7350,7 +7347,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -7512,13 +7509,13 @@
       </c>
       <c r="BB3" s="24"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -7586,7 +7583,7 @@
         <v>5646</v>
       </c>
       <c r="W5" s="15">
-        <v>0</v>
+        <v>5585</v>
       </c>
       <c r="X5" s="15">
         <v>0</v>
@@ -7680,7 +7677,7 @@
       </c>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -7748,7 +7745,7 @@
         <v>11471</v>
       </c>
       <c r="W6" s="6">
-        <v>0</v>
+        <v>11146</v>
       </c>
       <c r="X6" s="6">
         <v>0</v>
@@ -7842,7 +7839,7 @@
       </c>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -7910,7 +7907,7 @@
         <v>18630</v>
       </c>
       <c r="W7" s="6">
-        <v>0</v>
+        <v>19018</v>
       </c>
       <c r="X7" s="6">
         <v>0</v>
@@ -8004,7 +8001,7 @@
       </c>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -8072,7 +8069,7 @@
         <v>4133</v>
       </c>
       <c r="W8" s="6">
-        <v>0</v>
+        <v>3974</v>
       </c>
       <c r="X8" s="6">
         <v>0</v>
@@ -8166,7 +8163,7 @@
       </c>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -8234,7 +8231,7 @@
         <v>7557</v>
       </c>
       <c r="W9" s="6">
-        <v>0</v>
+        <v>8487</v>
       </c>
       <c r="X9" s="6">
         <v>0</v>
@@ -8328,7 +8325,7 @@
       </c>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -8396,7 +8393,7 @@
         <v>12746</v>
       </c>
       <c r="W10" s="15">
-        <v>0</v>
+        <v>12330</v>
       </c>
       <c r="X10" s="15">
         <v>0</v>
@@ -8490,7 +8487,7 @@
       </c>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -8558,7 +8555,7 @@
         <v>44186</v>
       </c>
       <c r="W11" s="6">
-        <v>0</v>
+        <v>48506</v>
       </c>
       <c r="X11" s="6">
         <v>0</v>
@@ -8652,7 +8649,7 @@
       </c>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -8720,7 +8717,7 @@
         <v>104369</v>
       </c>
       <c r="W12" s="7">
-        <v>0</v>
+        <v>109046</v>
       </c>
       <c r="X12" s="7">
         <v>0</v>
@@ -8814,7 +8811,7 @@
       </c>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -8870,13 +8867,13 @@
       <c r="BA13" s="6"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -8944,7 +8941,7 @@
         <v>404.07235600000001</v>
       </c>
       <c r="W15" s="15">
-        <v>0</v>
+        <v>400.02190300000001</v>
       </c>
       <c r="X15" s="15">
         <v>0</v>
@@ -9038,7 +9035,7 @@
       </c>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -9106,7 +9103,7 @@
         <v>790.26504399999999</v>
       </c>
       <c r="W16" s="6">
-        <v>0</v>
+        <v>777.18102799999997</v>
       </c>
       <c r="X16" s="6">
         <v>0</v>
@@ -9200,7 +9197,7 @@
       </c>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -9268,7 +9265,7 @@
         <v>587.69023500000003</v>
       </c>
       <c r="W17" s="6">
-        <v>0</v>
+        <v>624.11949100000004</v>
       </c>
       <c r="X17" s="6">
         <v>0</v>
@@ -9362,7 +9359,7 @@
       </c>
       <c r="BB17"/>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -9430,7 +9427,7 @@
         <v>56.712780000000002</v>
       </c>
       <c r="W18" s="6">
-        <v>0</v>
+        <v>64.680685999999994</v>
       </c>
       <c r="X18" s="6">
         <v>0</v>
@@ -9524,7 +9521,7 @@
       </c>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9592,7 +9589,7 @@
         <v>311.51239399999997</v>
       </c>
       <c r="W19" s="6">
-        <v>0</v>
+        <v>354.46993800000001</v>
       </c>
       <c r="X19" s="6">
         <v>0</v>
@@ -9686,7 +9683,7 @@
       </c>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -9754,7 +9751,7 @@
         <v>1151.7692930000001</v>
       </c>
       <c r="W20" s="15">
-        <v>0</v>
+        <v>1161.9312990000001</v>
       </c>
       <c r="X20" s="15">
         <v>0</v>
@@ -9848,7 +9845,7 @@
       </c>
       <c r="BB20"/>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -9916,7 +9913,7 @@
         <v>946.39353800000004</v>
       </c>
       <c r="W21" s="6">
-        <v>0</v>
+        <v>1104.5213160000001</v>
       </c>
       <c r="X21" s="6">
         <v>0</v>
@@ -10010,7 +10007,7 @@
       </c>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10078,7 +10075,7 @@
         <v>4248.4156400000002</v>
       </c>
       <c r="W22" s="7">
-        <v>0</v>
+        <v>4486.9256610000002</v>
       </c>
       <c r="X22" s="7">
         <v>0</v>
@@ -10172,100 +10169,100 @@
       </c>
       <c r="BB22"/>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="BB23"/>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB24"/>
     </row>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB25"/>
     </row>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB26"/>
     </row>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB27"/>
     </row>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB28"/>
     </row>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB29"/>
     </row>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB30"/>
     </row>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB31"/>
     </row>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB32"/>
     </row>
-    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB33"/>
     </row>
-    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB34"/>
     </row>
-    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB35"/>
     </row>
-    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB36"/>
     </row>
-    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB37"/>
     </row>
-    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB38"/>
     </row>
-    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB39"/>
     </row>
-    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB40"/>
     </row>
-    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB41"/>
     </row>
-    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB42"/>
     </row>
-    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB43"/>
     </row>
-    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB44"/>
     </row>
-    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB45"/>
     </row>
-    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB46"/>
     </row>
-    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB47"/>
     </row>
-    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB48"/>
     </row>
-    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB49"/>
     </row>
-    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB50"/>
     </row>
-    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB51"/>
     </row>
-    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB52"/>
     </row>
-    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB53"/>
     </row>
-    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB54"/>
     </row>
   </sheetData>
@@ -10298,16 +10295,16 @@
       <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="17" customWidth="1"/>
     <col min="53" max="53" width="9" style="17" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="17"/>
+    <col min="54" max="16384" width="6.7109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -10364,7 +10361,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -10525,7 +10522,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -10687,12 +10684,12 @@
       </c>
       <c r="BB3" s="23"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -10853,7 +10850,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -11014,7 +11011,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -11175,7 +11172,7 @@
         <v>15693</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -11336,7 +11333,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -11497,7 +11494,7 @@
         <v>6531</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11658,7 +11655,7 @@
         <v>10908</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -11819,7 +11816,7 @@
         <v>33194</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -11980,7 +11977,7 @@
         <v>88077</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -12035,12 +12032,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -12201,7 +12198,7 @@
         <v>448.48865799999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -12362,7 +12359,7 @@
         <v>863.31579299999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -12523,7 +12520,7 @@
         <v>424.08659699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -12684,7 +12681,7 @@
         <v>49.649962000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -12845,7 +12842,7 @@
         <v>235.51133100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -13006,7 +13003,7 @@
         <v>961.98002299999996</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -13167,7 +13164,7 @@
         <v>764.98213299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -13328,38 +13325,38 @@
         <v>3748.0144969999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -13388,16 +13385,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
@@ -13454,7 +13451,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -13615,7 +13612,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -13776,12 +13773,12 @@
         <v>43093</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -13942,7 +13939,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -14103,7 +14100,7 @@
         <v>9513</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -14264,7 +14261,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -14425,7 +14422,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -14586,7 +14583,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -14747,7 +14744,7 @@
         <v>9414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -14908,7 +14905,7 @@
         <v>36964</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -15069,7 +15066,7 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -15124,12 +15121,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -15290,7 +15287,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -15451,7 +15448,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -15612,7 +15609,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -15773,7 +15770,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -15934,7 +15931,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -16095,7 +16092,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -16256,7 +16253,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -16417,38 +16414,38 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -16473,16 +16470,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
     <col min="53" max="53" width="9" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -16539,7 +16536,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16700,7 +16697,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -16862,12 +16859,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -17028,7 +17025,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -17189,7 +17186,7 @@
         <v>12729</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -17350,7 +17347,7 @@
         <v>16661</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -17511,7 +17508,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -17672,7 +17669,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -17833,7 +17830,7 @@
         <v>12175</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -17994,7 +17991,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -18155,7 +18152,7 @@
         <v>97169</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -18210,12 +18207,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -18376,7 +18373,7 @@
         <v>345.26898999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -18537,7 +18534,7 @@
         <v>1137.3429249999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -18698,7 +18695,7 @@
         <v>337.41420499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -18859,7 +18856,7 @@
         <v>40.33334</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -19020,7 +19017,7 @@
         <v>339.10771799999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -19181,7 +19178,7 @@
         <v>1247.683331</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -19342,7 +19339,7 @@
         <v>821.21724600000005</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -19503,38 +19500,38 @@
         <v>4268.3677550000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -19551,16 +19548,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -19617,7 +19614,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -19778,7 +19775,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -19940,12 +19937,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -20106,7 +20103,7 @@
         <v>5356</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -20267,7 +20264,7 @@
         <v>12576</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -20428,7 +20425,7 @@
         <v>17944</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -20589,7 +20586,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -20750,7 +20747,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -20911,7 +20908,7 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -21072,7 +21069,7 @@
         <v>38154</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -21233,7 +21230,7 @@
         <v>92789</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -21288,12 +21285,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -21454,7 +21451,7 @@
         <v>356.60756500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -21615,7 +21612,7 @@
         <v>977.829027</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -21776,7 +21773,7 @@
         <v>495.993199</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -21937,7 +21934,7 @@
         <v>37.412531000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -22098,7 +22095,7 @@
         <v>351.68923999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -22259,7 +22256,7 @@
         <v>888.50449000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -22420,7 +22417,7 @@
         <v>804.61703199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -22581,38 +22578,38 @@
         <v>3912.6530840000005</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -22629,17 +22626,17 @@
       <selection activeCell="A5" sqref="A5:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
@@ -22696,7 +22693,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="23.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -22860,7 +22857,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -23022,7 +23019,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -23186,12 +23183,12 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -23355,7 +23352,7 @@
         <v>6187</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -23519,7 +23516,7 @@
         <v>11221</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -23683,7 +23680,7 @@
         <v>16946</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -23847,7 +23844,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
@@ -24011,7 +24008,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -24175,7 +24172,7 @@
         <v>13026</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -24339,7 +24336,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -24503,7 +24500,7 @@
         <v>99721</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -24559,12 +24556,12 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -24728,7 +24725,7 @@
         <v>469.697947</v>
       </c>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -24892,7 +24889,7 @@
         <v>800.96283800000003</v>
       </c>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -25056,7 +25053,7 @@
         <v>463.52606100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
@@ -25220,7 +25217,7 @@
         <v>39.121160000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -25384,7 +25381,7 @@
         <v>320.92344600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -25548,7 +25545,7 @@
         <v>1254.2732289999999</v>
       </c>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -25712,7 +25709,7 @@
         <v>905.27916400000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -25876,38 +25873,38 @@
         <v>4253.7838449999999</v>
       </c>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -25928,16 +25925,16 @@
       <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
@@ -25994,7 +25991,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -26155,7 +26152,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -26317,12 +26314,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -26483,7 +26480,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -26644,7 +26641,7 @@
         <v>10430</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -26805,7 +26802,7 @@
         <v>15971</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -26966,7 +26963,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -27127,7 +27124,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -27288,7 +27285,7 @@
         <v>8618</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -27449,7 +27446,7 @@
         <v>34889</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -27610,7 +27607,7 @@
         <v>83267</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -27665,12 +27662,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -27831,7 +27828,7 @@
         <v>326.63437199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -27992,7 +27989,7 @@
         <v>710.31911300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -28153,7 +28150,7 @@
         <v>390.89581099999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -28314,7 +28311,7 @@
         <v>36.150655</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -28475,7 +28472,7 @@
         <v>232.43127799999999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -28636,7 +28633,7 @@
         <v>750.77748799999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -28797,7 +28794,7 @@
         <v>735.26635299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28958,40 +28955,40 @@
         <v>3182.4750699999995</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -29019,16 +29016,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -29085,7 +29082,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -29246,7 +29243,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -29408,12 +29405,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -29574,7 +29571,7 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -29735,7 +29732,7 @@
         <v>11045</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -29896,7 +29893,7 @@
         <v>14998</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -30057,7 +30054,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -30218,7 +30215,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -30379,7 +30376,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -30540,7 +30537,7 @@
         <v>31551</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -30701,7 +30698,7 @@
         <v>81088</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -30756,12 +30753,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -30922,7 +30919,7 @@
         <v>307.73157300000003</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -31083,7 +31080,7 @@
         <v>782.92677600000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -31244,7 +31241,7 @@
         <v>401.64126599999997</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -31405,7 +31402,7 @@
         <v>32.955354</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -31566,7 +31563,7 @@
         <v>272.11873100000003</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -31727,7 +31724,7 @@
         <v>976.60348099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -31888,7 +31885,7 @@
         <v>752.63757299999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -32049,40 +32046,40 @@
         <v>3526.6147539999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -32110,16 +32107,16 @@
       <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -32176,7 +32173,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -32337,7 +32334,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -32499,12 +32496,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -32665,7 +32662,7 @@
         <v>4413</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -32826,7 +32823,7 @@
         <v>11673</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -32987,7 +32984,7 @@
         <v>15590</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -33148,7 +33145,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -33309,7 +33306,7 @@
         <v>8134</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -33470,7 +33467,7 @@
         <v>9863</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -33631,7 +33628,7 @@
         <v>34066</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -33792,7 +33789,7 @@
         <v>86245</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -33847,12 +33844,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -34013,7 +34010,7 @@
         <v>298.50642199999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -34174,7 +34171,7 @@
         <v>888.297684</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -34335,7 +34332,7 @@
         <v>533.92582100000004</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -34496,7 +34493,7 @@
         <v>38.857964000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -34657,7 +34654,7 @@
         <v>364.61675700000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -34818,7 +34815,7 @@
         <v>992.76339499999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -34979,7 +34976,7 @@
         <v>755.640308</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -35140,40 +35137,40 @@
         <v>3872.6083509999999</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Jun 10 05:31:42 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{614625A1-9704-44F0-8B6B-D6C5A2B10F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{360376F0-9384-432A-A790-EFB8A0840507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4025,7 +4025,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4493,7 +4493,7 @@
         <v>5853</v>
       </c>
       <c r="X5" s="15">
-        <v>5874</v>
+        <v>5846</v>
       </c>
       <c r="Y5" s="15">
         <v>5707</v>
@@ -4654,7 +4654,7 @@
         <v>11500</v>
       </c>
       <c r="X6" s="15">
-        <v>12095</v>
+        <v>12074</v>
       </c>
       <c r="Y6" s="15">
         <v>12546</v>
@@ -4815,7 +4815,7 @@
         <v>19963</v>
       </c>
       <c r="X7" s="15">
-        <v>18468</v>
+        <v>18878</v>
       </c>
       <c r="Y7" s="15">
         <v>17847</v>
@@ -4976,7 +4976,7 @@
         <v>4306</v>
       </c>
       <c r="X8" s="15">
-        <v>4571</v>
+        <v>4478</v>
       </c>
       <c r="Y8" s="15">
         <v>4645</v>
@@ -5298,7 +5298,7 @@
         <v>10896</v>
       </c>
       <c r="X10" s="15">
-        <v>11250</v>
+        <v>11223</v>
       </c>
       <c r="Y10" s="15">
         <v>11855</v>
@@ -5459,7 +5459,7 @@
         <v>45891</v>
       </c>
       <c r="X11" s="15">
-        <v>43589</v>
+        <v>43535</v>
       </c>
       <c r="Y11" s="15">
         <v>48765</v>
@@ -5620,7 +5620,7 @@
         <v>107482</v>
       </c>
       <c r="X12" s="7">
-        <v>103598</v>
+        <v>103785</v>
       </c>
       <c r="Y12" s="7">
         <v>111258</v>
@@ -5841,7 +5841,7 @@
         <v>429.16437500000001</v>
       </c>
       <c r="X15" s="15">
-        <v>428.31920300000002</v>
+        <v>427.53929099999999</v>
       </c>
       <c r="Y15" s="15">
         <v>435.25003800000002</v>
@@ -6002,7 +6002,7 @@
         <v>783.65950199999997</v>
       </c>
       <c r="X16" s="15">
-        <v>876.91632200000004</v>
+        <v>876.25199099999998</v>
       </c>
       <c r="Y16" s="15">
         <v>884.25497800000005</v>
@@ -6163,7 +6163,7 @@
         <v>534.56419600000004</v>
       </c>
       <c r="X17" s="15">
-        <v>646.64573700000005</v>
+        <v>640.87312799999995</v>
       </c>
       <c r="Y17" s="15">
         <v>566.83435699999995</v>
@@ -6324,7 +6324,7 @@
         <v>62.198132000000001</v>
       </c>
       <c r="X18" s="15">
-        <v>73.203108999999998</v>
+        <v>70.730726000000004</v>
       </c>
       <c r="Y18" s="15">
         <v>76.966457000000005</v>
@@ -6485,7 +6485,7 @@
         <v>393.15206699999999</v>
       </c>
       <c r="X19" s="15">
-        <v>332.23893800000002</v>
+        <v>331.97436800000003</v>
       </c>
       <c r="Y19" s="15">
         <v>414.18039399999998</v>
@@ -6646,7 +6646,7 @@
         <v>925.26028399999996</v>
       </c>
       <c r="X20" s="15">
-        <v>979.10364200000004</v>
+        <v>976.49057000000005</v>
       </c>
       <c r="Y20" s="15">
         <v>1044.429922</v>
@@ -6807,7 +6807,7 @@
         <v>1063.907545</v>
       </c>
       <c r="X21" s="15">
-        <v>1045.6775700000001</v>
+        <v>1044.940398</v>
       </c>
       <c r="Y21" s="15">
         <v>1148.5183999999999</v>
@@ -6968,7 +6968,7 @@
         <v>4191.9061010000005</v>
       </c>
       <c r="X22" s="7">
-        <v>4382.1045210000002</v>
+        <v>4368.8004719999999</v>
       </c>
       <c r="Y22" s="7">
         <v>4570.4345460000004</v>
@@ -7117,7 +7117,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7586,7 +7586,7 @@
         <v>5585</v>
       </c>
       <c r="X5" s="15">
-        <v>0</v>
+        <v>5274</v>
       </c>
       <c r="Y5" s="15">
         <v>0</v>
@@ -7748,7 +7748,7 @@
         <v>11146</v>
       </c>
       <c r="X6" s="6">
-        <v>0</v>
+        <v>12155</v>
       </c>
       <c r="Y6" s="6">
         <v>0</v>
@@ -7910,7 +7910,7 @@
         <v>19018</v>
       </c>
       <c r="X7" s="6">
-        <v>0</v>
+        <v>18685</v>
       </c>
       <c r="Y7" s="6">
         <v>0</v>
@@ -8072,7 +8072,7 @@
         <v>3974</v>
       </c>
       <c r="X8" s="6">
-        <v>0</v>
+        <v>4704</v>
       </c>
       <c r="Y8" s="6">
         <v>0</v>
@@ -8234,7 +8234,7 @@
         <v>8487</v>
       </c>
       <c r="X9" s="6">
-        <v>0</v>
+        <v>7980</v>
       </c>
       <c r="Y9" s="6">
         <v>0</v>
@@ -8396,7 +8396,7 @@
         <v>12330</v>
       </c>
       <c r="X10" s="15">
-        <v>0</v>
+        <v>13117</v>
       </c>
       <c r="Y10" s="15">
         <v>0</v>
@@ -8558,7 +8558,7 @@
         <v>48506</v>
       </c>
       <c r="X11" s="6">
-        <v>0</v>
+        <v>45218</v>
       </c>
       <c r="Y11" s="6">
         <v>0</v>
@@ -8720,7 +8720,7 @@
         <v>109046</v>
       </c>
       <c r="X12" s="7">
-        <v>0</v>
+        <v>107133</v>
       </c>
       <c r="Y12" s="7">
         <v>0</v>
@@ -8944,7 +8944,7 @@
         <v>400.02190300000001</v>
       </c>
       <c r="X15" s="15">
-        <v>0</v>
+        <v>393.33306399999998</v>
       </c>
       <c r="Y15" s="15">
         <v>0</v>
@@ -9106,7 +9106,7 @@
         <v>777.18102799999997</v>
       </c>
       <c r="X16" s="6">
-        <v>0</v>
+        <v>819.10305500000004</v>
       </c>
       <c r="Y16" s="6">
         <v>0</v>
@@ -9268,7 +9268,7 @@
         <v>624.11949100000004</v>
       </c>
       <c r="X17" s="6">
-        <v>0</v>
+        <v>603.64594899999997</v>
       </c>
       <c r="Y17" s="6">
         <v>0</v>
@@ -9430,7 +9430,7 @@
         <v>64.680685999999994</v>
       </c>
       <c r="X18" s="6">
-        <v>0</v>
+        <v>73.049284999999998</v>
       </c>
       <c r="Y18" s="6">
         <v>0</v>
@@ -9592,7 +9592,7 @@
         <v>354.46993800000001</v>
       </c>
       <c r="X19" s="6">
-        <v>0</v>
+        <v>350.85077100000001</v>
       </c>
       <c r="Y19" s="6">
         <v>0</v>
@@ -9754,7 +9754,7 @@
         <v>1161.9312990000001</v>
       </c>
       <c r="X20" s="15">
-        <v>0</v>
+        <v>1235.0265489999999</v>
       </c>
       <c r="Y20" s="15">
         <v>0</v>
@@ -9916,7 +9916,7 @@
         <v>1104.5213160000001</v>
       </c>
       <c r="X21" s="6">
-        <v>0</v>
+        <v>1054.44515</v>
       </c>
       <c r="Y21" s="6">
         <v>0</v>
@@ -10078,7 +10078,7 @@
         <v>4486.9256610000002</v>
       </c>
       <c r="X22" s="7">
-        <v>0</v>
+        <v>4529.4538229999998</v>
       </c>
       <c r="Y22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Jun 17 05:31:16 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{360376F0-9384-432A-A790-EFB8A0840507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC42BA5A-6A6F-4700-8AF3-C0E7D122F32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21285" yWindow="3870" windowWidth="24615" windowHeight="15885" tabRatio="591" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -4496,7 +4496,7 @@
         <v>5846</v>
       </c>
       <c r="Y5" s="15">
-        <v>5707</v>
+        <v>5684</v>
       </c>
       <c r="Z5" s="15">
         <v>5689</v>
@@ -4657,7 +4657,7 @@
         <v>12074</v>
       </c>
       <c r="Y6" s="15">
-        <v>12546</v>
+        <v>12533</v>
       </c>
       <c r="Z6" s="15">
         <v>12305</v>
@@ -4818,7 +4818,7 @@
         <v>18878</v>
       </c>
       <c r="Y7" s="15">
-        <v>17847</v>
+        <v>18214</v>
       </c>
       <c r="Z7" s="15">
         <v>17023</v>
@@ -4979,7 +4979,7 @@
         <v>4478</v>
       </c>
       <c r="Y8" s="15">
-        <v>4645</v>
+        <v>4634</v>
       </c>
       <c r="Z8" s="15">
         <v>4420</v>
@@ -5140,7 +5140,7 @@
         <v>7751</v>
       </c>
       <c r="Y9" s="15">
-        <v>9893</v>
+        <v>9664</v>
       </c>
       <c r="Z9" s="15">
         <v>9397</v>
@@ -5301,7 +5301,7 @@
         <v>11223</v>
       </c>
       <c r="Y10" s="15">
-        <v>11855</v>
+        <v>11866</v>
       </c>
       <c r="Z10" s="15">
         <v>11408</v>
@@ -5462,7 +5462,7 @@
         <v>43535</v>
       </c>
       <c r="Y11" s="15">
-        <v>48765</v>
+        <v>48701</v>
       </c>
       <c r="Z11" s="15">
         <v>44408</v>
@@ -5623,7 +5623,7 @@
         <v>103785</v>
       </c>
       <c r="Y12" s="7">
-        <v>111258</v>
+        <v>111296</v>
       </c>
       <c r="Z12" s="7">
         <v>104650</v>
@@ -5844,7 +5844,7 @@
         <v>427.53929099999999</v>
       </c>
       <c r="Y15" s="15">
-        <v>435.25003800000002</v>
+        <v>434.57279199999999</v>
       </c>
       <c r="Z15" s="15">
         <v>412.038387</v>
@@ -6005,7 +6005,7 @@
         <v>876.25199099999998</v>
       </c>
       <c r="Y16" s="15">
-        <v>884.25497800000005</v>
+        <v>884.46635300000003</v>
       </c>
       <c r="Z16" s="15">
         <v>828.28594899999996</v>
@@ -6166,7 +6166,7 @@
         <v>640.87312799999995</v>
       </c>
       <c r="Y17" s="15">
-        <v>566.83435699999995</v>
+        <v>566.32100200000002</v>
       </c>
       <c r="Z17" s="15">
         <v>567.27723700000001</v>
@@ -6327,7 +6327,7 @@
         <v>70.730726000000004</v>
       </c>
       <c r="Y18" s="15">
-        <v>76.966457000000005</v>
+        <v>76.783170999999996</v>
       </c>
       <c r="Z18" s="15">
         <v>77.346037999999993</v>
@@ -6488,7 +6488,7 @@
         <v>331.97436800000003</v>
       </c>
       <c r="Y19" s="15">
-        <v>414.18039399999998</v>
+        <v>413.39020900000003</v>
       </c>
       <c r="Z19" s="15">
         <v>440.194614</v>
@@ -6649,7 +6649,7 @@
         <v>976.49057000000005</v>
       </c>
       <c r="Y20" s="15">
-        <v>1044.429922</v>
+        <v>1045.092179</v>
       </c>
       <c r="Z20" s="15">
         <v>1000.158154</v>
@@ -6810,7 +6810,7 @@
         <v>1044.940398</v>
       </c>
       <c r="Y21" s="15">
-        <v>1148.5183999999999</v>
+        <v>1147.4865970000001</v>
       </c>
       <c r="Z21" s="15">
         <v>1025.8774169999999</v>
@@ -6971,7 +6971,7 @@
         <v>4368.8004719999999</v>
       </c>
       <c r="Y22" s="7">
-        <v>4570.4345460000004</v>
+        <v>4568.1123029999999</v>
       </c>
       <c r="Z22" s="7">
         <v>4351.177795999999</v>
@@ -7117,7 +7117,7 @@
       <selection activeCell="B3" sqref="B3:BB3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7589,7 +7589,7 @@
         <v>5274</v>
       </c>
       <c r="Y5" s="15">
-        <v>0</v>
+        <v>5376</v>
       </c>
       <c r="Z5" s="15">
         <v>0</v>
@@ -7751,7 +7751,7 @@
         <v>12155</v>
       </c>
       <c r="Y6" s="6">
-        <v>0</v>
+        <v>12375</v>
       </c>
       <c r="Z6" s="6">
         <v>0</v>
@@ -7913,7 +7913,7 @@
         <v>18685</v>
       </c>
       <c r="Y7" s="6">
-        <v>0</v>
+        <v>16698</v>
       </c>
       <c r="Z7" s="6">
         <v>0</v>
@@ -8075,7 +8075,7 @@
         <v>4704</v>
       </c>
       <c r="Y8" s="6">
-        <v>0</v>
+        <v>4647</v>
       </c>
       <c r="Z8" s="6">
         <v>0</v>
@@ -8237,7 +8237,7 @@
         <v>7980</v>
       </c>
       <c r="Y9" s="6">
-        <v>0</v>
+        <v>9164</v>
       </c>
       <c r="Z9" s="6">
         <v>0</v>
@@ -8399,7 +8399,7 @@
         <v>13117</v>
       </c>
       <c r="Y10" s="15">
-        <v>0</v>
+        <v>13038</v>
       </c>
       <c r="Z10" s="15">
         <v>0</v>
@@ -8561,7 +8561,7 @@
         <v>45218</v>
       </c>
       <c r="Y11" s="6">
-        <v>0</v>
+        <v>44431</v>
       </c>
       <c r="Z11" s="6">
         <v>0</v>
@@ -8723,7 +8723,7 @@
         <v>107133</v>
       </c>
       <c r="Y12" s="7">
-        <v>0</v>
+        <v>105729</v>
       </c>
       <c r="Z12" s="7">
         <v>0</v>
@@ -8947,7 +8947,7 @@
         <v>393.33306399999998</v>
       </c>
       <c r="Y15" s="15">
-        <v>0</v>
+        <v>389.06172500000002</v>
       </c>
       <c r="Z15" s="15">
         <v>0</v>
@@ -9109,7 +9109,7 @@
         <v>819.10305500000004</v>
       </c>
       <c r="Y16" s="6">
-        <v>0</v>
+        <v>849.25950899999998</v>
       </c>
       <c r="Z16" s="6">
         <v>0</v>
@@ -9271,7 +9271,7 @@
         <v>603.64594899999997</v>
       </c>
       <c r="Y17" s="6">
-        <v>0</v>
+        <v>491.91313100000002</v>
       </c>
       <c r="Z17" s="6">
         <v>0</v>
@@ -9433,7 +9433,7 @@
         <v>73.049284999999998</v>
       </c>
       <c r="Y18" s="6">
-        <v>0</v>
+        <v>71.354965000000007</v>
       </c>
       <c r="Z18" s="6">
         <v>0</v>
@@ -9595,7 +9595,7 @@
         <v>350.85077100000001</v>
       </c>
       <c r="Y19" s="6">
-        <v>0</v>
+        <v>362.07414999999997</v>
       </c>
       <c r="Z19" s="6">
         <v>0</v>
@@ -9757,7 +9757,7 @@
         <v>1235.0265489999999</v>
       </c>
       <c r="Y20" s="15">
-        <v>0</v>
+        <v>1143.941202</v>
       </c>
       <c r="Z20" s="15">
         <v>0</v>
@@ -9919,7 +9919,7 @@
         <v>1054.44515</v>
       </c>
       <c r="Y21" s="6">
-        <v>0</v>
+        <v>973.018777</v>
       </c>
       <c r="Z21" s="6">
         <v>0</v>
@@ -10081,7 +10081,7 @@
         <v>4529.4538229999998</v>
       </c>
       <c r="Y22" s="7">
-        <v>0</v>
+        <v>4280.6234590000004</v>
       </c>
       <c r="Z22" s="7">
         <v>0</v>
@@ -10277,9 +10277,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Jun 24 05:32:08 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC42BA5A-6A6F-4700-8AF3-C0E7D122F32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1965C6F-2E77-4006-8AD2-96F4CD930D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21285" yWindow="3870" windowWidth="24615" windowHeight="15885" tabRatio="591" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -4022,10 +4022,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection activeCell="E35" sqref="E35"/>
+      <selection pane="topRight" activeCell="E35" sqref="E35"/>
+      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
+      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7104,6 +7104,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -7114,10 +7117,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="J34" sqref="J34"/>
+      <selection activeCell="F30" sqref="F30"/>
+      <selection pane="topRight" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7592,7 +7595,7 @@
         <v>5376</v>
       </c>
       <c r="Z5" s="15">
-        <v>0</v>
+        <v>5179</v>
       </c>
       <c r="AA5" s="15">
         <v>0</v>
@@ -7754,7 +7757,7 @@
         <v>12375</v>
       </c>
       <c r="Z6" s="6">
-        <v>0</v>
+        <v>12363</v>
       </c>
       <c r="AA6" s="6">
         <v>0</v>
@@ -7916,7 +7919,7 @@
         <v>16698</v>
       </c>
       <c r="Z7" s="6">
-        <v>0</v>
+        <v>17440</v>
       </c>
       <c r="AA7" s="6">
         <v>0</v>
@@ -8078,7 +8081,7 @@
         <v>4647</v>
       </c>
       <c r="Z8" s="6">
-        <v>0</v>
+        <v>5050</v>
       </c>
       <c r="AA8" s="6">
         <v>0</v>
@@ -8240,7 +8243,7 @@
         <v>9164</v>
       </c>
       <c r="Z9" s="6">
-        <v>0</v>
+        <v>8266</v>
       </c>
       <c r="AA9" s="6">
         <v>0</v>
@@ -8402,7 +8405,7 @@
         <v>13038</v>
       </c>
       <c r="Z10" s="15">
-        <v>0</v>
+        <v>13007</v>
       </c>
       <c r="AA10" s="15">
         <v>0</v>
@@ -8564,7 +8567,7 @@
         <v>44431</v>
       </c>
       <c r="Z11" s="6">
-        <v>0</v>
+        <v>46886</v>
       </c>
       <c r="AA11" s="6">
         <v>0</v>
@@ -8726,7 +8729,7 @@
         <v>105729</v>
       </c>
       <c r="Z12" s="7">
-        <v>0</v>
+        <v>108191</v>
       </c>
       <c r="AA12" s="7">
         <v>0</v>
@@ -8950,7 +8953,7 @@
         <v>389.06172500000002</v>
       </c>
       <c r="Z15" s="15">
-        <v>0</v>
+        <v>375.520625</v>
       </c>
       <c r="AA15" s="15">
         <v>0</v>
@@ -9112,7 +9115,7 @@
         <v>849.25950899999998</v>
       </c>
       <c r="Z16" s="6">
-        <v>0</v>
+        <v>867.88953500000002</v>
       </c>
       <c r="AA16" s="6">
         <v>0</v>
@@ -9274,7 +9277,7 @@
         <v>491.91313100000002</v>
       </c>
       <c r="Z17" s="6">
-        <v>0</v>
+        <v>526.64351699999997</v>
       </c>
       <c r="AA17" s="6">
         <v>0</v>
@@ -9436,7 +9439,7 @@
         <v>71.354965000000007</v>
       </c>
       <c r="Z18" s="6">
-        <v>0</v>
+        <v>77.908767999999995</v>
       </c>
       <c r="AA18" s="6">
         <v>0</v>
@@ -9598,7 +9601,7 @@
         <v>362.07414999999997</v>
       </c>
       <c r="Z19" s="6">
-        <v>0</v>
+        <v>347.86033300000003</v>
       </c>
       <c r="AA19" s="6">
         <v>0</v>
@@ -9760,7 +9763,7 @@
         <v>1143.941202</v>
       </c>
       <c r="Z20" s="15">
-        <v>0</v>
+        <v>1120.9541850000001</v>
       </c>
       <c r="AA20" s="15">
         <v>0</v>
@@ -9922,7 +9925,7 @@
         <v>973.018777</v>
       </c>
       <c r="Z21" s="6">
-        <v>0</v>
+        <v>1075.3979440000001</v>
       </c>
       <c r="AA21" s="6">
         <v>0</v>
@@ -10084,7 +10087,7 @@
         <v>4280.6234590000004</v>
       </c>
       <c r="Z22" s="7">
-        <v>0</v>
+        <v>4392.1749069999996</v>
       </c>
       <c r="AA22" s="7">
         <v>0</v>
@@ -10277,6 +10280,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Jul  1 05:34:14 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1965C6F-2E77-4006-8AD2-96F4CD930D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B325698-5757-4DCB-B90E-7A66B04E5BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="591" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -971,16 +971,16 @@
       <selection pane="bottomRight" activeCell="O12" sqref="O12:X12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="9" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="9"/>
+    <col min="1" max="1" width="50.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.453125" style="9" customWidth="1"/>
+    <col min="53" max="53" width="9.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7265625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="23" x14ac:dyDescent="0.5">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -1359,12 +1359,12 @@
         <v>42365</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>6942</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>11626</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>12499</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>6294</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>81196</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2707,12 +2707,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>470.98508700000002</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>958.98562200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>296.27038100000027</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>48.659481</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>212.439166</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>901.73460399999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>700.69452899999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>3589.7688700000003</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -4022,22 +4022,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="E35" sqref="E35"/>
-      <selection pane="topRight" activeCell="E35" sqref="E35"/>
-      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
-      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -4094,7 +4094,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -4417,12 +4417,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4499,10 +4499,10 @@
         <v>5684</v>
       </c>
       <c r="Z5" s="15">
-        <v>5689</v>
+        <v>5673</v>
       </c>
       <c r="AA5" s="15">
-        <v>5733</v>
+        <v>5706</v>
       </c>
       <c r="AB5" s="15">
         <v>5546</v>
@@ -4583,7 +4583,7 @@
         <v>4363</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4660,10 +4660,10 @@
         <v>12533</v>
       </c>
       <c r="Z6" s="15">
-        <v>12305</v>
+        <v>12213</v>
       </c>
       <c r="AA6" s="15">
-        <v>13008</v>
+        <v>12954</v>
       </c>
       <c r="AB6" s="15">
         <v>12606</v>
@@ -4744,7 +4744,7 @@
         <v>11478</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -4821,10 +4821,10 @@
         <v>18214</v>
       </c>
       <c r="Z7" s="15">
-        <v>17023</v>
+        <v>17455</v>
       </c>
       <c r="AA7" s="15">
-        <v>19698</v>
+        <v>20139</v>
       </c>
       <c r="AB7" s="15">
         <v>20735</v>
@@ -4905,7 +4905,7 @@
         <v>16410</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -4982,10 +4982,10 @@
         <v>4634</v>
       </c>
       <c r="Z8" s="15">
-        <v>4420</v>
+        <v>4407</v>
       </c>
       <c r="AA8" s="15">
-        <v>4395</v>
+        <v>4357</v>
       </c>
       <c r="AB8" s="15">
         <v>3159</v>
@@ -5066,7 +5066,7 @@
         <v>2807</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -5143,10 +5143,10 @@
         <v>9664</v>
       </c>
       <c r="Z9" s="15">
-        <v>9397</v>
+        <v>9395</v>
       </c>
       <c r="AA9" s="15">
-        <v>9765</v>
+        <v>9782</v>
       </c>
       <c r="AB9" s="15">
         <v>9374</v>
@@ -5227,7 +5227,7 @@
         <v>8047</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -5304,10 +5304,10 @@
         <v>11866</v>
       </c>
       <c r="Z10" s="15">
-        <v>11408</v>
+        <v>11411</v>
       </c>
       <c r="AA10" s="15">
-        <v>11550</v>
+        <v>11569</v>
       </c>
       <c r="AB10" s="15">
         <v>12538</v>
@@ -5388,7 +5388,7 @@
         <v>12133</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -5465,10 +5465,10 @@
         <v>48701</v>
       </c>
       <c r="Z11" s="15">
-        <v>44408</v>
+        <v>44353</v>
       </c>
       <c r="AA11" s="15">
-        <v>42134</v>
+        <v>42029</v>
       </c>
       <c r="AB11" s="15">
         <v>41801</v>
@@ -5549,7 +5549,7 @@
         <v>29432</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -5626,10 +5626,10 @@
         <v>111296</v>
       </c>
       <c r="Z12" s="7">
-        <v>104650</v>
+        <v>104907</v>
       </c>
       <c r="AA12" s="7">
-        <v>106283</v>
+        <v>106536</v>
       </c>
       <c r="AB12" s="7">
         <v>105759</v>
@@ -5710,7 +5710,7 @@
         <v>84670</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5765,12 +5765,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -5847,10 +5847,10 @@
         <v>434.57279199999999</v>
       </c>
       <c r="Z15" s="15">
-        <v>412.038387</v>
+        <v>411.32436300000001</v>
       </c>
       <c r="AA15" s="15">
-        <v>415.20696900000002</v>
+        <v>413.00203800000003</v>
       </c>
       <c r="AB15" s="15">
         <v>386.429464</v>
@@ -5931,7 +5931,7 @@
         <v>303.44771800000001</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -6008,10 +6008,10 @@
         <v>884.46635300000003</v>
       </c>
       <c r="Z16" s="15">
-        <v>828.28594899999996</v>
+        <v>827.82538299999999</v>
       </c>
       <c r="AA16" s="15">
-        <v>961.30262000000005</v>
+        <v>961.01767400000006</v>
       </c>
       <c r="AB16" s="15">
         <v>868.32915100000002</v>
@@ -6092,7 +6092,7 @@
         <v>868.11864300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -6169,10 +6169,10 @@
         <v>566.32100200000002</v>
       </c>
       <c r="Z17" s="15">
-        <v>567.27723700000001</v>
+        <v>567.06766600000003</v>
       </c>
       <c r="AA17" s="15">
-        <v>664.89642300000003</v>
+        <v>664.18505400000004</v>
       </c>
       <c r="AB17" s="15">
         <v>660.70479899999998</v>
@@ -6253,7 +6253,7 @@
         <v>433.165955</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -6330,10 +6330,10 @@
         <v>76.783170999999996</v>
       </c>
       <c r="Z18" s="15">
-        <v>77.346037999999993</v>
+        <v>76.884073999999998</v>
       </c>
       <c r="AA18" s="15">
-        <v>73.828400000000002</v>
+        <v>72.687977000000004</v>
       </c>
       <c r="AB18" s="15">
         <v>61.666522999999998</v>
@@ -6414,7 +6414,7 @@
         <v>42.773207999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -6491,10 +6491,10 @@
         <v>413.39020900000003</v>
       </c>
       <c r="Z19" s="15">
-        <v>440.194614</v>
+        <v>440.08693599999998</v>
       </c>
       <c r="AA19" s="15">
-        <v>408.29897299999999</v>
+        <v>409.32937700000002</v>
       </c>
       <c r="AB19" s="15">
         <v>404.12152400000002</v>
@@ -6575,7 +6575,7 @@
         <v>374.79168900000002</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -6652,10 +6652,10 @@
         <v>1045.092179</v>
       </c>
       <c r="Z20" s="15">
-        <v>1000.158154</v>
+        <v>1000.6794</v>
       </c>
       <c r="AA20" s="15">
-        <v>1073.834382</v>
+        <v>1074.925176</v>
       </c>
       <c r="AB20" s="15">
         <v>1181.8938250000001</v>
@@ -6736,7 +6736,7 @@
         <v>1143.806075</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -6813,10 +6813,10 @@
         <v>1147.4865970000001</v>
       </c>
       <c r="Z21" s="15">
-        <v>1025.8774169999999</v>
+        <v>1025.0984249999999</v>
       </c>
       <c r="AA21" s="15">
-        <v>983.45082600000001</v>
+        <v>982.654223</v>
       </c>
       <c r="AB21" s="15">
         <v>952.284626</v>
@@ -6897,7 +6897,7 @@
         <v>657.70498399999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -6974,10 +6974,10 @@
         <v>4568.1123029999999</v>
       </c>
       <c r="Z22" s="7">
-        <v>4351.177795999999</v>
+        <v>4348.9662470000003</v>
       </c>
       <c r="AA22" s="7">
-        <v>4580.818593</v>
+        <v>4577.8015190000006</v>
       </c>
       <c r="AB22" s="7">
         <v>4515.4299119999996</v>
@@ -7058,40 +7058,40 @@
         <v>3823.8082720000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -7104,9 +7104,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -7117,22 +7114,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="F30" sqref="F30"/>
-      <selection pane="topRight" activeCell="F30" sqref="F30"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
-      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" sqref="A1:BA1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="53" width="9.42578125" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.42578125" customWidth="1"/>
-    <col min="55" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
+    <col min="3" max="53" width="9.453125" style="1" customWidth="1"/>
+    <col min="54" max="54" width="9.453125" customWidth="1"/>
+    <col min="55" max="16384" width="6.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
       <c r="A1" s="26" t="s">
         <v>25</v>
       </c>
@@ -7189,7 +7186,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -7350,7 +7347,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -7512,13 +7509,13 @@
       </c>
       <c r="BB3" s="24"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -7598,7 +7595,7 @@
         <v>5179</v>
       </c>
       <c r="AA5" s="15">
-        <v>0</v>
+        <v>5080</v>
       </c>
       <c r="AB5" s="15">
         <v>0</v>
@@ -7680,7 +7677,7 @@
       </c>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -7760,7 +7757,7 @@
         <v>12363</v>
       </c>
       <c r="AA6" s="6">
-        <v>0</v>
+        <v>11640</v>
       </c>
       <c r="AB6" s="6">
         <v>0</v>
@@ -7842,7 +7839,7 @@
       </c>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -7922,7 +7919,7 @@
         <v>17440</v>
       </c>
       <c r="AA7" s="6">
-        <v>0</v>
+        <v>17821</v>
       </c>
       <c r="AB7" s="6">
         <v>0</v>
@@ -8004,7 +8001,7 @@
       </c>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -8084,7 +8081,7 @@
         <v>5050</v>
       </c>
       <c r="AA8" s="6">
-        <v>0</v>
+        <v>4424</v>
       </c>
       <c r="AB8" s="6">
         <v>0</v>
@@ -8166,7 +8163,7 @@
       </c>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -8246,7 +8243,7 @@
         <v>8266</v>
       </c>
       <c r="AA9" s="6">
-        <v>0</v>
+        <v>8710</v>
       </c>
       <c r="AB9" s="6">
         <v>0</v>
@@ -8328,7 +8325,7 @@
       </c>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -8408,7 +8405,7 @@
         <v>13007</v>
       </c>
       <c r="AA10" s="15">
-        <v>0</v>
+        <v>11858</v>
       </c>
       <c r="AB10" s="15">
         <v>0</v>
@@ -8490,7 +8487,7 @@
       </c>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -8570,7 +8567,7 @@
         <v>46886</v>
       </c>
       <c r="AA11" s="6">
-        <v>0</v>
+        <v>48315</v>
       </c>
       <c r="AB11" s="6">
         <v>0</v>
@@ -8652,7 +8649,7 @@
       </c>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -8732,7 +8729,7 @@
         <v>108191</v>
       </c>
       <c r="AA12" s="7">
-        <v>0</v>
+        <v>107848</v>
       </c>
       <c r="AB12" s="7">
         <v>0</v>
@@ -8814,7 +8811,7 @@
       </c>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -8870,13 +8867,13 @@
       <c r="BA13" s="6"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -8956,7 +8953,7 @@
         <v>375.520625</v>
       </c>
       <c r="AA15" s="15">
-        <v>0</v>
+        <v>365.78277000000003</v>
       </c>
       <c r="AB15" s="15">
         <v>0</v>
@@ -9038,7 +9035,7 @@
       </c>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -9118,7 +9115,7 @@
         <v>867.88953500000002</v>
       </c>
       <c r="AA16" s="6">
-        <v>0</v>
+        <v>797.54447000000005</v>
       </c>
       <c r="AB16" s="6">
         <v>0</v>
@@ -9200,7 +9197,7 @@
       </c>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -9280,7 +9277,7 @@
         <v>526.64351699999997</v>
       </c>
       <c r="AA17" s="6">
-        <v>0</v>
+        <v>557.70666600000004</v>
       </c>
       <c r="AB17" s="6">
         <v>0</v>
@@ -9362,7 +9359,7 @@
       </c>
       <c r="BB17"/>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -9442,7 +9439,7 @@
         <v>77.908767999999995</v>
       </c>
       <c r="AA18" s="6">
-        <v>0</v>
+        <v>65.075076999999993</v>
       </c>
       <c r="AB18" s="6">
         <v>0</v>
@@ -9524,7 +9521,7 @@
       </c>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9604,7 +9601,7 @@
         <v>347.86033300000003</v>
       </c>
       <c r="AA19" s="6">
-        <v>0</v>
+        <v>341.69426499999997</v>
       </c>
       <c r="AB19" s="6">
         <v>0</v>
@@ -9686,7 +9683,7 @@
       </c>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -9766,7 +9763,7 @@
         <v>1120.9541850000001</v>
       </c>
       <c r="AA20" s="15">
-        <v>0</v>
+        <v>1072.4095500000001</v>
       </c>
       <c r="AB20" s="15">
         <v>0</v>
@@ -9848,7 +9845,7 @@
       </c>
       <c r="BB20"/>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -9928,7 +9925,7 @@
         <v>1075.3979440000001</v>
       </c>
       <c r="AA21" s="6">
-        <v>0</v>
+        <v>1107.0549920000001</v>
       </c>
       <c r="AB21" s="6">
         <v>0</v>
@@ -10010,7 +10007,7 @@
       </c>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10090,7 +10087,7 @@
         <v>4392.1749069999996</v>
       </c>
       <c r="AA22" s="7">
-        <v>0</v>
+        <v>4307.2677900000008</v>
       </c>
       <c r="AB22" s="7">
         <v>0</v>
@@ -10172,100 +10169,100 @@
       </c>
       <c r="BB22"/>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="BB23"/>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB24"/>
     </row>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB25"/>
     </row>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB26"/>
     </row>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB27"/>
     </row>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB28"/>
     </row>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB29"/>
     </row>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB30"/>
     </row>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB31"/>
     </row>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB32"/>
     </row>
-    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB33"/>
     </row>
-    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB34"/>
     </row>
-    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB35"/>
     </row>
-    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB36"/>
     </row>
-    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB37"/>
     </row>
-    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB38"/>
     </row>
-    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB39"/>
     </row>
-    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB40"/>
     </row>
-    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB41"/>
     </row>
-    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB42"/>
     </row>
-    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB43"/>
     </row>
-    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB44"/>
     </row>
-    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB45"/>
     </row>
-    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB46"/>
     </row>
-    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB47"/>
     </row>
-    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB48"/>
     </row>
-    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB49"/>
     </row>
-    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB50"/>
     </row>
-    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB51"/>
     </row>
-    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB52"/>
     </row>
-    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB53"/>
     </row>
-    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB54"/>
     </row>
   </sheetData>
@@ -10280,9 +10277,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -10298,16 +10292,16 @@
       <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="50.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.453125" style="17" customWidth="1"/>
     <col min="53" max="53" width="9" style="17" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="17"/>
+    <col min="54" max="16384" width="6.7265625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -10364,7 +10358,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -10525,7 +10519,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -10687,12 +10681,12 @@
       </c>
       <c r="BB3" s="23"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -10853,7 +10847,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -11014,7 +11008,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -11175,7 +11169,7 @@
         <v>15693</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -11336,7 +11330,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -11497,7 +11491,7 @@
         <v>6531</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11658,7 +11652,7 @@
         <v>10908</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -11819,7 +11813,7 @@
         <v>33194</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -11980,7 +11974,7 @@
         <v>88077</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -12035,12 +12029,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -12201,7 +12195,7 @@
         <v>448.48865799999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -12362,7 +12356,7 @@
         <v>863.31579299999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -12523,7 +12517,7 @@
         <v>424.08659699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -12684,7 +12678,7 @@
         <v>49.649962000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -12845,7 +12839,7 @@
         <v>235.51133100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -13006,7 +13000,7 @@
         <v>961.98002299999996</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -13167,7 +13161,7 @@
         <v>764.98213299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -13328,38 +13322,38 @@
         <v>3748.0144969999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -13388,16 +13382,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="23" x14ac:dyDescent="0.5">
       <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
@@ -13454,7 +13448,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -13615,7 +13609,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -13776,12 +13770,12 @@
         <v>43093</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -13942,7 +13936,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -14103,7 +14097,7 @@
         <v>9513</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -14264,7 +14258,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -14425,7 +14419,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -14586,7 +14580,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -14747,7 +14741,7 @@
         <v>9414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -14908,7 +14902,7 @@
         <v>36964</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -15069,7 +15063,7 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -15124,12 +15118,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -15290,7 +15284,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -15451,7 +15445,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -15612,7 +15606,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -15773,7 +15767,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -15934,7 +15928,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -16095,7 +16089,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -16256,7 +16250,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -16417,38 +16411,38 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -16473,16 +16467,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
     <col min="53" max="53" width="9" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="54" max="16384" width="6.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -16539,7 +16533,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16700,7 +16694,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -16862,12 +16856,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -17028,7 +17022,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -17189,7 +17183,7 @@
         <v>12729</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -17350,7 +17344,7 @@
         <v>16661</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -17511,7 +17505,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -17672,7 +17666,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -17833,7 +17827,7 @@
         <v>12175</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -17994,7 +17988,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -18155,7 +18149,7 @@
         <v>97169</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -18210,12 +18204,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -18376,7 +18370,7 @@
         <v>345.26898999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -18537,7 +18531,7 @@
         <v>1137.3429249999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -18698,7 +18692,7 @@
         <v>337.41420499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -18859,7 +18853,7 @@
         <v>40.33334</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -19020,7 +19014,7 @@
         <v>339.10771799999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -19181,7 +19175,7 @@
         <v>1247.683331</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -19342,7 +19336,7 @@
         <v>821.21724600000005</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -19503,38 +19497,38 @@
         <v>4268.3677550000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -19551,16 +19545,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -19617,7 +19611,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -19778,7 +19772,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -19940,12 +19934,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -20106,7 +20100,7 @@
         <v>5356</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -20267,7 +20261,7 @@
         <v>12576</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -20428,7 +20422,7 @@
         <v>17944</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -20589,7 +20583,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -20750,7 +20744,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -20911,7 +20905,7 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -21072,7 +21066,7 @@
         <v>38154</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -21233,7 +21227,7 @@
         <v>92789</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -21288,12 +21282,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -21454,7 +21448,7 @@
         <v>356.60756500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -21615,7 +21609,7 @@
         <v>977.829027</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -21776,7 +21770,7 @@
         <v>495.993199</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -21937,7 +21931,7 @@
         <v>37.412531000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -22098,7 +22092,7 @@
         <v>351.68923999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -22259,7 +22253,7 @@
         <v>888.50449000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -22420,7 +22414,7 @@
         <v>804.61703199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -22581,38 +22575,38 @@
         <v>3912.6530840000005</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -22629,17 +22623,17 @@
       <selection activeCell="A5" sqref="A5:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="6.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
       <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
@@ -22696,7 +22690,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" ht="23" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -22860,7 +22854,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -23022,7 +23016,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -23186,12 +23180,12 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -23355,7 +23349,7 @@
         <v>6187</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -23519,7 +23513,7 @@
         <v>11221</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -23683,7 +23677,7 @@
         <v>16946</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -23847,7 +23841,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
@@ -24011,7 +24005,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -24175,7 +24169,7 @@
         <v>13026</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -24339,7 +24333,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -24503,7 +24497,7 @@
         <v>99721</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -24559,12 +24553,12 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -24728,7 +24722,7 @@
         <v>469.697947</v>
       </c>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -24892,7 +24886,7 @@
         <v>800.96283800000003</v>
       </c>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -25056,7 +25050,7 @@
         <v>463.52606100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
@@ -25220,7 +25214,7 @@
         <v>39.121160000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -25384,7 +25378,7 @@
         <v>320.92344600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -25548,7 +25542,7 @@
         <v>1254.2732289999999</v>
       </c>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -25712,7 +25706,7 @@
         <v>905.27916400000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -25876,38 +25870,38 @@
         <v>4253.7838449999999</v>
       </c>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -25928,16 +25922,16 @@
       <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
@@ -25994,7 +25988,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -26155,7 +26149,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -26317,12 +26311,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -26483,7 +26477,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -26644,7 +26638,7 @@
         <v>10430</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -26805,7 +26799,7 @@
         <v>15971</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -26966,7 +26960,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -27127,7 +27121,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -27288,7 +27282,7 @@
         <v>8618</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -27449,7 +27443,7 @@
         <v>34889</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -27610,7 +27604,7 @@
         <v>83267</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -27665,12 +27659,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -27831,7 +27825,7 @@
         <v>326.63437199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -27992,7 +27986,7 @@
         <v>710.31911300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -28153,7 +28147,7 @@
         <v>390.89581099999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -28314,7 +28308,7 @@
         <v>36.150655</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -28475,7 +28469,7 @@
         <v>232.43127799999999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -28636,7 +28630,7 @@
         <v>750.77748799999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -28797,7 +28791,7 @@
         <v>735.26635299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28958,40 +28952,40 @@
         <v>3182.4750699999995</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -29019,16 +29013,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -29085,7 +29079,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -29246,7 +29240,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -29408,12 +29402,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -29574,7 +29568,7 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -29735,7 +29729,7 @@
         <v>11045</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -29896,7 +29890,7 @@
         <v>14998</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -30057,7 +30051,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -30218,7 +30212,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -30379,7 +30373,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -30540,7 +30534,7 @@
         <v>31551</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -30701,7 +30695,7 @@
         <v>81088</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -30756,12 +30750,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -30922,7 +30916,7 @@
         <v>307.73157300000003</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -31083,7 +31077,7 @@
         <v>782.92677600000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -31244,7 +31238,7 @@
         <v>401.64126599999997</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -31405,7 +31399,7 @@
         <v>32.955354</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -31566,7 +31560,7 @@
         <v>272.11873100000003</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -31727,7 +31721,7 @@
         <v>976.60348099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -31888,7 +31882,7 @@
         <v>752.63757299999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -32049,40 +32043,40 @@
         <v>3526.6147539999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -32110,16 +32104,16 @@
       <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -32176,7 +32170,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -32337,7 +32331,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -32499,12 +32493,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -32665,7 +32659,7 @@
         <v>4413</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -32826,7 +32820,7 @@
         <v>11673</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -32987,7 +32981,7 @@
         <v>15590</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -33148,7 +33142,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -33309,7 +33303,7 @@
         <v>8134</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -33470,7 +33464,7 @@
         <v>9863</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -33631,7 +33625,7 @@
         <v>34066</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -33792,7 +33786,7 @@
         <v>86245</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -33847,12 +33841,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -34013,7 +34007,7 @@
         <v>298.50642199999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -34174,7 +34168,7 @@
         <v>888.297684</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -34335,7 +34329,7 @@
         <v>533.92582100000004</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -34496,7 +34490,7 @@
         <v>38.857964000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -34657,7 +34651,7 @@
         <v>364.61675700000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -34818,7 +34812,7 @@
         <v>992.76339499999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -34979,7 +34973,7 @@
         <v>755.640308</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -35140,40 +35134,40 @@
         <v>3872.6083509999999</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Jul  8 05:32:18 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mtl-hq-f07\hq10aw2\planning\Reports\AAR\WebSummary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B325698-5757-4DCB-B90E-7A66B04E5BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{13E43EB9-4B07-473A-AFE3-69134558A7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="591" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -971,16 +971,16 @@
       <selection pane="bottomRight" activeCell="O12" sqref="O12:X12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.453125" style="9" customWidth="1"/>
-    <col min="53" max="53" width="9.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7265625" style="9"/>
+    <col min="1" max="1" width="50.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="9" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -1359,12 +1359,12 @@
         <v>42365</v>
       </c>
     </row>
-    <row r="4" spans="1:53" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>6942</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>11626</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>12499</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>6294</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>81196</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2707,12 +2707,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>470.98508700000002</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>958.98562200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>296.27038100000027</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>48.659481</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>212.439166</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>901.73460399999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>700.69452899999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>3589.7688700000003</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -4022,22 +4022,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection activeCell="F31" sqref="F31"/>
+      <selection pane="topRight" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7265625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -4094,7 +4094,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -4417,12 +4417,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>5706</v>
       </c>
       <c r="AB5" s="15">
-        <v>5546</v>
+        <v>5481</v>
       </c>
       <c r="AC5" s="15">
         <v>5871</v>
@@ -4583,7 +4583,7 @@
         <v>4363</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>12954</v>
       </c>
       <c r="AB6" s="15">
-        <v>12606</v>
+        <v>12528</v>
       </c>
       <c r="AC6" s="15">
         <v>12436</v>
@@ -4744,7 +4744,7 @@
         <v>11478</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -4827,7 +4827,7 @@
         <v>20139</v>
       </c>
       <c r="AB7" s="15">
-        <v>20735</v>
+        <v>21138</v>
       </c>
       <c r="AC7" s="15">
         <v>19123</v>
@@ -4905,7 +4905,7 @@
         <v>16410</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -4988,7 +4988,7 @@
         <v>4357</v>
       </c>
       <c r="AB8" s="15">
-        <v>3159</v>
+        <v>3060</v>
       </c>
       <c r="AC8" s="15">
         <v>2962</v>
@@ -5066,7 +5066,7 @@
         <v>2807</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>9782</v>
       </c>
       <c r="AB9" s="15">
-        <v>9374</v>
+        <v>9381</v>
       </c>
       <c r="AC9" s="15">
         <v>9598</v>
@@ -5227,7 +5227,7 @@
         <v>8047</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -5310,7 +5310,7 @@
         <v>11569</v>
       </c>
       <c r="AB10" s="15">
-        <v>12538</v>
+        <v>12539</v>
       </c>
       <c r="AC10" s="15">
         <v>11359</v>
@@ -5388,7 +5388,7 @@
         <v>12133</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>42029</v>
       </c>
       <c r="AB11" s="15">
-        <v>41801</v>
+        <v>41725</v>
       </c>
       <c r="AC11" s="15">
         <v>42569</v>
@@ -5549,7 +5549,7 @@
         <v>29432</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>106536</v>
       </c>
       <c r="AB12" s="7">
-        <v>105759</v>
+        <v>105852</v>
       </c>
       <c r="AC12" s="7">
         <v>103918</v>
@@ -5710,7 +5710,7 @@
         <v>84670</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5765,12 +5765,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -5853,7 +5853,7 @@
         <v>413.00203800000003</v>
       </c>
       <c r="AB15" s="15">
-        <v>386.429464</v>
+        <v>383.951571</v>
       </c>
       <c r="AC15" s="15">
         <v>422.52385800000002</v>
@@ -5931,7 +5931,7 @@
         <v>303.44771800000001</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -6014,7 +6014,7 @@
         <v>961.01767400000006</v>
       </c>
       <c r="AB16" s="15">
-        <v>868.32915100000002</v>
+        <v>867.55111099999999</v>
       </c>
       <c r="AC16" s="15">
         <v>896.38139899999999</v>
@@ -6092,7 +6092,7 @@
         <v>868.11864300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>664.18505400000004</v>
       </c>
       <c r="AB17" s="15">
-        <v>660.70479899999998</v>
+        <v>656.16408300000001</v>
       </c>
       <c r="AC17" s="15">
         <v>515.57698400000004</v>
@@ -6253,7 +6253,7 @@
         <v>433.165955</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>72.687977000000004</v>
       </c>
       <c r="AB18" s="15">
-        <v>61.666522999999998</v>
+        <v>58.066312000000003</v>
       </c>
       <c r="AC18" s="15">
         <v>53.912722000000002</v>
@@ -6414,7 +6414,7 @@
         <v>42.773207999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>409.32937700000002</v>
       </c>
       <c r="AB19" s="15">
-        <v>404.12152400000002</v>
+        <v>404.30506000000003</v>
       </c>
       <c r="AC19" s="15">
         <v>380.04726399999998</v>
@@ -6575,7 +6575,7 @@
         <v>374.79168900000002</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>1074.925176</v>
       </c>
       <c r="AB20" s="15">
-        <v>1181.8938250000001</v>
+        <v>1181.8572489999999</v>
       </c>
       <c r="AC20" s="15">
         <v>1063.2081720000001</v>
@@ -6736,7 +6736,7 @@
         <v>1143.806075</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -6819,7 +6819,7 @@
         <v>982.654223</v>
       </c>
       <c r="AB21" s="15">
-        <v>952.284626</v>
+        <v>952.53059299999995</v>
       </c>
       <c r="AC21" s="15">
         <v>1016.366184</v>
@@ -6897,7 +6897,7 @@
         <v>657.70498399999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>4577.8015190000006</v>
       </c>
       <c r="AB22" s="7">
-        <v>4515.4299119999996</v>
+        <v>4504.4259789999996</v>
       </c>
       <c r="AC22" s="7">
         <v>4348.0165830000005</v>
@@ -7058,40 +7058,40 @@
         <v>3823.8082720000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -7104,6 +7104,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -7114,22 +7117,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" sqref="A1:BA1"/>
+      <selection activeCell="I27" sqref="I27"/>
+      <selection pane="topRight" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
-    <col min="3" max="53" width="9.453125" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.453125" customWidth="1"/>
-    <col min="55" max="16384" width="6.7265625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="53" width="9.42578125" style="1" customWidth="1"/>
+    <col min="54" max="54" width="9.42578125" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>25</v>
       </c>
@@ -7186,7 +7189,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -7347,7 +7350,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -7509,13 +7512,13 @@
       </c>
       <c r="BB3" s="24"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -7598,7 +7601,7 @@
         <v>5080</v>
       </c>
       <c r="AB5" s="15">
-        <v>0</v>
+        <v>5009</v>
       </c>
       <c r="AC5" s="15">
         <v>0</v>
@@ -7677,7 +7680,7 @@
       </c>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -7760,7 +7763,7 @@
         <v>11640</v>
       </c>
       <c r="AB6" s="6">
-        <v>0</v>
+        <v>11713</v>
       </c>
       <c r="AC6" s="6">
         <v>0</v>
@@ -7839,7 +7842,7 @@
       </c>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -7922,7 +7925,7 @@
         <v>17821</v>
       </c>
       <c r="AB7" s="6">
-        <v>0</v>
+        <v>16986</v>
       </c>
       <c r="AC7" s="6">
         <v>0</v>
@@ -8001,7 +8004,7 @@
       </c>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -8084,7 +8087,7 @@
         <v>4424</v>
       </c>
       <c r="AB8" s="6">
-        <v>0</v>
+        <v>3464</v>
       </c>
       <c r="AC8" s="6">
         <v>0</v>
@@ -8163,7 +8166,7 @@
       </c>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -8246,7 +8249,7 @@
         <v>8710</v>
       </c>
       <c r="AB9" s="6">
-        <v>0</v>
+        <v>9486</v>
       </c>
       <c r="AC9" s="6">
         <v>0</v>
@@ -8325,7 +8328,7 @@
       </c>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -8408,7 +8411,7 @@
         <v>11858</v>
       </c>
       <c r="AB10" s="15">
-        <v>0</v>
+        <v>11814</v>
       </c>
       <c r="AC10" s="15">
         <v>0</v>
@@ -8487,7 +8490,7 @@
       </c>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -8570,7 +8573,7 @@
         <v>48315</v>
       </c>
       <c r="AB11" s="6">
-        <v>0</v>
+        <v>44353</v>
       </c>
       <c r="AC11" s="6">
         <v>0</v>
@@ -8649,7 +8652,7 @@
       </c>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -8732,7 +8735,7 @@
         <v>107848</v>
       </c>
       <c r="AB12" s="7">
-        <v>0</v>
+        <v>102825</v>
       </c>
       <c r="AC12" s="7">
         <v>0</v>
@@ -8811,7 +8814,7 @@
       </c>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -8867,13 +8870,13 @@
       <c r="BA13" s="6"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -8956,7 +8959,7 @@
         <v>365.78277000000003</v>
       </c>
       <c r="AB15" s="15">
-        <v>0</v>
+        <v>357.43256100000002</v>
       </c>
       <c r="AC15" s="15">
         <v>0</v>
@@ -9035,7 +9038,7 @@
       </c>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -9118,7 +9121,7 @@
         <v>797.54447000000005</v>
       </c>
       <c r="AB16" s="6">
-        <v>0</v>
+        <v>841.63460599999996</v>
       </c>
       <c r="AC16" s="6">
         <v>0</v>
@@ -9197,7 +9200,7 @@
       </c>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -9280,7 +9283,7 @@
         <v>557.70666600000004</v>
       </c>
       <c r="AB17" s="6">
-        <v>0</v>
+        <v>488.67721299999999</v>
       </c>
       <c r="AC17" s="6">
         <v>0</v>
@@ -9359,7 +9362,7 @@
       </c>
       <c r="BB17"/>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -9442,7 +9445,7 @@
         <v>65.075076999999993</v>
       </c>
       <c r="AB18" s="6">
-        <v>0</v>
+        <v>64.912823000000003</v>
       </c>
       <c r="AC18" s="6">
         <v>0</v>
@@ -9521,7 +9524,7 @@
       </c>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9604,7 +9607,7 @@
         <v>341.69426499999997</v>
       </c>
       <c r="AB19" s="6">
-        <v>0</v>
+        <v>354.55474700000002</v>
       </c>
       <c r="AC19" s="6">
         <v>0</v>
@@ -9683,7 +9686,7 @@
       </c>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -9766,7 +9769,7 @@
         <v>1072.4095500000001</v>
       </c>
       <c r="AB20" s="15">
-        <v>0</v>
+        <v>1033.8574739999999</v>
       </c>
       <c r="AC20" s="15">
         <v>0</v>
@@ -9845,7 +9848,7 @@
       </c>
       <c r="BB20"/>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -9928,7 +9931,7 @@
         <v>1107.0549920000001</v>
       </c>
       <c r="AB21" s="6">
-        <v>0</v>
+        <v>966.96226999999999</v>
       </c>
       <c r="AC21" s="6">
         <v>0</v>
@@ -10007,7 +10010,7 @@
       </c>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10090,7 +10093,7 @@
         <v>4307.2677900000008</v>
       </c>
       <c r="AB22" s="7">
-        <v>0</v>
+        <v>4108.0316939999993</v>
       </c>
       <c r="AC22" s="7">
         <v>0</v>
@@ -10169,100 +10172,100 @@
       </c>
       <c r="BB22"/>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="BB23"/>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB24"/>
     </row>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB25"/>
     </row>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB26"/>
     </row>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB27"/>
     </row>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB28"/>
     </row>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB29"/>
     </row>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB30"/>
     </row>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB31"/>
     </row>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB32"/>
     </row>
-    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB33"/>
     </row>
-    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB34"/>
     </row>
-    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB35"/>
     </row>
-    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB36"/>
     </row>
-    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB37"/>
     </row>
-    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB38"/>
     </row>
-    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB39"/>
     </row>
-    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB40"/>
     </row>
-    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB41"/>
     </row>
-    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB42"/>
     </row>
-    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB43"/>
     </row>
-    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB44"/>
     </row>
-    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB45"/>
     </row>
-    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB46"/>
     </row>
-    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB47"/>
     </row>
-    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB48"/>
     </row>
-    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB49"/>
     </row>
-    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB50"/>
     </row>
-    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB51"/>
     </row>
-    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB52"/>
     </row>
-    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB53"/>
     </row>
-    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB54"/>
     </row>
   </sheetData>
@@ -10277,6 +10280,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -10292,16 +10298,16 @@
       <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.453125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.453125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="17" customWidth="1"/>
     <col min="53" max="53" width="9" style="17" customWidth="1"/>
-    <col min="54" max="16384" width="6.7265625" style="17"/>
+    <col min="54" max="16384" width="6.7109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -10358,7 +10364,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -10519,7 +10525,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -10681,12 +10687,12 @@
       </c>
       <c r="BB3" s="23"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -10847,7 +10853,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -11008,7 +11014,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -11169,7 +11175,7 @@
         <v>15693</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -11330,7 +11336,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -11491,7 +11497,7 @@
         <v>6531</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11652,7 +11658,7 @@
         <v>10908</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -11813,7 +11819,7 @@
         <v>33194</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -11974,7 +11980,7 @@
         <v>88077</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -12029,12 +12035,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -12195,7 +12201,7 @@
         <v>448.48865799999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -12356,7 +12362,7 @@
         <v>863.31579299999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -12517,7 +12523,7 @@
         <v>424.08659699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -12678,7 +12684,7 @@
         <v>49.649962000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -12839,7 +12845,7 @@
         <v>235.51133100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -13000,7 +13006,7 @@
         <v>961.98002299999996</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -13161,7 +13167,7 @@
         <v>764.98213299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -13322,38 +13328,38 @@
         <v>3748.0144969999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -13382,16 +13388,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7265625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
@@ -13448,7 +13454,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -13609,7 +13615,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -13770,12 +13776,12 @@
         <v>43093</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -13936,7 +13942,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -14097,7 +14103,7 @@
         <v>9513</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -14258,7 +14264,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -14419,7 +14425,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -14580,7 +14586,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -14741,7 +14747,7 @@
         <v>9414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -14902,7 +14908,7 @@
         <v>36964</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -15063,7 +15069,7 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -15118,12 +15124,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -15284,7 +15290,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -15445,7 +15451,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -15606,7 +15612,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -15767,7 +15773,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -15928,7 +15934,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -16089,7 +16095,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -16250,7 +16256,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -16411,38 +16417,38 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -16467,16 +16473,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
     <col min="53" max="53" width="9" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7265625" style="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -16533,7 +16539,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16694,7 +16700,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -16856,12 +16862,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -17022,7 +17028,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -17183,7 +17189,7 @@
         <v>12729</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -17344,7 +17350,7 @@
         <v>16661</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -17505,7 +17511,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -17666,7 +17672,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -17827,7 +17833,7 @@
         <v>12175</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -17988,7 +17994,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -18149,7 +18155,7 @@
         <v>97169</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -18204,12 +18210,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -18370,7 +18376,7 @@
         <v>345.26898999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -18531,7 +18537,7 @@
         <v>1137.3429249999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -18692,7 +18698,7 @@
         <v>337.41420499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -18853,7 +18859,7 @@
         <v>40.33334</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -19014,7 +19020,7 @@
         <v>339.10771799999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -19175,7 +19181,7 @@
         <v>1247.683331</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -19336,7 +19342,7 @@
         <v>821.21724600000005</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -19497,38 +19503,38 @@
         <v>4268.3677550000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -19545,16 +19551,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7265625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -19611,7 +19617,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -19772,7 +19778,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -19934,12 +19940,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -20100,7 +20106,7 @@
         <v>5356</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -20261,7 +20267,7 @@
         <v>12576</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -20422,7 +20428,7 @@
         <v>17944</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -20583,7 +20589,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -20744,7 +20750,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -20905,7 +20911,7 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -21066,7 +21072,7 @@
         <v>38154</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -21227,7 +21233,7 @@
         <v>92789</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -21282,12 +21288,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -21448,7 +21454,7 @@
         <v>356.60756500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -21609,7 +21615,7 @@
         <v>977.829027</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -21770,7 +21776,7 @@
         <v>495.993199</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -21931,7 +21937,7 @@
         <v>37.412531000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -22092,7 +22098,7 @@
         <v>351.68923999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -22253,7 +22259,7 @@
         <v>888.50449000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -22414,7 +22420,7 @@
         <v>804.61703199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -22575,38 +22581,38 @@
         <v>3912.6530840000005</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -22623,17 +22629,17 @@
       <selection activeCell="A5" sqref="A5:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="6.7265625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
@@ -22690,7 +22696,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -22854,7 +22860,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="23.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -23016,7 +23022,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -23180,12 +23186,12 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -23349,7 +23355,7 @@
         <v>6187</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -23513,7 +23519,7 @@
         <v>11221</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -23677,7 +23683,7 @@
         <v>16946</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -23841,7 +23847,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
@@ -24005,7 +24011,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -24169,7 +24175,7 @@
         <v>13026</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -24333,7 +24339,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -24497,7 +24503,7 @@
         <v>99721</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -24553,12 +24559,12 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -24722,7 +24728,7 @@
         <v>469.697947</v>
       </c>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -24886,7 +24892,7 @@
         <v>800.96283800000003</v>
       </c>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -25050,7 +25056,7 @@
         <v>463.52606100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
@@ -25214,7 +25220,7 @@
         <v>39.121160000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -25378,7 +25384,7 @@
         <v>320.92344600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -25542,7 +25548,7 @@
         <v>1254.2732289999999</v>
       </c>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -25706,7 +25712,7 @@
         <v>905.27916400000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -25870,38 +25876,38 @@
         <v>4253.7838449999999</v>
       </c>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -25922,16 +25928,16 @@
       <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7265625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
@@ -25988,7 +25994,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -26149,7 +26155,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -26311,12 +26317,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -26477,7 +26483,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -26638,7 +26644,7 @@
         <v>10430</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -26799,7 +26805,7 @@
         <v>15971</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -26960,7 +26966,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -27121,7 +27127,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -27282,7 +27288,7 @@
         <v>8618</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -27443,7 +27449,7 @@
         <v>34889</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -27604,7 +27610,7 @@
         <v>83267</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -27659,12 +27665,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -27825,7 +27831,7 @@
         <v>326.63437199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -27986,7 +27992,7 @@
         <v>710.31911300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -28147,7 +28153,7 @@
         <v>390.89581099999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -28308,7 +28314,7 @@
         <v>36.150655</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -28469,7 +28475,7 @@
         <v>232.43127799999999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -28630,7 +28636,7 @@
         <v>750.77748799999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -28791,7 +28797,7 @@
         <v>735.26635299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28952,40 +28958,40 @@
         <v>3182.4750699999995</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -29013,16 +29019,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7265625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -29079,7 +29085,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -29240,7 +29246,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -29402,12 +29408,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -29568,7 +29574,7 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -29729,7 +29735,7 @@
         <v>11045</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -29890,7 +29896,7 @@
         <v>14998</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -30051,7 +30057,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -30212,7 +30218,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -30373,7 +30379,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -30534,7 +30540,7 @@
         <v>31551</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -30695,7 +30701,7 @@
         <v>81088</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -30750,12 +30756,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -30916,7 +30922,7 @@
         <v>307.73157300000003</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -31077,7 +31083,7 @@
         <v>782.92677600000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -31238,7 +31244,7 @@
         <v>401.64126599999997</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -31399,7 +31405,7 @@
         <v>32.955354</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -31560,7 +31566,7 @@
         <v>272.11873100000003</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -31721,7 +31727,7 @@
         <v>976.60348099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -31882,7 +31888,7 @@
         <v>752.63757299999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -32043,40 +32049,40 @@
         <v>3526.6147539999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -32104,16 +32110,16 @@
       <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.453125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7265625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -32170,7 +32176,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -32331,7 +32337,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -32493,12 +32499,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -32659,7 +32665,7 @@
         <v>4413</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -32820,7 +32826,7 @@
         <v>11673</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -32981,7 +32987,7 @@
         <v>15590</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -33142,7 +33148,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -33303,7 +33309,7 @@
         <v>8134</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -33464,7 +33470,7 @@
         <v>9863</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -33625,7 +33631,7 @@
         <v>34066</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -33786,7 +33792,7 @@
         <v>86245</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -33841,12 +33847,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -34007,7 +34013,7 @@
         <v>298.50642199999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -34168,7 +34174,7 @@
         <v>888.297684</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -34329,7 +34335,7 @@
         <v>533.92582100000004</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -34490,7 +34496,7 @@
         <v>38.857964000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -34651,7 +34657,7 @@
         <v>364.61675700000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -34812,7 +34818,7 @@
         <v>992.76339499999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -34973,7 +34979,7 @@
         <v>755.640308</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -35134,40 +35140,40 @@
         <v>3872.6083509999999</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Jul 15 05:36:15 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13E43EB9-4B07-473A-AFE3-69134558A7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9BBDDBC-21DA-4699-AEA0-7949B604A9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -4020,12 +4020,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="F31" sqref="F31"/>
-      <selection pane="topRight" activeCell="F31" sqref="F31"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
-      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
+      <selection sqref="A1:XFD1048576"/>
+      <selection pane="topRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4508,7 +4508,7 @@
         <v>5481</v>
       </c>
       <c r="AC5" s="15">
-        <v>5871</v>
+        <v>5857</v>
       </c>
       <c r="AD5" s="15">
         <v>5845</v>
@@ -4669,7 +4669,7 @@
         <v>12528</v>
       </c>
       <c r="AC6" s="15">
-        <v>12436</v>
+        <v>12378</v>
       </c>
       <c r="AD6" s="15">
         <v>12062</v>
@@ -4830,7 +4830,7 @@
         <v>21138</v>
       </c>
       <c r="AC7" s="15">
-        <v>19123</v>
+        <v>19319</v>
       </c>
       <c r="AD7" s="15">
         <v>19092</v>
@@ -4991,7 +4991,7 @@
         <v>3060</v>
       </c>
       <c r="AC8" s="15">
-        <v>2962</v>
+        <v>2956</v>
       </c>
       <c r="AD8" s="15">
         <v>3772</v>
@@ -5152,7 +5152,7 @@
         <v>9381</v>
       </c>
       <c r="AC9" s="15">
-        <v>9598</v>
+        <v>9432</v>
       </c>
       <c r="AD9" s="15">
         <v>9989</v>
@@ -5313,7 +5313,7 @@
         <v>12539</v>
       </c>
       <c r="AC10" s="15">
-        <v>11359</v>
+        <v>11356</v>
       </c>
       <c r="AD10" s="15">
         <v>12605</v>
@@ -5474,7 +5474,7 @@
         <v>41725</v>
       </c>
       <c r="AC11" s="15">
-        <v>42569</v>
+        <v>42477</v>
       </c>
       <c r="AD11" s="15">
         <v>40374</v>
@@ -5635,7 +5635,7 @@
         <v>105852</v>
       </c>
       <c r="AC12" s="7">
-        <v>103918</v>
+        <v>103775</v>
       </c>
       <c r="AD12" s="7">
         <v>103739</v>
@@ -5856,7 +5856,7 @@
         <v>383.951571</v>
       </c>
       <c r="AC15" s="15">
-        <v>422.52385800000002</v>
+        <v>421.595054</v>
       </c>
       <c r="AD15" s="15">
         <v>433.87811299999998</v>
@@ -6017,7 +6017,7 @@
         <v>867.55111099999999</v>
       </c>
       <c r="AC16" s="15">
-        <v>896.38139899999999</v>
+        <v>895.457086</v>
       </c>
       <c r="AD16" s="15">
         <v>853.149407</v>
@@ -6178,7 +6178,7 @@
         <v>656.16408300000001</v>
       </c>
       <c r="AC17" s="15">
-        <v>515.57698400000004</v>
+        <v>513.15248899999995</v>
       </c>
       <c r="AD17" s="15">
         <v>617.32262800000001</v>
@@ -6339,7 +6339,7 @@
         <v>58.066312000000003</v>
       </c>
       <c r="AC18" s="15">
-        <v>53.912722000000002</v>
+        <v>53.704225000000001</v>
       </c>
       <c r="AD18" s="15">
         <v>58.534090999999997</v>
@@ -6500,7 +6500,7 @@
         <v>404.30506000000003</v>
       </c>
       <c r="AC19" s="15">
-        <v>380.04726399999998</v>
+        <v>376.84693900000002</v>
       </c>
       <c r="AD19" s="15">
         <v>461.01832899999999</v>
@@ -6661,7 +6661,7 @@
         <v>1181.8572489999999</v>
       </c>
       <c r="AC20" s="15">
-        <v>1063.2081720000001</v>
+        <v>1062.910697</v>
       </c>
       <c r="AD20" s="15">
         <v>1273.432648</v>
@@ -6822,7 +6822,7 @@
         <v>952.53059299999995</v>
       </c>
       <c r="AC21" s="15">
-        <v>1016.366184</v>
+        <v>1015.210502</v>
       </c>
       <c r="AD21" s="15">
         <v>930.09202700000003</v>
@@ -6983,7 +6983,7 @@
         <v>4504.4259789999996</v>
       </c>
       <c r="AC22" s="7">
-        <v>4348.0165830000005</v>
+        <v>4338.8769919999995</v>
       </c>
       <c r="AD22" s="7">
         <v>4627.4272430000001</v>
@@ -7115,12 +7115,12 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="I27" sqref="I27"/>
-      <selection pane="topRight" activeCell="I27" sqref="I27"/>
-      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
-      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
+      <selection sqref="A1:XFD1048576"/>
+      <selection pane="topRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7604,7 +7604,7 @@
         <v>5009</v>
       </c>
       <c r="AC5" s="15">
-        <v>0</v>
+        <v>5341</v>
       </c>
       <c r="AD5" s="15">
         <v>0</v>
@@ -7766,7 +7766,7 @@
         <v>11713</v>
       </c>
       <c r="AC6" s="6">
-        <v>0</v>
+        <v>11717</v>
       </c>
       <c r="AD6" s="6">
         <v>0</v>
@@ -7928,7 +7928,7 @@
         <v>16986</v>
       </c>
       <c r="AC7" s="6">
-        <v>0</v>
+        <v>17486</v>
       </c>
       <c r="AD7" s="6">
         <v>0</v>
@@ -8090,7 +8090,7 @@
         <v>3464</v>
       </c>
       <c r="AC8" s="6">
-        <v>0</v>
+        <v>3412</v>
       </c>
       <c r="AD8" s="6">
         <v>0</v>
@@ -8252,7 +8252,7 @@
         <v>9486</v>
       </c>
       <c r="AC9" s="6">
-        <v>0</v>
+        <v>8838</v>
       </c>
       <c r="AD9" s="6">
         <v>0</v>
@@ -8414,7 +8414,7 @@
         <v>11814</v>
       </c>
       <c r="AC10" s="15">
-        <v>0</v>
+        <v>13091</v>
       </c>
       <c r="AD10" s="15">
         <v>0</v>
@@ -8576,7 +8576,7 @@
         <v>44353</v>
       </c>
       <c r="AC11" s="6">
-        <v>0</v>
+        <v>45423</v>
       </c>
       <c r="AD11" s="6">
         <v>0</v>
@@ -8738,7 +8738,7 @@
         <v>102825</v>
       </c>
       <c r="AC12" s="7">
-        <v>0</v>
+        <v>105308</v>
       </c>
       <c r="AD12" s="7">
         <v>0</v>
@@ -8962,7 +8962,7 @@
         <v>357.43256100000002</v>
       </c>
       <c r="AC15" s="15">
-        <v>0</v>
+        <v>397.92332099999999</v>
       </c>
       <c r="AD15" s="15">
         <v>0</v>
@@ -9124,7 +9124,7 @@
         <v>841.63460599999996</v>
       </c>
       <c r="AC16" s="6">
-        <v>0</v>
+        <v>762.90682100000004</v>
       </c>
       <c r="AD16" s="6">
         <v>0</v>
@@ -9286,7 +9286,7 @@
         <v>488.67721299999999</v>
       </c>
       <c r="AC17" s="6">
-        <v>0</v>
+        <v>525.11016099999995</v>
       </c>
       <c r="AD17" s="6">
         <v>0</v>
@@ -9448,7 +9448,7 @@
         <v>64.912823000000003</v>
       </c>
       <c r="AC18" s="6">
-        <v>0</v>
+        <v>59.627440999999997</v>
       </c>
       <c r="AD18" s="6">
         <v>0</v>
@@ -9610,7 +9610,7 @@
         <v>354.55474700000002</v>
       </c>
       <c r="AC19" s="6">
-        <v>0</v>
+        <v>368.24678899999998</v>
       </c>
       <c r="AD19" s="6">
         <v>0</v>
@@ -9772,7 +9772,7 @@
         <v>1033.8574739999999</v>
       </c>
       <c r="AC20" s="15">
-        <v>0</v>
+        <v>1146.3623070000001</v>
       </c>
       <c r="AD20" s="15">
         <v>0</v>
@@ -9934,7 +9934,7 @@
         <v>966.96226999999999</v>
       </c>
       <c r="AC21" s="6">
-        <v>0</v>
+        <v>1016.228458</v>
       </c>
       <c r="AD21" s="6">
         <v>0</v>
@@ -10096,7 +10096,7 @@
         <v>4108.0316939999993</v>
       </c>
       <c r="AC22" s="7">
-        <v>0</v>
+        <v>4276.4052979999997</v>
       </c>
       <c r="AD22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Jul 22 05:36:06 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9BBDDBC-21DA-4699-AEA0-7949B604A9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C73297B1-6B88-49CA-B1EE-1B85D569C684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -4020,12 +4020,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:XFD1048576"/>
-      <selection pane="topRight" sqref="A1:XFD1048576"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="E28" sqref="E28"/>
+      <selection pane="topRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4511,7 +4511,7 @@
         <v>5857</v>
       </c>
       <c r="AD5" s="15">
-        <v>5845</v>
+        <v>5791</v>
       </c>
       <c r="AE5" s="15">
         <v>5413</v>
@@ -4672,7 +4672,7 @@
         <v>12378</v>
       </c>
       <c r="AD6" s="15">
-        <v>12062</v>
+        <v>12009</v>
       </c>
       <c r="AE6" s="15">
         <v>11773</v>
@@ -4833,7 +4833,7 @@
         <v>19319</v>
       </c>
       <c r="AD7" s="15">
-        <v>19092</v>
+        <v>19495</v>
       </c>
       <c r="AE7" s="15">
         <v>18083</v>
@@ -4994,7 +4994,7 @@
         <v>2956</v>
       </c>
       <c r="AD8" s="15">
-        <v>3772</v>
+        <v>3763</v>
       </c>
       <c r="AE8" s="15">
         <v>3726</v>
@@ -5155,7 +5155,7 @@
         <v>9432</v>
       </c>
       <c r="AD9" s="15">
-        <v>9989</v>
+        <v>10004</v>
       </c>
       <c r="AE9" s="15">
         <v>7770</v>
@@ -5316,7 +5316,7 @@
         <v>11356</v>
       </c>
       <c r="AD10" s="15">
-        <v>12605</v>
+        <v>12602</v>
       </c>
       <c r="AE10" s="15">
         <v>10546</v>
@@ -5477,7 +5477,7 @@
         <v>42477</v>
       </c>
       <c r="AD11" s="15">
-        <v>40374</v>
+        <v>40251</v>
       </c>
       <c r="AE11" s="15">
         <v>36286</v>
@@ -5638,7 +5638,7 @@
         <v>103775</v>
       </c>
       <c r="AD12" s="7">
-        <v>103739</v>
+        <v>103915</v>
       </c>
       <c r="AE12" s="7">
         <v>93597</v>
@@ -5859,7 +5859,7 @@
         <v>421.595054</v>
       </c>
       <c r="AD15" s="15">
-        <v>433.87811299999998</v>
+        <v>430.08883400000002</v>
       </c>
       <c r="AE15" s="15">
         <v>380.56140900000003</v>
@@ -6020,7 +6020,7 @@
         <v>895.457086</v>
       </c>
       <c r="AD16" s="15">
-        <v>853.149407</v>
+        <v>852.48649499999999</v>
       </c>
       <c r="AE16" s="15">
         <v>830.34078899999997</v>
@@ -6181,7 +6181,7 @@
         <v>513.15248899999995</v>
       </c>
       <c r="AD17" s="15">
-        <v>617.32262800000001</v>
+        <v>617.48167999999998</v>
       </c>
       <c r="AE17" s="15">
         <v>615.61479199999997</v>
@@ -6342,7 +6342,7 @@
         <v>53.704225000000001</v>
       </c>
       <c r="AD18" s="15">
-        <v>58.534090999999997</v>
+        <v>58.262838000000002</v>
       </c>
       <c r="AE18" s="15">
         <v>55.373314999999998</v>
@@ -6503,7 +6503,7 @@
         <v>376.84693900000002</v>
       </c>
       <c r="AD19" s="15">
-        <v>461.01832899999999</v>
+        <v>461.69304</v>
       </c>
       <c r="AE19" s="15">
         <v>279.90213499999999</v>
@@ -6664,7 +6664,7 @@
         <v>1062.910697</v>
       </c>
       <c r="AD20" s="15">
-        <v>1273.432648</v>
+        <v>1273.451059</v>
       </c>
       <c r="AE20" s="15">
         <v>947.75155500000005</v>
@@ -6825,7 +6825,7 @@
         <v>1015.210502</v>
       </c>
       <c r="AD21" s="15">
-        <v>930.09202700000003</v>
+        <v>927.79157999999995</v>
       </c>
       <c r="AE21" s="15">
         <v>812.04394200000002</v>
@@ -6986,7 +6986,7 @@
         <v>4338.8769919999995</v>
       </c>
       <c r="AD22" s="7">
-        <v>4627.4272430000001</v>
+        <v>4621.2555259999999</v>
       </c>
       <c r="AE22" s="7">
         <v>3921.5879370000002</v>
@@ -7104,9 +7104,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -7115,12 +7112,12 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:XFD1048576"/>
-      <selection pane="topRight" sqref="A1:XFD1048576"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7607,7 +7604,7 @@
         <v>5341</v>
       </c>
       <c r="AD5" s="15">
-        <v>0</v>
+        <v>5197</v>
       </c>
       <c r="AE5" s="15">
         <v>0</v>
@@ -7769,7 +7766,7 @@
         <v>11717</v>
       </c>
       <c r="AD6" s="6">
-        <v>0</v>
+        <v>12349</v>
       </c>
       <c r="AE6" s="6">
         <v>0</v>
@@ -7931,7 +7928,7 @@
         <v>17486</v>
       </c>
       <c r="AD7" s="6">
-        <v>0</v>
+        <v>16538</v>
       </c>
       <c r="AE7" s="6">
         <v>0</v>
@@ -8093,7 +8090,7 @@
         <v>3412</v>
       </c>
       <c r="AD8" s="6">
-        <v>0</v>
+        <v>3796</v>
       </c>
       <c r="AE8" s="6">
         <v>0</v>
@@ -8255,7 +8252,7 @@
         <v>8838</v>
       </c>
       <c r="AD9" s="6">
-        <v>0</v>
+        <v>9966</v>
       </c>
       <c r="AE9" s="6">
         <v>0</v>
@@ -8417,7 +8414,7 @@
         <v>13091</v>
       </c>
       <c r="AD10" s="15">
-        <v>0</v>
+        <v>11287</v>
       </c>
       <c r="AE10" s="15">
         <v>0</v>
@@ -8579,7 +8576,7 @@
         <v>45423</v>
       </c>
       <c r="AD11" s="6">
-        <v>0</v>
+        <v>44009</v>
       </c>
       <c r="AE11" s="6">
         <v>0</v>
@@ -8741,7 +8738,7 @@
         <v>105308</v>
       </c>
       <c r="AD12" s="7">
-        <v>0</v>
+        <v>103142</v>
       </c>
       <c r="AE12" s="7">
         <v>0</v>
@@ -8965,7 +8962,7 @@
         <v>397.92332099999999</v>
       </c>
       <c r="AD15" s="15">
-        <v>0</v>
+        <v>387.33641699999998</v>
       </c>
       <c r="AE15" s="15">
         <v>0</v>
@@ -9127,7 +9124,7 @@
         <v>762.90682100000004</v>
       </c>
       <c r="AD16" s="6">
-        <v>0</v>
+        <v>886.37273900000002</v>
       </c>
       <c r="AE16" s="6">
         <v>0</v>
@@ -9289,7 +9286,7 @@
         <v>525.11016099999995</v>
       </c>
       <c r="AD17" s="6">
-        <v>0</v>
+        <v>496.195874</v>
       </c>
       <c r="AE17" s="6">
         <v>0</v>
@@ -9451,7 +9448,7 @@
         <v>59.627440999999997</v>
       </c>
       <c r="AD18" s="6">
-        <v>0</v>
+        <v>53.177581000000004</v>
       </c>
       <c r="AE18" s="6">
         <v>0</v>
@@ -9613,7 +9610,7 @@
         <v>368.24678899999998</v>
       </c>
       <c r="AD19" s="6">
-        <v>0</v>
+        <v>401.606021</v>
       </c>
       <c r="AE19" s="6">
         <v>0</v>
@@ -9775,7 +9772,7 @@
         <v>1146.3623070000001</v>
       </c>
       <c r="AD20" s="15">
-        <v>0</v>
+        <v>996.63184799999999</v>
       </c>
       <c r="AE20" s="15">
         <v>0</v>
@@ -9937,7 +9934,7 @@
         <v>1016.228458</v>
       </c>
       <c r="AD21" s="6">
-        <v>0</v>
+        <v>978.76567499999999</v>
       </c>
       <c r="AE21" s="6">
         <v>0</v>
@@ -10099,7 +10096,7 @@
         <v>4276.4052979999997</v>
       </c>
       <c r="AD22" s="7">
-        <v>0</v>
+        <v>4200.086155</v>
       </c>
       <c r="AE22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Jul 29 05:41:14 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C73297B1-6B88-49CA-B1EE-1B85D569C684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0448DE6A-5611-4A02-A4FB-72B5811C86A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -4022,10 +4022,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="E28" sqref="E28"/>
-      <selection pane="topRight" activeCell="E28" sqref="E28"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection sqref="A1:XFD1048576"/>
+      <selection pane="topRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4514,7 +4514,7 @@
         <v>5791</v>
       </c>
       <c r="AE5" s="15">
-        <v>5413</v>
+        <v>5387</v>
       </c>
       <c r="AF5" s="15">
         <v>5515</v>
@@ -4675,7 +4675,7 @@
         <v>12009</v>
       </c>
       <c r="AE6" s="15">
-        <v>11773</v>
+        <v>11704</v>
       </c>
       <c r="AF6" s="15">
         <v>12697</v>
@@ -4836,7 +4836,7 @@
         <v>19495</v>
       </c>
       <c r="AE7" s="15">
-        <v>18083</v>
+        <v>18248</v>
       </c>
       <c r="AF7" s="15">
         <v>20042</v>
@@ -4997,7 +4997,7 @@
         <v>3763</v>
       </c>
       <c r="AE8" s="15">
-        <v>3726</v>
+        <v>3727</v>
       </c>
       <c r="AF8" s="15">
         <v>3838</v>
@@ -5158,7 +5158,7 @@
         <v>10004</v>
       </c>
       <c r="AE9" s="15">
-        <v>7770</v>
+        <v>7679</v>
       </c>
       <c r="AF9" s="15">
         <v>9070</v>
@@ -5319,7 +5319,7 @@
         <v>12602</v>
       </c>
       <c r="AE10" s="15">
-        <v>10546</v>
+        <v>10550</v>
       </c>
       <c r="AF10" s="15">
         <v>12073</v>
@@ -5480,7 +5480,7 @@
         <v>40251</v>
       </c>
       <c r="AE11" s="15">
-        <v>36286</v>
+        <v>36151</v>
       </c>
       <c r="AF11" s="15">
         <v>34990</v>
@@ -5641,7 +5641,7 @@
         <v>103915</v>
       </c>
       <c r="AE12" s="7">
-        <v>93597</v>
+        <v>93446</v>
       </c>
       <c r="AF12" s="7">
         <v>98225</v>
@@ -5862,7 +5862,7 @@
         <v>430.08883400000002</v>
       </c>
       <c r="AE15" s="15">
-        <v>380.56140900000003</v>
+        <v>378.531429</v>
       </c>
       <c r="AF15" s="15">
         <v>415.58773500000001</v>
@@ -6023,7 +6023,7 @@
         <v>852.48649499999999</v>
       </c>
       <c r="AE16" s="15">
-        <v>830.34078899999997</v>
+        <v>829.702808</v>
       </c>
       <c r="AF16" s="15">
         <v>923.61398999999994</v>
@@ -6184,7 +6184,7 @@
         <v>617.48167999999998</v>
       </c>
       <c r="AE17" s="15">
-        <v>615.61479199999997</v>
+        <v>614.00238400000001</v>
       </c>
       <c r="AF17" s="15">
         <v>659.67492800000002</v>
@@ -6345,7 +6345,7 @@
         <v>58.262838000000002</v>
       </c>
       <c r="AE18" s="15">
-        <v>55.373314999999998</v>
+        <v>55.382570999999999</v>
       </c>
       <c r="AF18" s="15">
         <v>61.302722000000003</v>
@@ -6506,7 +6506,7 @@
         <v>461.69304</v>
       </c>
       <c r="AE19" s="15">
-        <v>279.90213499999999</v>
+        <v>279.95686699999999</v>
       </c>
       <c r="AF19" s="15">
         <v>373.06740200000002</v>
@@ -6667,7 +6667,7 @@
         <v>1273.451059</v>
       </c>
       <c r="AE20" s="15">
-        <v>947.75155500000005</v>
+        <v>950.05083000000002</v>
       </c>
       <c r="AF20" s="15">
         <v>1132.216349</v>
@@ -6828,7 +6828,7 @@
         <v>927.79157999999995</v>
       </c>
       <c r="AE21" s="15">
-        <v>812.04394200000002</v>
+        <v>809.81867999999997</v>
       </c>
       <c r="AF21" s="15">
         <v>853.15909999999997</v>
@@ -6989,7 +6989,7 @@
         <v>4621.2555259999999</v>
       </c>
       <c r="AE22" s="7">
-        <v>3921.5879370000002</v>
+        <v>3917.445569</v>
       </c>
       <c r="AF22" s="7">
         <v>4418.6222259999995</v>
@@ -7104,6 +7104,9 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -7114,10 +7117,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="H30" sqref="H30"/>
+      <selection activeCell="E34" sqref="E34"/>
+      <selection pane="topRight" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7607,7 +7610,7 @@
         <v>5197</v>
       </c>
       <c r="AE5" s="15">
-        <v>0</v>
+        <v>5354</v>
       </c>
       <c r="AF5" s="15">
         <v>0</v>
@@ -7769,7 +7772,7 @@
         <v>12349</v>
       </c>
       <c r="AE6" s="6">
-        <v>0</v>
+        <v>12490</v>
       </c>
       <c r="AF6" s="6">
         <v>0</v>
@@ -7931,7 +7934,7 @@
         <v>16538</v>
       </c>
       <c r="AE7" s="6">
-        <v>0</v>
+        <v>17696</v>
       </c>
       <c r="AF7" s="6">
         <v>0</v>
@@ -8093,7 +8096,7 @@
         <v>3796</v>
       </c>
       <c r="AE8" s="6">
-        <v>0</v>
+        <v>3684</v>
       </c>
       <c r="AF8" s="6">
         <v>0</v>
@@ -8255,7 +8258,7 @@
         <v>9966</v>
       </c>
       <c r="AE9" s="6">
-        <v>0</v>
+        <v>8883</v>
       </c>
       <c r="AF9" s="6">
         <v>0</v>
@@ -8417,7 +8420,7 @@
         <v>11287</v>
       </c>
       <c r="AE10" s="15">
-        <v>0</v>
+        <v>11643</v>
       </c>
       <c r="AF10" s="15">
         <v>0</v>
@@ -8579,7 +8582,7 @@
         <v>44009</v>
       </c>
       <c r="AE11" s="6">
-        <v>0</v>
+        <v>43611</v>
       </c>
       <c r="AF11" s="6">
         <v>0</v>
@@ -8741,7 +8744,7 @@
         <v>103142</v>
       </c>
       <c r="AE12" s="7">
-        <v>0</v>
+        <v>103361</v>
       </c>
       <c r="AF12" s="7">
         <v>0</v>
@@ -8965,7 +8968,7 @@
         <v>387.33641699999998</v>
       </c>
       <c r="AE15" s="15">
-        <v>0</v>
+        <v>404.68403799999999</v>
       </c>
       <c r="AF15" s="15">
         <v>0</v>
@@ -9127,7 +9130,7 @@
         <v>886.37273900000002</v>
       </c>
       <c r="AE16" s="6">
-        <v>0</v>
+        <v>859.638778</v>
       </c>
       <c r="AF16" s="6">
         <v>0</v>
@@ -9289,7 +9292,7 @@
         <v>496.195874</v>
       </c>
       <c r="AE17" s="6">
-        <v>0</v>
+        <v>548.61793499999999</v>
       </c>
       <c r="AF17" s="6">
         <v>0</v>
@@ -9451,7 +9454,7 @@
         <v>53.177581000000004</v>
       </c>
       <c r="AE18" s="6">
-        <v>0</v>
+        <v>60.448929999999997</v>
       </c>
       <c r="AF18" s="6">
         <v>0</v>
@@ -9613,7 +9616,7 @@
         <v>401.606021</v>
       </c>
       <c r="AE19" s="6">
-        <v>0</v>
+        <v>366.91344600000002</v>
       </c>
       <c r="AF19" s="6">
         <v>0</v>
@@ -9775,7 +9778,7 @@
         <v>996.63184799999999</v>
       </c>
       <c r="AE20" s="15">
-        <v>0</v>
+        <v>958.78646800000001</v>
       </c>
       <c r="AF20" s="15">
         <v>0</v>
@@ -9937,7 +9940,7 @@
         <v>978.76567499999999</v>
       </c>
       <c r="AE21" s="6">
-        <v>0</v>
+        <v>960.89804800000002</v>
       </c>
       <c r="AF21" s="6">
         <v>0</v>
@@ -10099,7 +10102,7 @@
         <v>4200.086155</v>
       </c>
       <c r="AE22" s="7">
-        <v>0</v>
+        <v>4159.9876430000004</v>
       </c>
       <c r="AF22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Aug  5 05:42:07 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0448DE6A-5611-4A02-A4FB-72B5811C86A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EFE2249-9BBC-4866-AC32-E9A02EAAAE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="591" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -971,16 +971,16 @@
       <selection pane="bottomRight" activeCell="O12" sqref="O12:X12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="9" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="9"/>
+    <col min="1" max="1" width="50.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="9" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -1359,12 +1359,12 @@
         <v>42365</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>6942</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>11626</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>12499</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>6294</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>81196</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2707,12 +2707,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>470.98508700000002</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>958.98562200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>296.27038100000027</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>48.659481</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>212.439166</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>901.73460399999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>700.69452899999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>3589.7688700000003</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -4022,22 +4022,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection sqref="A1:XFD1048576"/>
-      <selection pane="topRight" sqref="A1:XFD1048576"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <selection activeCell="D25" sqref="D25"/>
+      <selection pane="topRight" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -4094,7 +4094,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -4417,12 +4417,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>5387</v>
       </c>
       <c r="AF5" s="15">
-        <v>5515</v>
+        <v>5478</v>
       </c>
       <c r="AG5" s="15">
         <v>5766</v>
@@ -4583,7 +4583,7 @@
         <v>4363</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>11704</v>
       </c>
       <c r="AF6" s="15">
-        <v>12697</v>
+        <v>12660</v>
       </c>
       <c r="AG6" s="15">
         <v>12607</v>
@@ -4744,7 +4744,7 @@
         <v>11478</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>18248</v>
       </c>
       <c r="AF7" s="15">
-        <v>20042</v>
+        <v>20340</v>
       </c>
       <c r="AG7" s="15">
         <v>18319</v>
@@ -4905,7 +4905,7 @@
         <v>16410</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>3727</v>
       </c>
       <c r="AF8" s="15">
-        <v>3838</v>
+        <v>3833</v>
       </c>
       <c r="AG8" s="15">
         <v>4025</v>
@@ -5066,7 +5066,7 @@
         <v>2807</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>7679</v>
       </c>
       <c r="AF9" s="15">
-        <v>9070</v>
+        <v>9071</v>
       </c>
       <c r="AG9" s="15">
         <v>8846</v>
@@ -5227,7 +5227,7 @@
         <v>8047</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>10550</v>
       </c>
       <c r="AF10" s="15">
-        <v>12073</v>
+        <v>12067</v>
       </c>
       <c r="AG10" s="15">
         <v>12463</v>
@@ -5388,7 +5388,7 @@
         <v>12133</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>36151</v>
       </c>
       <c r="AF11" s="15">
-        <v>34990</v>
+        <v>34897</v>
       </c>
       <c r="AG11" s="15">
         <v>39166</v>
@@ -5549,7 +5549,7 @@
         <v>29432</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>93446</v>
       </c>
       <c r="AF12" s="7">
-        <v>98225</v>
+        <v>98346</v>
       </c>
       <c r="AG12" s="7">
         <v>101192</v>
@@ -5710,7 +5710,7 @@
         <v>84670</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5765,12 +5765,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>378.531429</v>
       </c>
       <c r="AF15" s="15">
-        <v>415.58773500000001</v>
+        <v>411.439482</v>
       </c>
       <c r="AG15" s="15">
         <v>427.68074100000001</v>
@@ -5931,7 +5931,7 @@
         <v>303.44771800000001</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -6026,7 +6026,7 @@
         <v>829.702808</v>
       </c>
       <c r="AF16" s="15">
-        <v>923.61398999999994</v>
+        <v>921.33457799999996</v>
       </c>
       <c r="AG16" s="15">
         <v>905.70455900000002</v>
@@ -6092,7 +6092,7 @@
         <v>868.11864300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -6187,7 +6187,7 @@
         <v>614.00238400000001</v>
       </c>
       <c r="AF17" s="15">
-        <v>659.67492800000002</v>
+        <v>659.46664699999997</v>
       </c>
       <c r="AG17" s="15">
         <v>642.541875</v>
@@ -6253,7 +6253,7 @@
         <v>433.165955</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -6348,7 +6348,7 @@
         <v>55.382570999999999</v>
       </c>
       <c r="AF18" s="15">
-        <v>61.302722000000003</v>
+        <v>61.255878000000003</v>
       </c>
       <c r="AG18" s="15">
         <v>57.728878000000002</v>
@@ -6414,7 +6414,7 @@
         <v>42.773207999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>279.95686699999999</v>
       </c>
       <c r="AF19" s="15">
-        <v>373.06740200000002</v>
+        <v>373.11177199999997</v>
       </c>
       <c r="AG19" s="15">
         <v>399.94396399999999</v>
@@ -6575,7 +6575,7 @@
         <v>374.79168900000002</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>950.05083000000002</v>
       </c>
       <c r="AF20" s="15">
-        <v>1132.216349</v>
+        <v>1132.3510699999999</v>
       </c>
       <c r="AG20" s="15">
         <v>1076.2912349999999</v>
@@ -6736,7 +6736,7 @@
         <v>1143.806075</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>809.81867999999997</v>
       </c>
       <c r="AF21" s="15">
-        <v>853.15909999999997</v>
+        <v>851.04168600000003</v>
       </c>
       <c r="AG21" s="15">
         <v>890.03262199999995</v>
@@ -6897,7 +6897,7 @@
         <v>657.70498399999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v>3917.445569</v>
       </c>
       <c r="AF22" s="7">
-        <v>4418.6222259999995</v>
+        <v>4410.0011130000003</v>
       </c>
       <c r="AG22" s="7">
         <v>4399.9238739999992</v>
@@ -7058,40 +7058,40 @@
         <v>3823.8082720000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -7116,23 +7116,23 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="E34" sqref="E34"/>
-      <selection pane="topRight" activeCell="E34" sqref="E34"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="D25" sqref="D25"/>
+      <selection pane="topRight" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="53" width="9.42578125" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.42578125" customWidth="1"/>
-    <col min="55" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="53" width="9.44140625" style="1" customWidth="1"/>
+    <col min="54" max="54" width="9.44140625" customWidth="1"/>
+    <col min="55" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>25</v>
       </c>
@@ -7189,7 +7189,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -7350,7 +7350,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -7512,13 +7512,13 @@
       </c>
       <c r="BB3" s="24"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -7613,7 +7613,7 @@
         <v>5354</v>
       </c>
       <c r="AF5" s="15">
-        <v>0</v>
+        <v>5362</v>
       </c>
       <c r="AG5" s="15">
         <v>0</v>
@@ -7680,7 +7680,7 @@
       </c>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -7775,7 +7775,7 @@
         <v>12490</v>
       </c>
       <c r="AF6" s="6">
-        <v>0</v>
+        <v>12439</v>
       </c>
       <c r="AG6" s="6">
         <v>0</v>
@@ -7842,7 +7842,7 @@
       </c>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -7937,7 +7937,7 @@
         <v>17696</v>
       </c>
       <c r="AF7" s="6">
-        <v>0</v>
+        <v>17707</v>
       </c>
       <c r="AG7" s="6">
         <v>0</v>
@@ -8004,7 +8004,7 @@
       </c>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -8099,7 +8099,7 @@
         <v>3684</v>
       </c>
       <c r="AF8" s="6">
-        <v>0</v>
+        <v>3694</v>
       </c>
       <c r="AG8" s="6">
         <v>0</v>
@@ -8166,7 +8166,7 @@
       </c>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -8261,7 +8261,7 @@
         <v>8883</v>
       </c>
       <c r="AF9" s="6">
-        <v>0</v>
+        <v>9851</v>
       </c>
       <c r="AG9" s="6">
         <v>0</v>
@@ -8328,7 +8328,7 @@
       </c>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -8423,7 +8423,7 @@
         <v>11643</v>
       </c>
       <c r="AF10" s="15">
-        <v>0</v>
+        <v>11366</v>
       </c>
       <c r="AG10" s="15">
         <v>0</v>
@@ -8490,7 +8490,7 @@
       </c>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -8585,7 +8585,7 @@
         <v>43611</v>
       </c>
       <c r="AF11" s="6">
-        <v>0</v>
+        <v>43793</v>
       </c>
       <c r="AG11" s="6">
         <v>0</v>
@@ -8652,7 +8652,7 @@
       </c>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -8747,7 +8747,7 @@
         <v>103361</v>
       </c>
       <c r="AF12" s="7">
-        <v>0</v>
+        <v>104212</v>
       </c>
       <c r="AG12" s="7">
         <v>0</v>
@@ -8814,7 +8814,7 @@
       </c>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -8870,13 +8870,13 @@
       <c r="BA13" s="6"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -8971,7 +8971,7 @@
         <v>404.68403799999999</v>
       </c>
       <c r="AF15" s="15">
-        <v>0</v>
+        <v>399.22666700000002</v>
       </c>
       <c r="AG15" s="15">
         <v>0</v>
@@ -9038,7 +9038,7 @@
       </c>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -9133,7 +9133,7 @@
         <v>859.638778</v>
       </c>
       <c r="AF16" s="6">
-        <v>0</v>
+        <v>909.42033000000004</v>
       </c>
       <c r="AG16" s="6">
         <v>0</v>
@@ -9200,7 +9200,7 @@
       </c>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -9295,7 +9295,7 @@
         <v>548.61793499999999</v>
       </c>
       <c r="AF17" s="6">
-        <v>0</v>
+        <v>588.55939599999999</v>
       </c>
       <c r="AG17" s="6">
         <v>0</v>
@@ -9362,7 +9362,7 @@
       </c>
       <c r="BB17"/>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -9457,7 +9457,7 @@
         <v>60.448929999999997</v>
       </c>
       <c r="AF18" s="6">
-        <v>0</v>
+        <v>56.876569000000003</v>
       </c>
       <c r="AG18" s="6">
         <v>0</v>
@@ -9524,7 +9524,7 @@
       </c>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9619,7 +9619,7 @@
         <v>366.91344600000002</v>
       </c>
       <c r="AF19" s="6">
-        <v>0</v>
+        <v>422.06519200000002</v>
       </c>
       <c r="AG19" s="6">
         <v>0</v>
@@ -9686,7 +9686,7 @@
       </c>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -9781,7 +9781,7 @@
         <v>958.78646800000001</v>
       </c>
       <c r="AF20" s="15">
-        <v>0</v>
+        <v>1018.263691</v>
       </c>
       <c r="AG20" s="15">
         <v>0</v>
@@ -9848,7 +9848,7 @@
       </c>
       <c r="BB20"/>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -9943,7 +9943,7 @@
         <v>960.89804800000002</v>
       </c>
       <c r="AF21" s="6">
-        <v>0</v>
+        <v>1010.360158</v>
       </c>
       <c r="AG21" s="6">
         <v>0</v>
@@ -10010,7 +10010,7 @@
       </c>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10105,7 +10105,7 @@
         <v>4159.9876430000004</v>
       </c>
       <c r="AF22" s="7">
-        <v>0</v>
+        <v>4404.772003</v>
       </c>
       <c r="AG22" s="7">
         <v>0</v>
@@ -10172,100 +10172,100 @@
       </c>
       <c r="BB22"/>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="BB23"/>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB24"/>
     </row>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB25"/>
     </row>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB26"/>
     </row>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB27"/>
     </row>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB28"/>
     </row>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB29"/>
     </row>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB30"/>
     </row>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB31"/>
     </row>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB32"/>
     </row>
-    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB33"/>
     </row>
-    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB34"/>
     </row>
-    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB35"/>
     </row>
-    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB36"/>
     </row>
-    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB37"/>
     </row>
-    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB38"/>
     </row>
-    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB39"/>
     </row>
-    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB40"/>
     </row>
-    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB41"/>
     </row>
-    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB42"/>
     </row>
-    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB43"/>
     </row>
-    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB44"/>
     </row>
-    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB45"/>
     </row>
-    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB46"/>
     </row>
-    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB47"/>
     </row>
-    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB48"/>
     </row>
-    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB49"/>
     </row>
-    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB50"/>
     </row>
-    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB51"/>
     </row>
-    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB52"/>
     </row>
-    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB53"/>
     </row>
-    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="BB54"/>
     </row>
   </sheetData>
@@ -10298,16 +10298,16 @@
       <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="17" customWidth="1"/>
     <col min="53" max="53" width="9" style="17" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="17"/>
+    <col min="54" max="16384" width="6.6640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -10364,7 +10364,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -10525,7 +10525,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -10687,12 +10687,12 @@
       </c>
       <c r="BB3" s="23"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -10853,7 +10853,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -11014,7 +11014,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -11175,7 +11175,7 @@
         <v>15693</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -11336,7 +11336,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -11497,7 +11497,7 @@
         <v>6531</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11658,7 +11658,7 @@
         <v>10908</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -11819,7 +11819,7 @@
         <v>33194</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -11980,7 +11980,7 @@
         <v>88077</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -12035,12 +12035,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -12201,7 +12201,7 @@
         <v>448.48865799999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -12362,7 +12362,7 @@
         <v>863.31579299999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -12523,7 +12523,7 @@
         <v>424.08659699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -12684,7 +12684,7 @@
         <v>49.649962000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -12845,7 +12845,7 @@
         <v>235.51133100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -13006,7 +13006,7 @@
         <v>961.98002299999996</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -13167,7 +13167,7 @@
         <v>764.98213299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -13328,38 +13328,38 @@
         <v>3748.0144969999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -13388,16 +13388,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
@@ -13454,7 +13454,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -13615,7 +13615,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -13776,12 +13776,12 @@
         <v>43093</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -13942,7 +13942,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -14103,7 +14103,7 @@
         <v>9513</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -14264,7 +14264,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -14425,7 +14425,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -14586,7 +14586,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -14747,7 +14747,7 @@
         <v>9414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -14908,7 +14908,7 @@
         <v>36964</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -15069,7 +15069,7 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -15124,12 +15124,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -15290,7 +15290,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -15451,7 +15451,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -15612,7 +15612,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -15773,7 +15773,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -15934,7 +15934,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -16095,7 +16095,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -16256,7 +16256,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -16417,38 +16417,38 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -16473,16 +16473,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
     <col min="53" max="53" width="9" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -16539,7 +16539,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16700,7 +16700,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -16862,12 +16862,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -17028,7 +17028,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -17189,7 +17189,7 @@
         <v>12729</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -17350,7 +17350,7 @@
         <v>16661</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -17511,7 +17511,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -17672,7 +17672,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -17833,7 +17833,7 @@
         <v>12175</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -17994,7 +17994,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -18155,7 +18155,7 @@
         <v>97169</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -18210,12 +18210,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -18376,7 +18376,7 @@
         <v>345.26898999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -18537,7 +18537,7 @@
         <v>1137.3429249999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -18698,7 +18698,7 @@
         <v>337.41420499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -18859,7 +18859,7 @@
         <v>40.33334</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -19020,7 +19020,7 @@
         <v>339.10771799999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -19181,7 +19181,7 @@
         <v>1247.683331</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -19342,7 +19342,7 @@
         <v>821.21724600000005</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -19503,38 +19503,38 @@
         <v>4268.3677550000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -19551,16 +19551,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -19617,7 +19617,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -19778,7 +19778,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -19940,12 +19940,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -20106,7 +20106,7 @@
         <v>5356</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -20267,7 +20267,7 @@
         <v>12576</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -20428,7 +20428,7 @@
         <v>17944</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -20589,7 +20589,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -20750,7 +20750,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -20911,7 +20911,7 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -21072,7 +21072,7 @@
         <v>38154</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -21233,7 +21233,7 @@
         <v>92789</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -21288,12 +21288,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -21454,7 +21454,7 @@
         <v>356.60756500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -21615,7 +21615,7 @@
         <v>977.829027</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -21776,7 +21776,7 @@
         <v>495.993199</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -21937,7 +21937,7 @@
         <v>37.412531000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -22098,7 +22098,7 @@
         <v>351.68923999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -22259,7 +22259,7 @@
         <v>888.50449000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -22420,7 +22420,7 @@
         <v>804.61703199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -22581,38 +22581,38 @@
         <v>3912.6530840000005</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -22629,17 +22629,17 @@
       <selection activeCell="A5" sqref="A5:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
@@ -22696,7 +22696,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -22860,7 +22860,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -23022,7 +23022,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -23186,12 +23186,12 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -23355,7 +23355,7 @@
         <v>6187</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -23519,7 +23519,7 @@
         <v>11221</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -23683,7 +23683,7 @@
         <v>16946</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -23847,7 +23847,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
@@ -24011,7 +24011,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -24175,7 +24175,7 @@
         <v>13026</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -24339,7 +24339,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -24503,7 +24503,7 @@
         <v>99721</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -24559,12 +24559,12 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -24728,7 +24728,7 @@
         <v>469.697947</v>
       </c>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -24892,7 +24892,7 @@
         <v>800.96283800000003</v>
       </c>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -25056,7 +25056,7 @@
         <v>463.52606100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
@@ -25220,7 +25220,7 @@
         <v>39.121160000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -25384,7 +25384,7 @@
         <v>320.92344600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -25548,7 +25548,7 @@
         <v>1254.2732289999999</v>
       </c>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -25712,7 +25712,7 @@
         <v>905.27916400000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -25876,38 +25876,38 @@
         <v>4253.7838449999999</v>
       </c>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -25928,16 +25928,16 @@
       <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
@@ -25994,7 +25994,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -26155,7 +26155,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -26317,12 +26317,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -26483,7 +26483,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -26644,7 +26644,7 @@
         <v>10430</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -26805,7 +26805,7 @@
         <v>15971</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -26966,7 +26966,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -27127,7 +27127,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -27288,7 +27288,7 @@
         <v>8618</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -27449,7 +27449,7 @@
         <v>34889</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -27610,7 +27610,7 @@
         <v>83267</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -27665,12 +27665,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -27831,7 +27831,7 @@
         <v>326.63437199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -27992,7 +27992,7 @@
         <v>710.31911300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -28153,7 +28153,7 @@
         <v>390.89581099999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -28314,7 +28314,7 @@
         <v>36.150655</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -28475,7 +28475,7 @@
         <v>232.43127799999999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -28636,7 +28636,7 @@
         <v>750.77748799999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -28797,7 +28797,7 @@
         <v>735.26635299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28958,40 +28958,40 @@
         <v>3182.4750699999995</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -29019,16 +29019,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -29085,7 +29085,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -29246,7 +29246,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -29408,12 +29408,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -29574,7 +29574,7 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -29735,7 +29735,7 @@
         <v>11045</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -29896,7 +29896,7 @@
         <v>14998</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -30057,7 +30057,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -30218,7 +30218,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -30379,7 +30379,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -30540,7 +30540,7 @@
         <v>31551</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -30701,7 +30701,7 @@
         <v>81088</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -30756,12 +30756,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -30922,7 +30922,7 @@
         <v>307.73157300000003</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -31083,7 +31083,7 @@
         <v>782.92677600000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -31244,7 +31244,7 @@
         <v>401.64126599999997</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -31405,7 +31405,7 @@
         <v>32.955354</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -31566,7 +31566,7 @@
         <v>272.11873100000003</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -31727,7 +31727,7 @@
         <v>976.60348099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -31888,7 +31888,7 @@
         <v>752.63757299999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -32049,40 +32049,40 @@
         <v>3526.6147539999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -32110,16 +32110,16 @@
       <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.7109375" style="1"/>
+    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -32176,7 +32176,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -32337,7 +32337,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -32499,12 +32499,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -32665,7 +32665,7 @@
         <v>4413</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -32826,7 +32826,7 @@
         <v>11673</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -32987,7 +32987,7 @@
         <v>15590</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -33148,7 +33148,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -33309,7 +33309,7 @@
         <v>8134</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -33470,7 +33470,7 @@
         <v>9863</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -33631,7 +33631,7 @@
         <v>34066</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -33792,7 +33792,7 @@
         <v>86245</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -33847,12 +33847,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -34013,7 +34013,7 @@
         <v>298.50642199999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -34174,7 +34174,7 @@
         <v>888.297684</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -34335,7 +34335,7 @@
         <v>533.92582100000004</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -34496,7 +34496,7 @@
         <v>38.857964000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -34657,7 +34657,7 @@
         <v>364.61675700000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -34818,7 +34818,7 @@
         <v>992.76339499999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -34979,7 +34979,7 @@
         <v>755.640308</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -35140,40 +35140,40 @@
         <v>3872.6083509999999</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Aug 12 05:31:58 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EFE2249-9BBC-4866-AC32-E9A02EAAAE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E456DD85-809D-45A3-82AF-51EFAC8EC324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="591" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -971,16 +971,16 @@
       <selection pane="bottomRight" activeCell="O12" sqref="O12:X12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="9" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="9"/>
+    <col min="1" max="1" width="50.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="9" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -1359,12 +1359,12 @@
         <v>42365</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>6942</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>11626</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>12499</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>6294</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>31058</v>
       </c>
     </row>
-    <row r="12" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>81196</v>
       </c>
     </row>
-    <row r="13" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2707,12 +2707,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>470.98508700000002</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>958.98562200000003</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>296.27038100000027</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>48.659481</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>212.439166</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>901.73460399999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>700.69452899999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>3589.7688700000003</v>
       </c>
     </row>
-    <row r="23" spans="1:53" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -4022,22 +4022,22 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="D25" sqref="D25"/>
-      <selection pane="topRight" activeCell="D25" sqref="D25"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
-      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
+      <selection activeCell="E34" sqref="E34"/>
+      <selection pane="topRight" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -4094,7 +4094,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -4417,12 +4417,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>5478</v>
       </c>
       <c r="AG5" s="15">
-        <v>5766</v>
+        <v>5718</v>
       </c>
       <c r="AH5" s="15">
         <v>5922</v>
@@ -4583,7 +4583,7 @@
         <v>4363</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>12660</v>
       </c>
       <c r="AG6" s="15">
-        <v>12607</v>
+        <v>12553</v>
       </c>
       <c r="AH6" s="15">
         <v>13011</v>
@@ -4744,7 +4744,7 @@
         <v>11478</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>20340</v>
       </c>
       <c r="AG7" s="15">
-        <v>18319</v>
+        <v>18689</v>
       </c>
       <c r="AH7" s="15">
         <v>14949</v>
@@ -4905,7 +4905,7 @@
         <v>16410</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>2807</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>9071</v>
       </c>
       <c r="AG9" s="15">
-        <v>8846</v>
+        <v>8866</v>
       </c>
       <c r="AH9" s="15">
         <v>8842</v>
@@ -5227,7 +5227,7 @@
         <v>8047</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>12067</v>
       </c>
       <c r="AG10" s="15">
-        <v>12463</v>
+        <v>12453</v>
       </c>
       <c r="AH10" s="15">
         <v>12130</v>
@@ -5388,7 +5388,7 @@
         <v>12133</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>34897</v>
       </c>
       <c r="AG11" s="15">
-        <v>39166</v>
+        <v>39057</v>
       </c>
       <c r="AH11" s="15">
         <v>39058</v>
@@ -5549,7 +5549,7 @@
         <v>29432</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -5647,7 +5647,7 @@
         <v>98346</v>
       </c>
       <c r="AG12" s="7">
-        <v>101192</v>
+        <v>101361</v>
       </c>
       <c r="AH12" s="7">
         <v>97993</v>
@@ -5710,7 +5710,7 @@
         <v>84670</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5765,12 +5765,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>411.439482</v>
       </c>
       <c r="AG15" s="15">
-        <v>427.68074100000001</v>
+        <v>424.02806199999998</v>
       </c>
       <c r="AH15" s="15">
         <v>450.18517000000003</v>
@@ -5931,7 +5931,7 @@
         <v>303.44771800000001</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -6029,7 +6029,7 @@
         <v>921.33457799999996</v>
       </c>
       <c r="AG16" s="15">
-        <v>905.70455900000002</v>
+        <v>903.15429700000004</v>
       </c>
       <c r="AH16" s="15">
         <v>953.28650700000003</v>
@@ -6092,7 +6092,7 @@
         <v>868.11864300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -6190,7 +6190,7 @@
         <v>659.46664699999997</v>
       </c>
       <c r="AG17" s="15">
-        <v>642.541875</v>
+        <v>641.52587300000005</v>
       </c>
       <c r="AH17" s="15">
         <v>648.69403</v>
@@ -6253,7 +6253,7 @@
         <v>433.165955</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -6351,7 +6351,7 @@
         <v>61.255878000000003</v>
       </c>
       <c r="AG18" s="15">
-        <v>57.728878000000002</v>
+        <v>57.705795999999999</v>
       </c>
       <c r="AH18" s="15">
         <v>72.158365000000003</v>
@@ -6414,7 +6414,7 @@
         <v>42.773207999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -6512,7 +6512,7 @@
         <v>373.11177199999997</v>
       </c>
       <c r="AG19" s="15">
-        <v>399.94396399999999</v>
+        <v>400.56517200000002</v>
       </c>
       <c r="AH19" s="15">
         <v>361.26725900000002</v>
@@ -6575,7 +6575,7 @@
         <v>374.79168900000002</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -6673,7 +6673,7 @@
         <v>1132.3510699999999</v>
       </c>
       <c r="AG20" s="15">
-        <v>1076.2912349999999</v>
+        <v>1075.235312</v>
       </c>
       <c r="AH20" s="15">
         <v>1147.503254</v>
@@ -6736,7 +6736,7 @@
         <v>1143.806075</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -6834,7 +6834,7 @@
         <v>851.04168600000003</v>
       </c>
       <c r="AG21" s="15">
-        <v>890.03262199999995</v>
+        <v>889.05551200000002</v>
       </c>
       <c r="AH21" s="15">
         <v>931.29774999999995</v>
@@ -6897,7 +6897,7 @@
         <v>657.70498399999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -6995,7 +6995,7 @@
         <v>4410.0011130000003</v>
       </c>
       <c r="AG22" s="7">
-        <v>4399.9238739999992</v>
+        <v>4391.2700239999995</v>
       </c>
       <c r="AH22" s="7">
         <v>4564.3923350000005</v>
@@ -7058,40 +7058,40 @@
         <v>3823.8082720000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -7104,9 +7104,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -7116,23 +7113,23 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="D25" sqref="D25"/>
-      <selection pane="topRight" activeCell="D25" sqref="D25"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
-      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="53" width="9.44140625" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.44140625" customWidth="1"/>
-    <col min="55" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="53" width="9.42578125" style="1" customWidth="1"/>
+    <col min="54" max="54" width="9.42578125" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>25</v>
       </c>
@@ -7189,7 +7186,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -7350,7 +7347,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -7512,13 +7509,13 @@
       </c>
       <c r="BB3" s="24"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -7616,7 +7613,7 @@
         <v>5362</v>
       </c>
       <c r="AG5" s="15">
-        <v>0</v>
+        <v>4988</v>
       </c>
       <c r="AH5" s="15">
         <v>0</v>
@@ -7680,7 +7677,7 @@
       </c>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -7778,7 +7775,7 @@
         <v>12439</v>
       </c>
       <c r="AG6" s="6">
-        <v>0</v>
+        <v>11704</v>
       </c>
       <c r="AH6" s="6">
         <v>0</v>
@@ -7842,7 +7839,7 @@
       </c>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -7940,7 +7937,7 @@
         <v>17707</v>
       </c>
       <c r="AG7" s="6">
-        <v>0</v>
+        <v>16882</v>
       </c>
       <c r="AH7" s="6">
         <v>0</v>
@@ -8004,7 +8001,7 @@
       </c>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -8102,7 +8099,7 @@
         <v>3694</v>
       </c>
       <c r="AG8" s="6">
-        <v>0</v>
+        <v>3877</v>
       </c>
       <c r="AH8" s="6">
         <v>0</v>
@@ -8166,7 +8163,7 @@
       </c>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -8264,7 +8261,7 @@
         <v>9851</v>
       </c>
       <c r="AG9" s="6">
-        <v>0</v>
+        <v>8689</v>
       </c>
       <c r="AH9" s="6">
         <v>0</v>
@@ -8328,7 +8325,7 @@
       </c>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -8426,7 +8423,7 @@
         <v>11366</v>
       </c>
       <c r="AG10" s="15">
-        <v>0</v>
+        <v>11439</v>
       </c>
       <c r="AH10" s="15">
         <v>0</v>
@@ -8490,7 +8487,7 @@
       </c>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -8588,7 +8585,7 @@
         <v>43793</v>
       </c>
       <c r="AG11" s="6">
-        <v>0</v>
+        <v>44996</v>
       </c>
       <c r="AH11" s="6">
         <v>0</v>
@@ -8652,7 +8649,7 @@
       </c>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -8750,7 +8747,7 @@
         <v>104212</v>
       </c>
       <c r="AG12" s="7">
-        <v>0</v>
+        <v>102575</v>
       </c>
       <c r="AH12" s="7">
         <v>0</v>
@@ -8814,7 +8811,7 @@
       </c>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -8870,13 +8867,13 @@
       <c r="BA13" s="6"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -8974,7 +8971,7 @@
         <v>399.22666700000002</v>
       </c>
       <c r="AG15" s="15">
-        <v>0</v>
+        <v>371.14814200000001</v>
       </c>
       <c r="AH15" s="15">
         <v>0</v>
@@ -9038,7 +9035,7 @@
       </c>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -9136,7 +9133,7 @@
         <v>909.42033000000004</v>
       </c>
       <c r="AG16" s="6">
-        <v>0</v>
+        <v>853.30135399999995</v>
       </c>
       <c r="AH16" s="6">
         <v>0</v>
@@ -9200,7 +9197,7 @@
       </c>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -9298,7 +9295,7 @@
         <v>588.55939599999999</v>
       </c>
       <c r="AG17" s="6">
-        <v>0</v>
+        <v>572.016481</v>
       </c>
       <c r="AH17" s="6">
         <v>0</v>
@@ -9362,7 +9359,7 @@
       </c>
       <c r="BB17"/>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -9460,7 +9457,7 @@
         <v>56.876569000000003</v>
       </c>
       <c r="AG18" s="6">
-        <v>0</v>
+        <v>47.867184999999999</v>
       </c>
       <c r="AH18" s="6">
         <v>0</v>
@@ -9524,7 +9521,7 @@
       </c>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -9622,7 +9619,7 @@
         <v>422.06519200000002</v>
       </c>
       <c r="AG19" s="6">
-        <v>0</v>
+        <v>361.03214800000001</v>
       </c>
       <c r="AH19" s="6">
         <v>0</v>
@@ -9686,7 +9683,7 @@
       </c>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -9784,7 +9781,7 @@
         <v>1018.263691</v>
       </c>
       <c r="AG20" s="15">
-        <v>0</v>
+        <v>1001.68426</v>
       </c>
       <c r="AH20" s="15">
         <v>0</v>
@@ -9848,7 +9845,7 @@
       </c>
       <c r="BB20"/>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -9946,7 +9943,7 @@
         <v>1010.360158</v>
       </c>
       <c r="AG21" s="6">
-        <v>0</v>
+        <v>1008.637739</v>
       </c>
       <c r="AH21" s="6">
         <v>0</v>
@@ -10010,7 +10007,7 @@
       </c>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -10108,7 +10105,7 @@
         <v>4404.772003</v>
       </c>
       <c r="AG22" s="7">
-        <v>0</v>
+        <v>4215.6873089999999</v>
       </c>
       <c r="AH22" s="7">
         <v>0</v>
@@ -10172,100 +10169,100 @@
       </c>
       <c r="BB22"/>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="BB23"/>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB24"/>
     </row>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB25"/>
     </row>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB26"/>
     </row>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB27"/>
     </row>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB28"/>
     </row>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB29"/>
     </row>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB30"/>
     </row>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB31"/>
     </row>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB32"/>
     </row>
-    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB33"/>
     </row>
-    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB34"/>
     </row>
-    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB35"/>
     </row>
-    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB36"/>
     </row>
-    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB37"/>
     </row>
-    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB38"/>
     </row>
-    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB39"/>
     </row>
-    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB40"/>
     </row>
-    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB41"/>
     </row>
-    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB42"/>
     </row>
-    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB43"/>
     </row>
-    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB44"/>
     </row>
-    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB45"/>
     </row>
-    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB46"/>
     </row>
-    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB47"/>
     </row>
-    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB48"/>
     </row>
-    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB49"/>
     </row>
-    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB50"/>
     </row>
-    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB51"/>
     </row>
-    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB52"/>
     </row>
-    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB53"/>
     </row>
-    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="54:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BB54"/>
     </row>
   </sheetData>
@@ -10280,9 +10277,6 @@
     <brk id="27" max="48" man="1"/>
     <brk id="40" max="48" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -10298,16 +10292,16 @@
       <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="8" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="17" customWidth="1"/>
     <col min="53" max="53" width="9" style="17" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="17"/>
+    <col min="54" max="16384" width="6.7109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -10364,7 +10358,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -10525,7 +10519,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -10687,12 +10681,12 @@
       </c>
       <c r="BB3" s="23"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -10853,7 +10847,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -11014,7 +11008,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -11175,7 +11169,7 @@
         <v>15693</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -11336,7 +11330,7 @@
         <v>3926</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -11497,7 +11491,7 @@
         <v>6531</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11658,7 +11652,7 @@
         <v>10908</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -11819,7 +11813,7 @@
         <v>33194</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -11980,7 +11974,7 @@
         <v>88077</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -12035,12 +12029,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -12201,7 +12195,7 @@
         <v>448.48865799999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -12362,7 +12356,7 @@
         <v>863.31579299999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -12523,7 +12517,7 @@
         <v>424.08659699999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -12684,7 +12678,7 @@
         <v>49.649962000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -12845,7 +12839,7 @@
         <v>235.51133100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -13006,7 +13000,7 @@
         <v>961.98002299999996</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -13167,7 +13161,7 @@
         <v>764.98213299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -13328,38 +13322,38 @@
         <v>3748.0144969999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -13388,16 +13382,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
@@ -13454,7 +13448,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:53" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -13615,7 +13609,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -13776,12 +13770,12 @@
         <v>43093</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -13942,7 +13936,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -14103,7 +14097,7 @@
         <v>9513</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -14264,7 +14258,7 @@
         <v>16470</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -14425,7 +14419,7 @@
         <v>2770</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -14586,7 +14580,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -14747,7 +14741,7 @@
         <v>9414</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -14908,7 +14902,7 @@
         <v>36964</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -15069,7 +15063,7 @@
         <v>85200</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -15124,12 +15118,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -15290,7 +15284,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -15451,7 +15445,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -15612,7 +15606,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -15773,7 +15767,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -15934,7 +15928,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -16095,7 +16089,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -16256,7 +16250,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -16417,38 +16411,38 @@
         <v>3298</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -16473,16 +16467,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
     <col min="53" max="53" width="9" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>15</v>
       </c>
@@ -16539,7 +16533,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -16700,7 +16694,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -16862,12 +16856,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -17028,7 +17022,7 @@
         <v>5334</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -17189,7 +17183,7 @@
         <v>12729</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -17350,7 +17344,7 @@
         <v>16661</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -17511,7 +17505,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -17672,7 +17666,7 @@
         <v>6690</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -17833,7 +17827,7 @@
         <v>12175</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -17994,7 +17988,7 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -18155,7 +18149,7 @@
         <v>97169</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -18210,12 +18204,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -18376,7 +18370,7 @@
         <v>345.26898999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -18537,7 +18531,7 @@
         <v>1137.3429249999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -18698,7 +18692,7 @@
         <v>337.41420499999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -18859,7 +18853,7 @@
         <v>40.33334</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -19020,7 +19014,7 @@
         <v>339.10771799999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -19181,7 +19175,7 @@
         <v>1247.683331</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -19342,7 +19336,7 @@
         <v>821.21724600000005</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -19503,38 +19497,38 @@
         <v>4268.3677550000002</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -19551,16 +19545,16 @@
       <selection activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
@@ -19617,7 +19611,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -19778,7 +19772,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -19940,12 +19934,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -20106,7 +20100,7 @@
         <v>5356</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -20267,7 +20261,7 @@
         <v>12576</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -20428,7 +20422,7 @@
         <v>17944</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -20589,7 +20583,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -20750,7 +20744,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -20911,7 +20905,7 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -21072,7 +21066,7 @@
         <v>38154</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -21233,7 +21227,7 @@
         <v>92789</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -21288,12 +21282,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -21454,7 +21448,7 @@
         <v>356.60756500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -21615,7 +21609,7 @@
         <v>977.829027</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -21776,7 +21770,7 @@
         <v>495.993199</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -21937,7 +21931,7 @@
         <v>37.412531000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -22098,7 +22092,7 @@
         <v>351.68923999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -22259,7 +22253,7 @@
         <v>888.50449000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -22420,7 +22414,7 @@
         <v>804.61703199999999</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -22581,38 +22575,38 @@
         <v>3912.6530840000005</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -22629,17 +22623,17 @@
       <selection activeCell="A5" sqref="A5:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
@@ -22696,7 +22690,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="23.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>18</v>
       </c>
@@ -22860,7 +22854,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>19</v>
       </c>
@@ -23022,7 +23016,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -23186,12 +23180,12 @@
         <v>44192</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -23355,7 +23349,7 @@
         <v>6187</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -23519,7 +23513,7 @@
         <v>11221</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>0</v>
       </c>
@@ -23683,7 +23677,7 @@
         <v>16946</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -23847,7 +23841,7 @@
         <v>2757</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
@@ -24011,7 +24005,7 @@
         <v>5377</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
@@ -24175,7 +24169,7 @@
         <v>13026</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -24339,7 +24333,7 @@
         <v>44207</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -24503,7 +24497,7 @@
         <v>99721</v>
       </c>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -24559,12 +24553,12 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -24728,7 +24722,7 @@
         <v>469.697947</v>
       </c>
     </row>
-    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -24892,7 +24886,7 @@
         <v>800.96283800000003</v>
       </c>
     </row>
-    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
@@ -25056,7 +25050,7 @@
         <v>463.52606100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
@@ -25220,7 +25214,7 @@
         <v>39.121160000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -25384,7 +25378,7 @@
         <v>320.92344600000001</v>
       </c>
     </row>
-    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -25548,7 +25542,7 @@
         <v>1254.2732289999999</v>
       </c>
     </row>
-    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -25712,7 +25706,7 @@
         <v>905.27916400000004</v>
       </c>
     </row>
-    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -25876,38 +25870,38 @@
         <v>4253.7838449999999</v>
       </c>
     </row>
-    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -25928,16 +25922,16 @@
       <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
@@ -25994,7 +25988,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -26155,7 +26149,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -26317,12 +26311,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -26483,7 +26477,7 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -26644,7 +26638,7 @@
         <v>10430</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -26805,7 +26799,7 @@
         <v>15971</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -26966,7 +26960,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -27127,7 +27121,7 @@
         <v>5679</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -27288,7 +27282,7 @@
         <v>8618</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -27449,7 +27443,7 @@
         <v>34889</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -27610,7 +27604,7 @@
         <v>83267</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -27665,12 +27659,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -27831,7 +27825,7 @@
         <v>326.63437199999998</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -27992,7 +27986,7 @@
         <v>710.31911300000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -28153,7 +28147,7 @@
         <v>390.89581099999998</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -28314,7 +28308,7 @@
         <v>36.150655</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -28475,7 +28469,7 @@
         <v>232.43127799999999</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -28636,7 +28630,7 @@
         <v>750.77748799999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -28797,7 +28791,7 @@
         <v>735.26635299999998</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28958,40 +28952,40 @@
         <v>3182.4750699999995</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -29019,16 +29013,16 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
@@ -29085,7 +29079,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -29246,7 +29240,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -29408,12 +29402,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -29574,7 +29568,7 @@
         <v>4405</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -29735,7 +29729,7 @@
         <v>11045</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -29896,7 +29890,7 @@
         <v>14998</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -30057,7 +30051,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -30218,7 +30212,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -30379,7 +30373,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -30540,7 +30534,7 @@
         <v>31551</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -30701,7 +30695,7 @@
         <v>81088</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -30756,12 +30750,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -30922,7 +30916,7 @@
         <v>307.73157300000003</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -31083,7 +31077,7 @@
         <v>782.92677600000002</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -31244,7 +31238,7 @@
         <v>401.64126599999997</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -31405,7 +31399,7 @@
         <v>32.955354</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -31566,7 +31560,7 @@
         <v>272.11873100000003</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -31727,7 +31721,7 @@
         <v>976.60348099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -31888,7 +31882,7 @@
         <v>752.63757299999997</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -32049,40 +32043,40 @@
         <v>3526.6147539999997</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>
@@ -32110,16 +32104,16 @@
       <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="3" customWidth="1"/>
-    <col min="3" max="52" width="9.44140625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="6.6640625" style="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="52" width="9.42578125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="6.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:54" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
@@ -32176,7 +32170,7 @@
       <c r="AZ1" s="26"/>
       <c r="BA1" s="26"/>
     </row>
-    <row r="2" spans="1:54" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -32337,7 +32331,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="2" customFormat="1" ht="23.4" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -32499,12 +32493,12 @@
       </c>
       <c r="BB3" s="25"/>
     </row>
-    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
@@ -32665,7 +32659,7 @@
         <v>4413</v>
       </c>
     </row>
-    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -32826,7 +32820,7 @@
         <v>11673</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -32987,7 +32981,7 @@
         <v>15590</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -33148,7 +33142,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -33309,7 +33303,7 @@
         <v>8134</v>
       </c>
     </row>
-    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -33470,7 +33464,7 @@
         <v>9863</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -33631,7 +33625,7 @@
         <v>34066</v>
       </c>
     </row>
-    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -33792,7 +33786,7 @@
         <v>86245</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -33847,12 +33841,12 @@
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
     </row>
-    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -34013,7 +34007,7 @@
         <v>298.50642199999999</v>
       </c>
     </row>
-    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -34174,7 +34168,7 @@
         <v>888.297684</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>0</v>
       </c>
@@ -34335,7 +34329,7 @@
         <v>533.92582100000004</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -34496,7 +34490,7 @@
         <v>38.857964000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1</v>
       </c>
@@ -34657,7 +34651,7 @@
         <v>364.61675700000001</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
@@ -34818,7 +34812,7 @@
         <v>992.76339499999995</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -34979,7 +34973,7 @@
         <v>755.640308</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:53" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>6</v>
       </c>
@@ -35140,40 +35134,40 @@
         <v>3872.6083509999999</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:53" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:53" s="9" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:53" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:BA1"/>

</xml_diff>

<commit_message>
GH ACTION Autorun Wed Aug 20 05:30:18 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E456DD85-809D-45A3-82AF-51EFAC8EC324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F678B630-A451-4B33-BB11-2C6D0AB3FDC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -4022,10 +4022,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="E34" sqref="E34"/>
-      <selection pane="topRight" activeCell="E34" sqref="E34"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <selection activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
+      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4523,7 +4523,7 @@
         <v>5718</v>
       </c>
       <c r="AH5" s="15">
-        <v>5922</v>
+        <v>5888</v>
       </c>
       <c r="AI5" s="15">
         <v>4724</v>
@@ -4684,7 +4684,7 @@
         <v>12553</v>
       </c>
       <c r="AH6" s="15">
-        <v>13011</v>
+        <v>12984</v>
       </c>
       <c r="AI6" s="15">
         <v>10292</v>
@@ -4845,7 +4845,7 @@
         <v>18689</v>
       </c>
       <c r="AH7" s="15">
-        <v>14949</v>
+        <v>15562</v>
       </c>
       <c r="AI7" s="15">
         <v>15168</v>
@@ -5006,7 +5006,7 @@
         <v>4025</v>
       </c>
       <c r="AH8" s="15">
-        <v>4081</v>
+        <v>4080</v>
       </c>
       <c r="AI8" s="15">
         <v>3396</v>
@@ -5167,7 +5167,7 @@
         <v>8866</v>
       </c>
       <c r="AH9" s="15">
-        <v>8842</v>
+        <v>8740</v>
       </c>
       <c r="AI9" s="15">
         <v>7250</v>
@@ -5328,7 +5328,7 @@
         <v>12453</v>
       </c>
       <c r="AH10" s="15">
-        <v>12130</v>
+        <v>11976</v>
       </c>
       <c r="AI10" s="15">
         <v>8727</v>
@@ -5489,7 +5489,7 @@
         <v>39057</v>
       </c>
       <c r="AH11" s="15">
-        <v>39058</v>
+        <v>38944</v>
       </c>
       <c r="AI11" s="15">
         <v>28728</v>
@@ -5650,7 +5650,7 @@
         <v>101361</v>
       </c>
       <c r="AH12" s="7">
-        <v>97993</v>
+        <v>98174</v>
       </c>
       <c r="AI12" s="7">
         <v>78285</v>
@@ -5871,7 +5871,7 @@
         <v>424.02806199999998</v>
       </c>
       <c r="AH15" s="15">
-        <v>450.18517000000003</v>
+        <v>448.371287</v>
       </c>
       <c r="AI15" s="15">
         <v>336.97846700000002</v>
@@ -6032,7 +6032,7 @@
         <v>903.15429700000004</v>
       </c>
       <c r="AH16" s="15">
-        <v>953.28650700000003</v>
+        <v>952.98530400000004</v>
       </c>
       <c r="AI16" s="15">
         <v>706.90092900000002</v>
@@ -6193,7 +6193,7 @@
         <v>641.52587300000005</v>
       </c>
       <c r="AH17" s="15">
-        <v>648.69403</v>
+        <v>646.69913299999996</v>
       </c>
       <c r="AI17" s="15">
         <v>344.75138600000002</v>
@@ -6354,7 +6354,7 @@
         <v>57.705795999999999</v>
       </c>
       <c r="AH18" s="15">
-        <v>72.158365000000003</v>
+        <v>72.154160000000005</v>
       </c>
       <c r="AI18" s="15">
         <v>44.145868999999998</v>
@@ -6515,7 +6515,7 @@
         <v>400.56517200000002</v>
       </c>
       <c r="AH19" s="15">
-        <v>361.26725900000002</v>
+        <v>361.51413500000001</v>
       </c>
       <c r="AI19" s="15">
         <v>307.15985599999999</v>
@@ -6676,7 +6676,7 @@
         <v>1075.235312</v>
       </c>
       <c r="AH20" s="15">
-        <v>1147.503254</v>
+        <v>1133.5927830000001</v>
       </c>
       <c r="AI20" s="15">
         <v>740.64947099999995</v>
@@ -6837,7 +6837,7 @@
         <v>889.05551200000002</v>
       </c>
       <c r="AH21" s="15">
-        <v>931.29774999999995</v>
+        <v>930.01921100000004</v>
       </c>
       <c r="AI21" s="15">
         <v>602.18869299999994</v>
@@ -6998,7 +6998,7 @@
         <v>4391.2700239999995</v>
       </c>
       <c r="AH22" s="7">
-        <v>4564.3923350000005</v>
+        <v>4545.3360130000001</v>
       </c>
       <c r="AI22" s="7">
         <v>3082.7746710000001</v>
@@ -7114,10 +7114,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <selection activeCell="D35" sqref="D35"/>
+      <selection pane="topRight" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7616,7 +7616,7 @@
         <v>4988</v>
       </c>
       <c r="AH5" s="15">
-        <v>0</v>
+        <v>5194</v>
       </c>
       <c r="AI5" s="15">
         <v>0</v>
@@ -7778,7 +7778,7 @@
         <v>11704</v>
       </c>
       <c r="AH6" s="6">
-        <v>0</v>
+        <v>11951</v>
       </c>
       <c r="AI6" s="6">
         <v>0</v>
@@ -7940,7 +7940,7 @@
         <v>16882</v>
       </c>
       <c r="AH7" s="6">
-        <v>0</v>
+        <v>13554</v>
       </c>
       <c r="AI7" s="6">
         <v>0</v>
@@ -8102,7 +8102,7 @@
         <v>3877</v>
       </c>
       <c r="AH8" s="6">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="AI8" s="6">
         <v>0</v>
@@ -8264,7 +8264,7 @@
         <v>8689</v>
       </c>
       <c r="AH9" s="6">
-        <v>0</v>
+        <v>9293</v>
       </c>
       <c r="AI9" s="6">
         <v>0</v>
@@ -8426,7 +8426,7 @@
         <v>11439</v>
       </c>
       <c r="AH10" s="15">
-        <v>0</v>
+        <v>11290</v>
       </c>
       <c r="AI10" s="15">
         <v>0</v>
@@ -8588,7 +8588,7 @@
         <v>44996</v>
       </c>
       <c r="AH11" s="6">
-        <v>0</v>
+        <v>44199</v>
       </c>
       <c r="AI11" s="6">
         <v>0</v>
@@ -8750,7 +8750,7 @@
         <v>102575</v>
       </c>
       <c r="AH12" s="7">
-        <v>0</v>
+        <v>99481</v>
       </c>
       <c r="AI12" s="7">
         <v>0</v>
@@ -8974,7 +8974,7 @@
         <v>371.14814200000001</v>
       </c>
       <c r="AH15" s="15">
-        <v>0</v>
+        <v>394.76492999999999</v>
       </c>
       <c r="AI15" s="15">
         <v>0</v>
@@ -9136,7 +9136,7 @@
         <v>853.30135399999995</v>
       </c>
       <c r="AH16" s="6">
-        <v>0</v>
+        <v>821.78398500000003</v>
       </c>
       <c r="AI16" s="6">
         <v>0</v>
@@ -9298,7 +9298,7 @@
         <v>572.016481</v>
       </c>
       <c r="AH17" s="6">
-        <v>0</v>
+        <v>537.42531199999996</v>
       </c>
       <c r="AI17" s="6">
         <v>0</v>
@@ -9460,7 +9460,7 @@
         <v>47.867184999999999</v>
       </c>
       <c r="AH18" s="6">
-        <v>0</v>
+        <v>59.411977999999998</v>
       </c>
       <c r="AI18" s="6">
         <v>0</v>
@@ -9622,7 +9622,7 @@
         <v>361.03214800000001</v>
       </c>
       <c r="AH19" s="6">
-        <v>0</v>
+        <v>403.74636199999998</v>
       </c>
       <c r="AI19" s="6">
         <v>0</v>
@@ -9784,7 +9784,7 @@
         <v>1001.68426</v>
       </c>
       <c r="AH20" s="15">
-        <v>0</v>
+        <v>1012.4116320000001</v>
       </c>
       <c r="AI20" s="15">
         <v>0</v>
@@ -9946,7 +9946,7 @@
         <v>1008.637739</v>
       </c>
       <c r="AH21" s="6">
-        <v>0</v>
+        <v>981.40062699999999</v>
       </c>
       <c r="AI21" s="6">
         <v>0</v>
@@ -10108,7 +10108,7 @@
         <v>4215.6873089999999</v>
       </c>
       <c r="AH22" s="7">
-        <v>0</v>
+        <v>4210.9448259999999</v>
       </c>
       <c r="AI22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Aug 26 05:31:05 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F678B630-A451-4B33-BB11-2C6D0AB3FDC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D94FBE-ECBE-483C-86CA-218B37DA50D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -4022,10 +4022,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:BB3"/>
-      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
+      <selection sqref="A1:XFD1048576"/>
+      <selection pane="topRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4526,7 +4526,7 @@
         <v>5888</v>
       </c>
       <c r="AI5" s="15">
-        <v>4724</v>
+        <v>4693</v>
       </c>
       <c r="AJ5" s="15">
         <v>5247</v>
@@ -4687,7 +4687,7 @@
         <v>12984</v>
       </c>
       <c r="AI6" s="15">
-        <v>10292</v>
+        <v>10242</v>
       </c>
       <c r="AJ6" s="15">
         <v>11935</v>
@@ -4848,7 +4848,7 @@
         <v>15562</v>
       </c>
       <c r="AI7" s="15">
-        <v>15168</v>
+        <v>14613</v>
       </c>
       <c r="AJ7" s="15">
         <v>19412</v>
@@ -5009,7 +5009,7 @@
         <v>4080</v>
       </c>
       <c r="AI8" s="15">
-        <v>3396</v>
+        <v>3395</v>
       </c>
       <c r="AJ8" s="15">
         <v>4144</v>
@@ -5170,7 +5170,7 @@
         <v>8740</v>
       </c>
       <c r="AI9" s="15">
-        <v>7250</v>
+        <v>7252</v>
       </c>
       <c r="AJ9" s="15">
         <v>8621</v>
@@ -5331,7 +5331,7 @@
         <v>11976</v>
       </c>
       <c r="AI10" s="15">
-        <v>8727</v>
+        <v>8720</v>
       </c>
       <c r="AJ10" s="15">
         <v>11555</v>
@@ -5492,7 +5492,7 @@
         <v>38944</v>
       </c>
       <c r="AI11" s="15">
-        <v>28728</v>
+        <v>28655</v>
       </c>
       <c r="AJ11" s="15">
         <v>35373</v>
@@ -5653,7 +5653,7 @@
         <v>98174</v>
       </c>
       <c r="AI12" s="7">
-        <v>78285</v>
+        <v>77570</v>
       </c>
       <c r="AJ12" s="7">
         <v>96287</v>
@@ -5874,7 +5874,7 @@
         <v>448.371287</v>
       </c>
       <c r="AI15" s="15">
-        <v>336.97846700000002</v>
+        <v>335.07634000000002</v>
       </c>
       <c r="AJ15" s="15">
         <v>391.73318799999998</v>
@@ -6035,7 +6035,7 @@
         <v>952.98530400000004</v>
       </c>
       <c r="AI16" s="15">
-        <v>706.90092900000002</v>
+        <v>706.45891800000004</v>
       </c>
       <c r="AJ16" s="15">
         <v>880.103342</v>
@@ -6196,7 +6196,7 @@
         <v>646.69913299999996</v>
       </c>
       <c r="AI17" s="15">
-        <v>344.75138600000002</v>
+        <v>322.986062</v>
       </c>
       <c r="AJ17" s="15">
         <v>552.36141399999997</v>
@@ -6357,7 +6357,7 @@
         <v>72.154160000000005</v>
       </c>
       <c r="AI18" s="15">
-        <v>44.145868999999998</v>
+        <v>44.140965999999999</v>
       </c>
       <c r="AJ18" s="15">
         <v>60.779040999999999</v>
@@ -6518,7 +6518,7 @@
         <v>361.51413500000001</v>
       </c>
       <c r="AI19" s="15">
-        <v>307.15985599999999</v>
+        <v>307.258758</v>
       </c>
       <c r="AJ19" s="15">
         <v>358.97626300000002</v>
@@ -6679,7 +6679,7 @@
         <v>1133.5927830000001</v>
       </c>
       <c r="AI20" s="15">
-        <v>740.64947099999995</v>
+        <v>740.062726</v>
       </c>
       <c r="AJ20" s="15">
         <v>1076.9260509999999</v>
@@ -6840,7 +6840,7 @@
         <v>930.01921100000004</v>
       </c>
       <c r="AI21" s="15">
-        <v>602.18869299999994</v>
+        <v>601.44562599999995</v>
       </c>
       <c r="AJ21" s="15">
         <v>883.33743300000003</v>
@@ -7001,7 +7001,7 @@
         <v>4545.3360130000001</v>
       </c>
       <c r="AI22" s="7">
-        <v>3082.7746710000001</v>
+        <v>3057.4293959999995</v>
       </c>
       <c r="AJ22" s="7">
         <v>4204.2167319999999</v>
@@ -7114,10 +7114,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="D35" sqref="D35"/>
-      <selection pane="topRight" activeCell="D35" sqref="D35"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
-      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
+      <selection activeCell="D34" sqref="D34"/>
+      <selection pane="topRight" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7619,7 +7619,7 @@
         <v>5194</v>
       </c>
       <c r="AI5" s="15">
-        <v>0</v>
+        <v>5201</v>
       </c>
       <c r="AJ5" s="15">
         <v>0</v>
@@ -7781,7 +7781,7 @@
         <v>11951</v>
       </c>
       <c r="AI6" s="6">
-        <v>0</v>
+        <v>12561</v>
       </c>
       <c r="AJ6" s="6">
         <v>0</v>
@@ -7943,7 +7943,7 @@
         <v>13554</v>
       </c>
       <c r="AI7" s="6">
-        <v>0</v>
+        <v>14258</v>
       </c>
       <c r="AJ7" s="6">
         <v>0</v>
@@ -8105,7 +8105,7 @@
         <v>4000</v>
       </c>
       <c r="AI8" s="6">
-        <v>0</v>
+        <v>3758</v>
       </c>
       <c r="AJ8" s="6">
         <v>0</v>
@@ -8267,7 +8267,7 @@
         <v>9293</v>
       </c>
       <c r="AI9" s="6">
-        <v>0</v>
+        <v>9861</v>
       </c>
       <c r="AJ9" s="6">
         <v>0</v>
@@ -8429,7 +8429,7 @@
         <v>11290</v>
       </c>
       <c r="AI10" s="15">
-        <v>0</v>
+        <v>9849</v>
       </c>
       <c r="AJ10" s="15">
         <v>0</v>
@@ -8591,7 +8591,7 @@
         <v>44199</v>
       </c>
       <c r="AI11" s="6">
-        <v>0</v>
+        <v>46410</v>
       </c>
       <c r="AJ11" s="6">
         <v>0</v>
@@ -8753,7 +8753,7 @@
         <v>99481</v>
       </c>
       <c r="AI12" s="7">
-        <v>0</v>
+        <v>101898</v>
       </c>
       <c r="AJ12" s="7">
         <v>0</v>
@@ -8977,7 +8977,7 @@
         <v>394.76492999999999</v>
       </c>
       <c r="AI15" s="15">
-        <v>0</v>
+        <v>381.64281199999999</v>
       </c>
       <c r="AJ15" s="15">
         <v>0</v>
@@ -9139,7 +9139,7 @@
         <v>821.78398500000003</v>
       </c>
       <c r="AI16" s="6">
-        <v>0</v>
+        <v>928.44029999999998</v>
       </c>
       <c r="AJ16" s="6">
         <v>0</v>
@@ -9301,7 +9301,7 @@
         <v>537.42531199999996</v>
       </c>
       <c r="AI17" s="6">
-        <v>0</v>
+        <v>514.473296</v>
       </c>
       <c r="AJ17" s="6">
         <v>0</v>
@@ -9463,7 +9463,7 @@
         <v>59.411977999999998</v>
       </c>
       <c r="AI18" s="6">
-        <v>0</v>
+        <v>54.584521000000002</v>
       </c>
       <c r="AJ18" s="6">
         <v>0</v>
@@ -9625,7 +9625,7 @@
         <v>403.74636199999998</v>
       </c>
       <c r="AI19" s="6">
-        <v>0</v>
+        <v>423.05175600000001</v>
       </c>
       <c r="AJ19" s="6">
         <v>0</v>
@@ -9787,7 +9787,7 @@
         <v>1012.4116320000001</v>
       </c>
       <c r="AI20" s="15">
-        <v>0</v>
+        <v>830.03298500000005</v>
       </c>
       <c r="AJ20" s="15">
         <v>0</v>
@@ -9949,7 +9949,7 @@
         <v>981.40062699999999</v>
       </c>
       <c r="AI21" s="6">
-        <v>0</v>
+        <v>1013.313163</v>
       </c>
       <c r="AJ21" s="6">
         <v>0</v>
@@ -10111,7 +10111,7 @@
         <v>4210.9448259999999</v>
       </c>
       <c r="AI22" s="7">
-        <v>0</v>
+        <v>4145.5388329999996</v>
       </c>
       <c r="AJ22" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Wed Sep  3 05:27:39 UTC 2025
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles_V2.xlsx
+++ b/Data/Revenue_ton_miles_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D94FBE-ECBE-483C-86CA-218B37DA50D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FC7EA9-432E-4362-91AD-030D7E460FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="591" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4025,7 +4025,7 @@
       <selection sqref="A1:XFD1048576"/>
       <selection pane="topRight" sqref="A1:XFD1048576"/>
       <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
-      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4529,7 +4529,7 @@
         <v>4693</v>
       </c>
       <c r="AJ5" s="15">
-        <v>5247</v>
+        <v>5213</v>
       </c>
       <c r="AK5" s="15">
         <v>5559</v>
@@ -4690,7 +4690,7 @@
         <v>10242</v>
       </c>
       <c r="AJ6" s="15">
-        <v>11935</v>
+        <v>11919</v>
       </c>
       <c r="AK6" s="15">
         <v>11624</v>
@@ -4851,7 +4851,7 @@
         <v>14613</v>
       </c>
       <c r="AJ7" s="15">
-        <v>19412</v>
+        <v>19511</v>
       </c>
       <c r="AK7" s="15">
         <v>19195</v>
@@ -5012,7 +5012,7 @@
         <v>3395</v>
       </c>
       <c r="AJ8" s="15">
-        <v>4144</v>
+        <v>4138</v>
       </c>
       <c r="AK8" s="15">
         <v>4107</v>
@@ -5173,7 +5173,7 @@
         <v>7252</v>
       </c>
       <c r="AJ9" s="15">
-        <v>8621</v>
+        <v>8510</v>
       </c>
       <c r="AK9" s="15">
         <v>8599</v>
@@ -5334,7 +5334,7 @@
         <v>8720</v>
       </c>
       <c r="AJ10" s="15">
-        <v>11555</v>
+        <v>11534</v>
       </c>
       <c r="AK10" s="15">
         <v>12166</v>
@@ -5495,7 +5495,7 @@
         <v>28655</v>
       </c>
       <c r="AJ11" s="15">
-        <v>35373</v>
+        <v>35325</v>
       </c>
       <c r="AK11" s="15">
         <v>38385</v>
@@ -5656,7 +5656,7 @@
         <v>77570</v>
       </c>
       <c r="AJ12" s="7">
-        <v>96287</v>
+        <v>96150</v>
       </c>
       <c r="AK12" s="7">
         <v>99635</v>
@@ -5877,7 +5877,7 @@
         <v>335.07634000000002</v>
       </c>
       <c r="AJ15" s="15">
-        <v>391.73318799999998</v>
+        <v>389.53436799999997</v>
       </c>
       <c r="AK15" s="15">
         <v>394.86603700000001</v>
@@ -6038,7 +6038,7 @@
         <v>706.45891800000004</v>
       </c>
       <c r="AJ16" s="15">
-        <v>880.103342</v>
+        <v>879.91801599999997</v>
       </c>
       <c r="AK16" s="15">
         <v>815.923317</v>
@@ -6199,7 +6199,7 @@
         <v>322.986062</v>
       </c>
       <c r="AJ17" s="15">
-        <v>552.36141399999997</v>
+        <v>551.62663499999996</v>
       </c>
       <c r="AK17" s="15">
         <v>588.57835399999999</v>
@@ -6360,7 +6360,7 @@
         <v>44.140965999999999</v>
       </c>
       <c r="AJ18" s="15">
-        <v>60.779040999999999</v>
+        <v>60.741216999999999</v>
       </c>
       <c r="AK18" s="15">
         <v>68.022459999999995</v>
@@ -6521,7 +6521,7 @@
         <v>307.258758</v>
       </c>
       <c r="AJ19" s="15">
-        <v>358.97626300000002</v>
+        <v>358.85806100000002</v>
       </c>
       <c r="AK19" s="15">
         <v>372.73333100000002</v>
@@ -6682,7 +6682,7 @@
         <v>740.062726</v>
       </c>
       <c r="AJ20" s="15">
-        <v>1076.9260509999999</v>
+        <v>1047.2509520000001</v>
       </c>
       <c r="AK20" s="15">
         <v>1165.080271</v>
@@ -6843,7 +6843,7 @@
         <v>601.44562599999995</v>
       </c>
       <c r="AJ21" s="15">
-        <v>883.33743300000003</v>
+        <v>882.71577500000001</v>
       </c>
       <c r="AK21" s="15">
         <v>939.34409700000003</v>
@@ -7004,7 +7004,7 @@
         <v>3057.4293959999995</v>
       </c>
       <c r="AJ22" s="7">
-        <v>4204.2167319999999</v>
+        <v>4170.6450239999995</v>
       </c>
       <c r="AK22" s="7">
         <v>4344.5478670000002</v>
@@ -7114,10 +7114,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="D34" sqref="D34"/>
-      <selection pane="topRight" activeCell="D34" sqref="D34"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
-      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
+      <selection sqref="A1:XFD1048576"/>
+      <selection pane="topRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7622,7 +7622,7 @@
         <v>5201</v>
       </c>
       <c r="AJ5" s="15">
-        <v>0</v>
+        <v>5108</v>
       </c>
       <c r="AK5" s="15">
         <v>0</v>
@@ -7784,7 +7784,7 @@
         <v>12561</v>
       </c>
       <c r="AJ6" s="6">
-        <v>0</v>
+        <v>13214</v>
       </c>
       <c r="AK6" s="6">
         <v>0</v>
@@ -7946,7 +7946,7 @@
         <v>14258</v>
       </c>
       <c r="AJ7" s="6">
-        <v>0</v>
+        <v>17577</v>
       </c>
       <c r="AK7" s="6">
         <v>0</v>
@@ -8108,7 +8108,7 @@
         <v>3758</v>
       </c>
       <c r="AJ8" s="6">
-        <v>0</v>
+        <v>3847</v>
       </c>
       <c r="AK8" s="6">
         <v>0</v>
@@ -8270,7 +8270,7 @@
         <v>9861</v>
       </c>
       <c r="AJ9" s="6">
-        <v>0</v>
+        <v>9015</v>
       </c>
       <c r="AK9" s="6">
         <v>0</v>
@@ -8432,7 +8432,7 @@
         <v>9849</v>
       </c>
       <c r="AJ10" s="15">
-        <v>0</v>
+        <v>11721</v>
       </c>
       <c r="AK10" s="15">
         <v>0</v>
@@ -8594,7 +8594,7 @@
         <v>46410</v>
       </c>
       <c r="AJ11" s="6">
-        <v>0</v>
+        <v>43408</v>
       </c>
       <c r="AK11" s="6">
         <v>0</v>
@@ -8756,7 +8756,7 @@
         <v>101898</v>
       </c>
       <c r="AJ12" s="7">
-        <v>0</v>
+        <v>103890</v>
       </c>
       <c r="AK12" s="7">
         <v>0</v>
@@ -8980,7 +8980,7 @@
         <v>381.64281199999999</v>
       </c>
       <c r="AJ15" s="15">
-        <v>0</v>
+        <v>395.688738</v>
       </c>
       <c r="AK15" s="15">
         <v>0</v>
@@ -9142,7 +9142,7 @@
         <v>928.44029999999998</v>
       </c>
       <c r="AJ16" s="6">
-        <v>0</v>
+        <v>988.31156099999998</v>
       </c>
       <c r="AK16" s="6">
         <v>0</v>
@@ -9304,7 +9304,7 @@
         <v>514.473296</v>
       </c>
       <c r="AJ17" s="6">
-        <v>0</v>
+        <v>549.06363999999996</v>
       </c>
       <c r="AK17" s="6">
         <v>0</v>
@@ -9466,7 +9466,7 @@
         <v>54.584521000000002</v>
       </c>
       <c r="AJ18" s="6">
-        <v>0</v>
+        <v>59.251081999999997</v>
       </c>
       <c r="AK18" s="6">
         <v>0</v>
@@ -9628,7 +9628,7 @@
         <v>423.05175600000001</v>
       </c>
       <c r="AJ19" s="6">
-        <v>0</v>
+        <v>413.37038799999999</v>
       </c>
       <c r="AK19" s="6">
         <v>0</v>
@@ -9790,7 +9790,7 @@
         <v>830.03298500000005</v>
       </c>
       <c r="AJ20" s="15">
-        <v>0</v>
+        <v>970.44166299999995</v>
       </c>
       <c r="AK20" s="15">
         <v>0</v>
@@ -9952,7 +9952,7 @@
         <v>1013.313163</v>
       </c>
       <c r="AJ21" s="6">
-        <v>0</v>
+        <v>1007.88144</v>
       </c>
       <c r="AK21" s="6">
         <v>0</v>
@@ -10114,7 +10114,7 @@
         <v>4145.5388329999996</v>
       </c>
       <c r="AJ22" s="7">
-        <v>0</v>
+        <v>4384.0085120000003</v>
       </c>
       <c r="AK22" s="7">
         <v>0</v>

</xml_diff>